<commit_message>
added phenology dataset for Arkensas
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8CE722-75C7-4A0D-A7E4-8DDF44BF4D4A}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CDDBE5-3B30-45A8-A569-D5908102FDFD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
   <si>
     <t>SimulationName</t>
   </si>
@@ -261,6 +261,87 @@
   </si>
   <si>
     <t>Soybean.Leaf.AppearedCohortNo</t>
+  </si>
+  <si>
+    <t>Soybean.Phenology.EmergenceDAS</t>
+  </si>
+  <si>
+    <t>Soybean.Phenology.FloweringDAS</t>
+  </si>
+  <si>
+    <t>Soybean.Phenology.MaturityDAS</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvTrial_MG00</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvLambert_MG0</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvIA1006_MG01</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvIA2008_MG02</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvMacon_MG03</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvPioneer94B01_MG04</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvHutcheson_MG05</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvNK622_MG06</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvTrial_MG00</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvLambert_MG0</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvIA1006_MG01</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvIA2008_MG02</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvMacon_MG03</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvPioneer94B01_MG04</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvHutcheson_MG05</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvNK622_MG06</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvTrial_MG00</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvLambert_MG0</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvIA1006_MG01</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvIA2008_MG02</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvMacon_MG03</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvPioneer94B01_MG04</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvHutcheson_MG05</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvNK622_MG06</t>
   </si>
 </sst>
 </file>
@@ -296,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -306,6 +387,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1329,29 +1413,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
-  <dimension ref="A1:BQ22"/>
+  <dimension ref="A1:BT46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23:C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="16.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.89453125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.05078125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.05078125" customWidth="1"/>
-    <col min="8" max="8" width="14.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.1015625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.83984375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.83984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.05078125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.83984375" customWidth="1"/>
+    <col min="3" max="6" width="12.05078125" customWidth="1"/>
+    <col min="11" max="11" width="14.15625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.734375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.1015625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.83984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.68359375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.05078125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1362,205 +1446,214 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="H1" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="I1" t="s">
         <v>78</v>
       </c>
-      <c r="G1" t="s">
+      <c r="J1" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" t="s">
         <v>72</v>
       </c>
-      <c r="I1" t="s">
+      <c r="L1" t="s">
         <v>18</v>
       </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="N1" t="s">
         <v>73</v>
       </c>
-      <c r="L1" t="s">
+      <c r="O1" t="s">
         <v>74</v>
       </c>
-      <c r="M1" t="s">
+      <c r="P1" t="s">
         <v>75</v>
       </c>
-      <c r="N1" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="O1" t="s">
+      <c r="R1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="S1" t="s">
         <v>76</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="T1" t="s">
         <v>7</v>
       </c>
-      <c r="R1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="S1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="T1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="U1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AK1" t="s">
         <v>36</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AL1" t="s">
         <v>37</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AN1" t="s">
         <v>39</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AR1" t="s">
         <v>43</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AS1" t="s">
         <v>44</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AT1" t="s">
         <v>45</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AU1" t="s">
         <v>46</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AV1" t="s">
         <v>47</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AW1" t="s">
         <v>48</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AX1" t="s">
         <v>49</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AY1" t="s">
         <v>50</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AZ1" t="s">
         <v>51</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BA1" t="s">
         <v>52</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BC1" t="s">
         <v>54</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BD1" t="s">
         <v>55</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BE1" t="s">
         <v>56</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BF1" t="s">
         <v>57</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BG1" t="s">
         <v>58</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BH1" t="s">
         <v>59</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BI1" t="s">
         <v>60</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BJ1" t="s">
         <v>61</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BK1" t="s">
         <v>62</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BL1" t="s">
         <v>63</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BM1" t="s">
         <v>64</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BN1" t="s">
         <v>65</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BO1" t="s">
         <v>66</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BP1" t="s">
         <v>67</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BQ1" t="s">
         <v>68</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BR1" t="s">
         <v>69</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BS1" t="s">
         <v>70</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BT1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1568,119 +1661,122 @@
         <v>42895</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2">
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2">
         <v>31.666666670000001</v>
       </c>
-      <c r="E2">
+      <c r="H2">
         <v>31.333333329999999</v>
       </c>
-      <c r="F2">
+      <c r="I2">
         <v>2</v>
       </c>
-      <c r="H2">
+      <c r="K2">
         <v>0.18906666699999999</v>
       </c>
-      <c r="I2">
+      <c r="L2">
         <v>26.54399239</v>
       </c>
-      <c r="J2">
+      <c r="M2">
         <v>7.4</v>
       </c>
-      <c r="L2">
+      <c r="O2">
         <v>7.4</v>
       </c>
-      <c r="M2">
+      <c r="P2">
         <v>4.9000000000000004</v>
       </c>
-      <c r="Q2">
+      <c r="T2">
         <v>12.3</v>
       </c>
-      <c r="R2">
+      <c r="U2">
         <v>4.6311446829999996</v>
       </c>
-      <c r="T2">
+      <c r="W2">
         <v>2.0514227950000001</v>
       </c>
-      <c r="X2">
+      <c r="AA2">
         <v>0.34375607200000002</v>
       </c>
-      <c r="Z2">
+      <c r="AC2">
         <v>0.101174293</v>
       </c>
-      <c r="AD2">
+      <c r="AG2">
         <v>0.44493036499999999</v>
       </c>
-      <c r="AE2">
+      <c r="AH2">
         <v>1.8991813280000001</v>
       </c>
-      <c r="AF2">
+      <c r="AI2">
         <v>26543.992389999999</v>
       </c>
-      <c r="AG2">
+      <c r="AJ2">
         <v>26543.992389999999</v>
       </c>
-      <c r="AH2">
+      <c r="AK2">
         <v>187.7777778</v>
       </c>
-      <c r="AI2">
+      <c r="AL2">
         <v>71.666666669999998</v>
       </c>
-      <c r="AK2">
+      <c r="AN2">
         <v>3.2145502540000002</v>
       </c>
-      <c r="AL2">
+      <c r="AO2">
         <v>6.5064070989999996</v>
       </c>
-      <c r="AO2">
+      <c r="AR2">
         <v>3.9638261000000001E-2</v>
       </c>
-      <c r="AP2">
+      <c r="AS2">
         <v>9.3893029850000005</v>
       </c>
-      <c r="AQ2">
+      <c r="AT2">
         <v>1.3228756559999999</v>
       </c>
-      <c r="AS2">
+      <c r="AV2">
         <v>1.3228756559999999</v>
       </c>
-      <c r="AT2">
+      <c r="AW2">
         <v>1.276714533</v>
       </c>
-      <c r="AX2">
+      <c r="BA2">
         <v>25.94224354</v>
       </c>
-      <c r="AY2">
+      <c r="BB2">
         <v>0.30950257399999997</v>
       </c>
-      <c r="BA2">
+      <c r="BD2">
         <v>9.1647271000000002E-2</v>
       </c>
-      <c r="BE2">
+      <c r="BH2">
         <v>7.4699906999999996E-2</v>
       </c>
-      <c r="BG2">
+      <c r="BJ2">
         <v>3.0704688000000001E-2</v>
       </c>
-      <c r="BK2">
+      <c r="BN2">
         <v>0.104369884</v>
       </c>
-      <c r="BL2">
+      <c r="BO2">
         <v>0.70476370899999996</v>
       </c>
-      <c r="BM2">
+      <c r="BP2">
         <v>9389.3029850000003</v>
       </c>
-      <c r="BN2">
+      <c r="BQ2">
         <v>9389.3029850000003</v>
       </c>
-      <c r="BO2">
+      <c r="BR2">
         <v>22.194427059999999</v>
       </c>
-      <c r="BP2">
+      <c r="BS2">
         <v>10.92576008</v>
       </c>
     </row>
-    <row r="3" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1688,122 +1784,125 @@
         <v>42909</v>
       </c>
       <c r="C3" s="4"/>
-      <c r="D3">
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3">
         <v>32.333333330000002</v>
       </c>
-      <c r="E3">
+      <c r="H3">
         <v>31.666666670000001</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>6.3333333329999997</v>
       </c>
-      <c r="H3">
+      <c r="K3">
         <v>1.063767667</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>26.039953109999999</v>
       </c>
-      <c r="J3">
+      <c r="M3">
         <v>29.06666667</v>
       </c>
-      <c r="L3">
+      <c r="O3">
         <v>29.06666667</v>
       </c>
-      <c r="M3">
+      <c r="P3">
         <v>21.233333330000001</v>
       </c>
-      <c r="Q3">
+      <c r="T3">
         <v>50.3</v>
       </c>
-      <c r="R3">
+      <c r="U3">
         <v>5.0692481989999996</v>
       </c>
-      <c r="T3">
+      <c r="W3">
         <v>1.8245937029999999</v>
       </c>
-      <c r="X3">
+      <c r="AA3">
         <v>1.476158393</v>
       </c>
-      <c r="Z3">
+      <c r="AC3">
         <v>0.38724224699999998</v>
       </c>
-      <c r="AD3">
+      <c r="AG3">
         <v>1.8634006400000001</v>
       </c>
-      <c r="AE3">
+      <c r="AH3">
         <v>1.396620913</v>
       </c>
-      <c r="AF3">
+      <c r="AI3">
         <v>36472.462169999999</v>
       </c>
-      <c r="AG3">
+      <c r="AJ3">
         <v>36472.462169999999</v>
       </c>
-      <c r="AH3">
+      <c r="AK3">
         <v>704.44444439999995</v>
       </c>
-      <c r="AI3">
+      <c r="AL3">
         <v>158.88999999999999</v>
       </c>
-      <c r="AK3">
+      <c r="AN3">
         <v>2.0816659990000002</v>
       </c>
-      <c r="AL3">
+      <c r="AO3">
         <v>3.5118845840000001</v>
       </c>
-      <c r="AM3">
+      <c r="AP3">
         <v>0.33501243800000002</v>
       </c>
-      <c r="AO3">
+      <c r="AR3">
         <v>0.17414084099999999</v>
       </c>
-      <c r="AP3">
+      <c r="AS3">
         <v>0.97779424000000004</v>
       </c>
-      <c r="AQ3">
+      <c r="AT3">
         <v>1.2096831539999999</v>
       </c>
-      <c r="AS3">
+      <c r="AV3">
         <v>1.2096831539999999</v>
       </c>
-      <c r="AT3">
+      <c r="AW3">
         <v>1.1372481409999999</v>
       </c>
-      <c r="AX3">
+      <c r="BA3">
         <v>22.5166605</v>
       </c>
-      <c r="AY3">
+      <c r="BB3">
         <v>0.40163393800000002</v>
       </c>
-      <c r="BA3">
+      <c r="BD3">
         <v>3.4294910999999997E-2</v>
       </c>
-      <c r="BE3">
+      <c r="BH3">
         <v>0.171303912</v>
       </c>
-      <c r="BG3">
+      <c r="BJ3">
         <v>1.6357283E-2</v>
       </c>
-      <c r="BK3">
+      <c r="BN3">
         <v>0.18747316999999999</v>
       </c>
-      <c r="BL3">
+      <c r="BO3">
         <v>9.5373146000000006E-2</v>
       </c>
-      <c r="BM3">
+      <c r="BP3">
         <v>4554.4144660000002</v>
       </c>
-      <c r="BN3">
+      <c r="BQ3">
         <v>4554.4144660000002</v>
       </c>
-      <c r="BO3">
+      <c r="BR3">
         <v>15.39600718</v>
       </c>
-      <c r="BP3">
+      <c r="BS3">
         <v>1.922576396</v>
       </c>
     </row>
-    <row r="4" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1811,122 +1910,125 @@
         <v>42926</v>
       </c>
       <c r="C4" s="4"/>
-      <c r="D4">
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4">
         <v>32.333333330000002</v>
       </c>
-      <c r="E4">
+      <c r="H4">
         <v>32.666666669999998</v>
       </c>
-      <c r="F4">
+      <c r="I4">
         <v>10.33333333</v>
       </c>
-      <c r="H4">
+      <c r="K4">
         <v>2.6299103330000002</v>
       </c>
-      <c r="I4">
+      <c r="L4">
         <v>23.228438700000002</v>
       </c>
-      <c r="J4">
+      <c r="M4">
         <v>91</v>
       </c>
-      <c r="L4">
+      <c r="O4">
         <v>91</v>
       </c>
-      <c r="M4">
+      <c r="P4">
         <v>89.85</v>
       </c>
-      <c r="Q4">
+      <c r="T4">
         <v>180.85</v>
       </c>
-      <c r="R4">
+      <c r="U4">
         <v>5.2969261809999999</v>
       </c>
-      <c r="T4">
+      <c r="W4">
         <v>1.830695073</v>
       </c>
-      <c r="X4">
+      <c r="AA4">
         <v>4.8199299030000002</v>
       </c>
-      <c r="Z4">
+      <c r="AC4">
         <v>1.626351627</v>
       </c>
-      <c r="AD4">
+      <c r="AG4">
         <v>6.4462815300000003</v>
       </c>
-      <c r="AE4">
+      <c r="AH4">
         <v>1.862830607</v>
       </c>
-      <c r="AF4">
+      <c r="AI4">
         <v>29045.95592</v>
       </c>
-      <c r="AG4">
+      <c r="AJ4">
         <v>29045.95592</v>
       </c>
-      <c r="AH4">
+      <c r="AK4">
         <v>1085</v>
       </c>
-      <c r="AI4">
+      <c r="AL4">
         <v>334.33333329999999</v>
       </c>
-      <c r="AK4">
+      <c r="AN4">
         <v>3.2145502540000002</v>
       </c>
-      <c r="AL4">
+      <c r="AO4">
         <v>4.9328828619999996</v>
       </c>
-      <c r="AM4">
+      <c r="AP4">
         <v>0.66500626600000001</v>
       </c>
-      <c r="AO4">
+      <c r="AR4">
         <v>0.46288053699999998</v>
       </c>
-      <c r="AP4">
+      <c r="AS4">
         <v>3.2982417559999999</v>
       </c>
-      <c r="AQ4">
+      <c r="AT4">
         <v>9.4684159179999998</v>
       </c>
-      <c r="AS4">
+      <c r="AV4">
         <v>9.4684159179999998</v>
       </c>
-      <c r="AT4">
+      <c r="AW4">
         <v>15.176860680000001</v>
       </c>
-      <c r="AX4">
+      <c r="BA4">
         <v>238.09991600000001</v>
       </c>
-      <c r="AY4">
+      <c r="BB4">
         <v>6.9166196999999999E-2</v>
       </c>
-      <c r="BA4">
+      <c r="BD4">
         <v>0.18654817900000001</v>
       </c>
-      <c r="BE4">
+      <c r="BH4">
         <v>0.499844024</v>
       </c>
-      <c r="BG4">
+      <c r="BJ4">
         <v>0.128898914</v>
       </c>
-      <c r="BK4">
+      <c r="BN4">
         <v>0.62868809000000003</v>
       </c>
-      <c r="BL4">
+      <c r="BO4">
         <v>0.33258388300000002</v>
       </c>
-      <c r="BM4">
+      <c r="BP4">
         <v>5162.1325269999998</v>
       </c>
-      <c r="BN4">
+      <c r="BQ4">
         <v>5162.1325269999998</v>
       </c>
-      <c r="BO4">
+      <c r="BR4">
         <v>63.83572667</v>
       </c>
-      <c r="BP4">
+      <c r="BS4">
         <v>25.026652460000001</v>
       </c>
     </row>
-    <row r="5" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1934,164 +2036,167 @@
         <v>42942</v>
       </c>
       <c r="C5" s="4"/>
-      <c r="D5">
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5">
         <v>31</v>
       </c>
-      <c r="E5">
+      <c r="H5">
         <v>23.666666670000001</v>
       </c>
-      <c r="F5">
+      <c r="I5">
         <v>16.11</v>
       </c>
-      <c r="G5">
+      <c r="J5">
         <v>29.943333330000002</v>
       </c>
-      <c r="H5">
+      <c r="K5">
         <v>3.5467477330000001</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>25.804700629999999</v>
       </c>
-      <c r="J5">
+      <c r="M5">
         <v>142.46666669999999</v>
       </c>
-      <c r="K5">
+      <c r="N5">
         <v>13.6</v>
       </c>
-      <c r="L5">
+      <c r="O5">
         <v>156.06666670000001</v>
       </c>
-      <c r="M5">
+      <c r="P5">
         <v>211.7</v>
       </c>
-      <c r="N5">
+      <c r="Q5">
         <v>7.0333333329999999</v>
       </c>
-      <c r="Q5">
+      <c r="T5">
         <v>374.8</v>
       </c>
-      <c r="R5">
+      <c r="U5">
         <v>5.2664065359999999</v>
       </c>
-      <c r="S5">
+      <c r="V5">
         <v>2.4026684359999999</v>
       </c>
-      <c r="T5">
+      <c r="W5">
         <v>1.5933583579999999</v>
       </c>
-      <c r="U5">
+      <c r="X5">
         <v>3.462394953</v>
       </c>
-      <c r="X5">
+      <c r="AA5">
         <v>7.4919406620000002</v>
       </c>
-      <c r="Y5">
+      <c r="AB5">
         <v>0.32024770200000002</v>
       </c>
-      <c r="Z5">
+      <c r="AC5">
         <v>3.3575160039999998</v>
       </c>
-      <c r="AA5">
+      <c r="AD5">
         <v>0.24408219</v>
       </c>
-      <c r="AD5">
+      <c r="AG5">
         <v>11.41378656</v>
       </c>
-      <c r="AE5">
+      <c r="AH5">
         <v>2.1940391859999999</v>
       </c>
-      <c r="AF5">
+      <c r="AI5">
         <v>24806.254580000001</v>
       </c>
-      <c r="AG5">
+      <c r="AJ5">
         <v>22662.548620000001</v>
       </c>
-      <c r="AH5">
+      <c r="AK5">
         <v>1218.333333</v>
       </c>
-      <c r="AI5">
+      <c r="AL5">
         <v>588.33333330000005</v>
       </c>
-      <c r="AK5">
+      <c r="AN5">
         <v>5</v>
       </c>
-      <c r="AL5">
+      <c r="AO5">
         <v>6.1101009270000004</v>
       </c>
-      <c r="AM5">
+      <c r="AP5">
         <v>1.168888361</v>
       </c>
-      <c r="AN5">
+      <c r="AQ5">
         <v>4.3617236650000004</v>
       </c>
-      <c r="AO5">
+      <c r="AR5">
         <v>0.85323291099999998</v>
       </c>
-      <c r="AP5">
+      <c r="AS5">
         <v>2.0822463170000001</v>
       </c>
-      <c r="AQ5">
+      <c r="AT5">
         <v>8.8911941460000001</v>
       </c>
-      <c r="AR5">
+      <c r="AU5">
         <v>1.8248287590000001</v>
       </c>
-      <c r="AS5">
+      <c r="AV5">
         <v>10.46151678</v>
       </c>
-      <c r="AT5">
+      <c r="AW5">
         <v>21.254411309999998</v>
       </c>
-      <c r="AU5">
+      <c r="AX5">
         <v>2.0502032419999998</v>
       </c>
-      <c r="AX5">
+      <c r="BA5">
         <v>291.83557009999998</v>
       </c>
-      <c r="AY5">
+      <c r="BB5">
         <v>0.18584066599999999</v>
       </c>
-      <c r="AZ5">
+      <c r="BC5">
         <v>0.61849928700000001</v>
       </c>
-      <c r="BA5">
+      <c r="BD5">
         <v>0.13053358400000001</v>
       </c>
-      <c r="BB5">
+      <c r="BE5">
         <v>4.5969863999999999E-2</v>
       </c>
-      <c r="BE5">
+      <c r="BH5">
         <v>0.20450197000000001</v>
       </c>
-      <c r="BF5">
+      <c r="BI5">
         <v>5.2578893000000002E-2</v>
       </c>
-      <c r="BG5">
+      <c r="BJ5">
         <v>0.168207088</v>
       </c>
-      <c r="BH5">
+      <c r="BK5">
         <v>7.3650926000000005E-2</v>
       </c>
-      <c r="BK5">
+      <c r="BN5">
         <v>0.26653564099999999</v>
       </c>
-      <c r="BL5">
+      <c r="BO5">
         <v>0.52397094600000005</v>
       </c>
-      <c r="BM5">
+      <c r="BP5">
         <v>5045.6976729999997</v>
       </c>
-      <c r="BN5">
+      <c r="BQ5">
         <v>4682.6751670000003</v>
       </c>
-      <c r="BO5">
+      <c r="BR5">
         <v>127.1154331</v>
       </c>
-      <c r="BP5">
+      <c r="BS5">
         <v>38.837267330000003</v>
       </c>
     </row>
-    <row r="6" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -2099,161 +2204,164 @@
         <v>42951</v>
       </c>
       <c r="C6" s="4"/>
-      <c r="D6">
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6">
         <v>31</v>
       </c>
-      <c r="E6">
+      <c r="H6">
         <v>32.333333330000002</v>
       </c>
-      <c r="F6">
+      <c r="I6">
         <v>18.11333333</v>
       </c>
-      <c r="G6">
+      <c r="J6">
         <v>67.5</v>
       </c>
-      <c r="H6">
+      <c r="K6">
         <v>4.4898179999999996</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>23.959276200000001</v>
       </c>
-      <c r="J6">
+      <c r="M6">
         <v>171.7666667</v>
       </c>
-      <c r="K6">
+      <c r="N6">
         <v>14.16666667</v>
       </c>
-      <c r="L6">
+      <c r="O6">
         <v>185.93333329999999</v>
       </c>
-      <c r="M6">
+      <c r="P6">
         <v>286.26666669999997</v>
       </c>
-      <c r="N6">
+      <c r="Q6">
         <v>51.5</v>
       </c>
-      <c r="Q6">
+      <c r="T6">
         <v>523.70000000000005</v>
       </c>
-      <c r="R6">
+      <c r="U6">
         <v>4.9020051960000002</v>
       </c>
-      <c r="S6">
+      <c r="V6">
         <v>2.7312035560000001</v>
       </c>
-      <c r="T6">
+      <c r="W6">
         <v>1.4922018850000001</v>
       </c>
-      <c r="U6">
+      <c r="X6">
         <v>3.4</v>
       </c>
-      <c r="X6">
+      <c r="AA6">
         <v>8.395316459</v>
       </c>
-      <c r="Y6">
+      <c r="AB6">
         <v>0.369270916</v>
       </c>
-      <c r="Z6">
+      <c r="AC6">
         <v>4.2699831179999999</v>
       </c>
-      <c r="AA6">
+      <c r="AD6">
         <v>1.7509999999999999</v>
       </c>
-      <c r="AD6">
+      <c r="AG6">
         <v>14.78557049</v>
       </c>
-      <c r="AE6">
+      <c r="AH6">
         <v>1.8879088310000001</v>
       </c>
-      <c r="AF6">
+      <c r="AI6">
         <v>26076.93547</v>
       </c>
-      <c r="AG6">
+      <c r="AJ6">
         <v>24126.09287</v>
       </c>
-      <c r="AH6">
+      <c r="AK6">
         <v>1466.666667</v>
       </c>
-      <c r="AI6">
+      <c r="AL6">
         <v>751.11</v>
       </c>
-      <c r="AK6">
+      <c r="AN6">
         <v>5</v>
       </c>
-      <c r="AL6">
+      <c r="AO6">
         <v>2.309401077</v>
       </c>
-      <c r="AM6">
+      <c r="AP6">
         <v>1.3891124260000001</v>
       </c>
-      <c r="AN6">
+      <c r="AQ6">
         <v>5.4083269129999998</v>
       </c>
-      <c r="AO6">
+      <c r="AR6">
         <v>0.55618144700000005</v>
       </c>
-      <c r="AP6">
+      <c r="AS6">
         <v>1.034755525</v>
       </c>
-      <c r="AQ6">
+      <c r="AT6">
         <v>11.72959221</v>
       </c>
-      <c r="AR6">
+      <c r="AU6">
         <v>9.4118719360000007</v>
       </c>
-      <c r="AS6">
+      <c r="AV6">
         <v>20.71432677</v>
       </c>
-      <c r="AT6">
+      <c r="AW6">
         <v>23.508579990000001</v>
       </c>
-      <c r="AU6">
+      <c r="AX6">
         <v>12.73891675</v>
       </c>
-      <c r="AX6">
+      <c r="BA6">
         <v>559.41844800000001</v>
       </c>
-      <c r="AY6">
+      <c r="BB6">
         <v>0.31818848199999999</v>
       </c>
-      <c r="AZ6">
+      <c r="BC6">
         <v>0.288776054</v>
       </c>
-      <c r="BA6">
+      <c r="BD6">
         <v>0.111296059</v>
       </c>
-      <c r="BE6">
+      <c r="BH6">
         <v>8.5131423999999997E-2</v>
       </c>
-      <c r="BF6">
+      <c r="BI6">
         <v>0.203212321</v>
       </c>
-      <c r="BG6">
+      <c r="BJ6">
         <v>0.44190556399999997</v>
       </c>
-      <c r="BH6">
+      <c r="BK6">
         <v>0.43312317</v>
       </c>
-      <c r="BK6">
+      <c r="BN6">
         <v>0.92400618499999998</v>
       </c>
-      <c r="BL6">
+      <c r="BO6">
         <v>0.218956975</v>
       </c>
-      <c r="BM6">
+      <c r="BP6">
         <v>1456.8509300000001</v>
       </c>
-      <c r="BN6">
+      <c r="BQ6">
         <v>291.09515390000001</v>
       </c>
-      <c r="BO6">
+      <c r="BR6">
         <v>35.472994419999999</v>
       </c>
-      <c r="BP6">
+      <c r="BS6">
         <v>46.227657309999998</v>
       </c>
     </row>
-    <row r="7" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -2261,158 +2369,161 @@
         <v>42968</v>
       </c>
       <c r="C7" s="4"/>
-      <c r="D7">
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7">
         <v>31</v>
       </c>
-      <c r="E7">
+      <c r="H7">
         <v>33.666666669999998</v>
       </c>
-      <c r="F7">
+      <c r="I7">
         <v>20.88666667</v>
       </c>
-      <c r="G7">
+      <c r="J7">
         <v>73.556666669999998</v>
       </c>
-      <c r="H7">
+      <c r="K7">
         <v>4.4933822670000003</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>24.640407339999999</v>
       </c>
-      <c r="J7">
+      <c r="M7">
         <v>182.15666669999999</v>
       </c>
-      <c r="K7">
+      <c r="N7">
         <v>5.1566666669999996</v>
       </c>
-      <c r="L7">
+      <c r="O7">
         <v>187.31333330000001</v>
       </c>
-      <c r="M7">
+      <c r="P7">
         <v>317.98333330000003</v>
       </c>
-      <c r="N7">
+      <c r="Q7">
         <v>217.55666669999999</v>
       </c>
-      <c r="Q7">
+      <c r="T7">
         <v>722.85333330000003</v>
       </c>
-      <c r="R7">
+      <c r="U7">
         <v>4.5780029300000002</v>
       </c>
-      <c r="S7">
+      <c r="V7">
         <v>2.434477131</v>
       </c>
-      <c r="T7">
+      <c r="W7">
         <v>1.360071177</v>
       </c>
-      <c r="U7">
+      <c r="X7">
         <v>3.3245203499999998</v>
       </c>
-      <c r="X7">
+      <c r="AA7">
         <v>8.3967630989999993</v>
       </c>
-      <c r="Y7">
+      <c r="AB7">
         <v>0.12453468099999999</v>
       </c>
-      <c r="Z7">
+      <c r="AC7">
         <v>4.3441109280000001</v>
       </c>
-      <c r="AA7">
+      <c r="AD7">
         <v>7.2355102880000004</v>
       </c>
-      <c r="AD7">
+      <c r="AG7">
         <v>20.100919000000001</v>
       </c>
-      <c r="AE7">
+      <c r="AH7">
         <v>1.875228895</v>
       </c>
-      <c r="AF7">
+      <c r="AI7">
         <v>24555.750319999999</v>
       </c>
-      <c r="AG7">
+      <c r="AJ7">
         <v>23879.62084</v>
       </c>
-      <c r="AI7">
+      <c r="AL7">
         <v>764.44666670000004</v>
       </c>
-      <c r="AK7">
+      <c r="AN7">
         <v>5</v>
       </c>
-      <c r="AL7">
+      <c r="AO7">
         <v>3.2145502540000002</v>
       </c>
-      <c r="AM7">
+      <c r="AP7">
         <v>1.3891124260000001</v>
       </c>
-      <c r="AN7">
+      <c r="AQ7">
         <v>7.2353046470000004</v>
       </c>
-      <c r="AO7">
+      <c r="AR7">
         <v>0.86346009099999999</v>
       </c>
-      <c r="AP7">
+      <c r="AS7">
         <v>2.576694426</v>
       </c>
-      <c r="AQ7">
+      <c r="AT7">
         <v>19.453620059999999</v>
       </c>
-      <c r="AR7">
+      <c r="AU7">
         <v>0.32145502500000001</v>
       </c>
-      <c r="AS7">
+      <c r="AV7">
         <v>19.296718200000001</v>
       </c>
-      <c r="AT7">
+      <c r="AW7">
         <v>17.073468699999999</v>
       </c>
-      <c r="AU7">
+      <c r="AX7">
         <v>34.734037100000002</v>
       </c>
-      <c r="AX7">
+      <c r="BA7">
         <v>382.55239289999997</v>
       </c>
-      <c r="AY7">
+      <c r="BB7">
         <v>0.45637277100000001</v>
       </c>
-      <c r="AZ7">
+      <c r="BC7">
         <v>0.498811324</v>
       </c>
-      <c r="BA7">
+      <c r="BD7">
         <v>0.230868765</v>
       </c>
-      <c r="BB7">
+      <c r="BE7">
         <v>0.19983250499999999</v>
       </c>
-      <c r="BE7">
+      <c r="BH7">
         <v>1.6763243489999999</v>
       </c>
-      <c r="BF7">
+      <c r="BI7">
         <v>1.8367544E-2</v>
       </c>
-      <c r="BG7">
+      <c r="BJ7">
         <v>0.90041895800000005</v>
       </c>
-      <c r="BH7">
+      <c r="BK7">
         <v>1.2573499420000001</v>
       </c>
-      <c r="BK7">
+      <c r="BN7">
         <v>2.554901455</v>
       </c>
-      <c r="BL7">
+      <c r="BO7">
         <v>0.22672908</v>
       </c>
-      <c r="BM7">
+      <c r="BP7">
         <v>2864.8653640000002</v>
       </c>
-      <c r="BN7">
+      <c r="BQ7">
         <v>2871.5604330000001</v>
       </c>
-      <c r="BP7">
+      <c r="BS7">
         <v>19.532783550000001</v>
       </c>
     </row>
-    <row r="8" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -2420,158 +2531,161 @@
         <v>42983</v>
       </c>
       <c r="C8" s="4"/>
-      <c r="D8">
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8">
         <v>31</v>
       </c>
-      <c r="E8">
+      <c r="H8">
         <v>33.666666669999998</v>
       </c>
-      <c r="F8">
+      <c r="I8">
         <v>20.88666667</v>
       </c>
-      <c r="G8">
+      <c r="J8">
         <v>61.39</v>
       </c>
-      <c r="H8">
+      <c r="K8">
         <v>3.3484526670000001</v>
       </c>
-      <c r="I8">
+      <c r="L8">
         <v>21.194937469999999</v>
       </c>
-      <c r="J8">
+      <c r="M8">
         <v>160.69666670000001</v>
       </c>
-      <c r="K8">
+      <c r="N8">
         <v>25.616666670000001</v>
       </c>
-      <c r="L8">
+      <c r="O8">
         <v>186.31333330000001</v>
       </c>
-      <c r="M8">
+      <c r="P8">
         <v>302.48333330000003</v>
       </c>
-      <c r="N8">
+      <c r="Q8">
         <v>409.21666670000002</v>
       </c>
-      <c r="Q8">
+      <c r="T8">
         <v>898.0133333</v>
       </c>
-      <c r="R8">
+      <c r="U8">
         <v>2.7464925450000002</v>
       </c>
-      <c r="S8">
+      <c r="V8">
         <v>1.897563656</v>
       </c>
-      <c r="T8">
+      <c r="W8">
         <v>0.81153414599999996</v>
       </c>
-      <c r="U8">
+      <c r="X8">
         <v>3.87950778</v>
       </c>
-      <c r="X8">
+      <c r="AA8">
         <v>4.4259175710000003</v>
       </c>
-      <c r="Y8">
+      <c r="AB8">
         <v>0.40085383000000002</v>
       </c>
-      <c r="Z8">
+      <c r="AC8">
         <v>2.4556705980000002</v>
       </c>
-      <c r="AA8">
+      <c r="AD8">
         <v>15.840236429999999</v>
       </c>
-      <c r="AD8">
+      <c r="AG8">
         <v>23.122678430000001</v>
       </c>
-      <c r="AE8">
+      <c r="AH8">
         <v>1.326094729</v>
       </c>
-      <c r="AF8">
+      <c r="AI8">
         <v>20822.952379999999</v>
       </c>
-      <c r="AG8">
+      <c r="AJ8">
         <v>18258.099859999998</v>
       </c>
-      <c r="AI8">
+      <c r="AL8">
         <v>764.44666670000004</v>
       </c>
-      <c r="AK8">
+      <c r="AN8">
         <v>5</v>
       </c>
-      <c r="AL8">
+      <c r="AO8">
         <v>6.1101009270000004</v>
       </c>
-      <c r="AM8">
+      <c r="AP8">
         <v>1.3891124260000001</v>
       </c>
-      <c r="AN8">
+      <c r="AQ8">
         <v>6.4250525290000002</v>
       </c>
-      <c r="AO8">
+      <c r="AR8">
         <v>0.45081993999999997</v>
       </c>
-      <c r="AP8">
+      <c r="AS8">
         <v>1.0506225199999999</v>
       </c>
-      <c r="AQ8">
+      <c r="AT8">
         <v>14.28787365</v>
       </c>
-      <c r="AR8">
+      <c r="AU8">
         <v>25.268004139999999</v>
       </c>
-      <c r="AS8">
+      <c r="AV8">
         <v>24.959227420000001</v>
       </c>
-      <c r="AT8">
+      <c r="AW8">
         <v>8.0512938920000003</v>
       </c>
-      <c r="AU8">
+      <c r="AX8">
         <v>16.405305039999998</v>
       </c>
-      <c r="AX8">
+      <c r="BA8">
         <v>486.49708459999999</v>
       </c>
-      <c r="AY8">
+      <c r="BB8">
         <v>0.131513876</v>
       </c>
-      <c r="AZ8">
+      <c r="BC8">
         <v>0.51635507199999997</v>
       </c>
-      <c r="BA8">
+      <c r="BD8">
         <v>0.156608992</v>
       </c>
-      <c r="BB8">
+      <c r="BE8">
         <v>0.442822455</v>
       </c>
-      <c r="BE8">
+      <c r="BH8">
         <v>0.60551635000000004</v>
       </c>
-      <c r="BF8">
+      <c r="BI8">
         <v>0.28019391900000001</v>
       </c>
-      <c r="BG8">
+      <c r="BJ8">
         <v>0.48310399900000001</v>
       </c>
-      <c r="BH8">
+      <c r="BK8">
         <v>1.4177898360000001</v>
       </c>
-      <c r="BK8">
+      <c r="BN8">
         <v>2.2663543150000001</v>
       </c>
-      <c r="BL8">
+      <c r="BO8">
         <v>0.13615085800000001</v>
       </c>
-      <c r="BM8">
+      <c r="BP8">
         <v>1816.972784</v>
       </c>
-      <c r="BN8">
+      <c r="BQ8">
         <v>3785.7399789999999</v>
       </c>
-      <c r="BP8">
+      <c r="BS8">
         <v>19.532783550000001</v>
       </c>
     </row>
-    <row r="9" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>3</v>
       </c>
@@ -2579,170 +2693,173 @@
         <v>42997</v>
       </c>
       <c r="C9" s="4"/>
-      <c r="D9">
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9">
         <v>31</v>
       </c>
-      <c r="E9">
+      <c r="H9">
         <v>32.333333330000002</v>
       </c>
-      <c r="F9">
+      <c r="I9">
         <v>20.88666667</v>
       </c>
-      <c r="G9">
+      <c r="J9">
         <v>62.666666669999998</v>
       </c>
-      <c r="J9">
+      <c r="M9">
         <v>15.393333330000001</v>
       </c>
-      <c r="K9">
+      <c r="N9">
         <v>14.86</v>
       </c>
-      <c r="L9">
+      <c r="O9">
         <v>30.25333333</v>
       </c>
-      <c r="M9">
+      <c r="P9">
         <v>213.95</v>
       </c>
-      <c r="N9">
+      <c r="Q9">
         <v>444.09</v>
       </c>
-      <c r="O9">
+      <c r="R9">
         <v>125.55666669999999</v>
       </c>
-      <c r="P9">
+      <c r="S9">
         <v>318.53333329999998</v>
       </c>
-      <c r="Q9">
+      <c r="T9">
         <v>688.29333329999997</v>
       </c>
-      <c r="R9">
+      <c r="U9">
         <v>2.2859224079999998</v>
       </c>
-      <c r="S9">
+      <c r="V9">
         <v>1.7393941879999999</v>
       </c>
-      <c r="T9">
+      <c r="W9">
         <v>0.490818898</v>
       </c>
-      <c r="U9">
+      <c r="X9">
         <v>4.4114886699999998</v>
       </c>
-      <c r="V9">
+      <c r="Y9">
         <v>0.79016911999999995</v>
       </c>
-      <c r="W9">
+      <c r="Z9">
         <v>5.8392753600000002</v>
       </c>
-      <c r="X9">
+      <c r="AA9">
         <v>0.36035655300000002</v>
       </c>
-      <c r="Y9">
+      <c r="AB9">
         <v>0.24390679800000001</v>
       </c>
-      <c r="Z9">
+      <c r="AC9">
         <v>1.0493157440000001</v>
       </c>
-      <c r="AA9">
+      <c r="AD9">
         <v>19.553729329999999</v>
       </c>
-      <c r="AB9">
+      <c r="AE9">
         <v>0.99398109099999998</v>
       </c>
-      <c r="AC9">
+      <c r="AF9">
         <v>18.559748240000001</v>
       </c>
-      <c r="AD9">
+      <c r="AG9">
         <v>21.20730842</v>
       </c>
-      <c r="AI9">
+      <c r="AL9">
         <v>764.44666670000004</v>
       </c>
-      <c r="AJ9">
+      <c r="AM9">
         <v>54.553409960000003</v>
       </c>
-      <c r="AK9">
+      <c r="AN9">
         <v>5</v>
       </c>
-      <c r="AL9">
+      <c r="AO9">
         <v>3.0550504630000002</v>
       </c>
-      <c r="AM9">
+      <c r="AP9">
         <v>1.3891124260000001</v>
       </c>
-      <c r="AN9">
+      <c r="AQ9">
         <v>4.6671440229999996</v>
       </c>
-      <c r="AQ9">
+      <c r="AT9">
         <v>19.191926250000002</v>
       </c>
-      <c r="AR9">
+      <c r="AU9">
         <v>17.12383427</v>
       </c>
-      <c r="AS9">
+      <c r="AV9">
         <v>36.310441109999999</v>
       </c>
-      <c r="AT9">
+      <c r="AW9">
         <v>62.57163894</v>
       </c>
-      <c r="AU9">
+      <c r="AX9">
         <v>71.288638649999996</v>
       </c>
-      <c r="AV9">
+      <c r="AY9">
         <v>19.623540290000001</v>
       </c>
-      <c r="AW9">
+      <c r="AZ9">
         <v>51.892228060000001</v>
       </c>
-      <c r="AX9">
+      <c r="BA9">
         <v>1351.075206</v>
       </c>
-      <c r="AY9">
+      <c r="BB9">
         <v>0.28147503000000001</v>
       </c>
-      <c r="AZ9">
+      <c r="BC9">
         <v>0.12760889</v>
       </c>
-      <c r="BA9">
+      <c r="BD9">
         <v>6.7670759999999996E-2</v>
       </c>
-      <c r="BB9">
+      <c r="BE9">
         <v>0.37165287400000002</v>
       </c>
-      <c r="BC9">
+      <c r="BF9">
         <v>0.143930472</v>
       </c>
-      <c r="BD9">
+      <c r="BG9">
         <v>0.42906704699999998</v>
       </c>
-      <c r="BE9">
+      <c r="BH9">
         <v>0.49645715800000001</v>
       </c>
-      <c r="BF9">
+      <c r="BI9">
         <v>0.26708691099999998</v>
       </c>
-      <c r="BG9">
+      <c r="BJ9">
         <v>0.358529082</v>
       </c>
-      <c r="BH9">
+      <c r="BK9">
         <v>3.0864769270000001</v>
       </c>
-      <c r="BI9">
+      <c r="BL9">
         <v>0.233257305</v>
       </c>
-      <c r="BJ9">
+      <c r="BM9">
         <v>2.85535483</v>
       </c>
-      <c r="BK9">
+      <c r="BN9">
         <v>3.8043212409999998</v>
       </c>
-      <c r="BP9">
+      <c r="BS9">
         <v>19.532783550000001</v>
       </c>
-      <c r="BQ9">
+      <c r="BT9">
         <v>8.887289634</v>
       </c>
     </row>
-    <row r="10" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>3</v>
       </c>
@@ -2752,20 +2869,23 @@
       <c r="C10" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P10">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="S10">
         <v>310.3</v>
       </c>
-      <c r="AJ10">
+      <c r="AM10">
         <v>53.143333329999997</v>
       </c>
-      <c r="AW10">
+      <c r="AZ10">
         <v>36.299450839999999</v>
       </c>
-      <c r="BQ10">
+      <c r="BT10">
         <v>6.2168025010000001</v>
       </c>
     </row>
-    <row r="11" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>3</v>
       </c>
@@ -2773,14 +2893,17 @@
         <v>42916</v>
       </c>
       <c r="C11" s="4"/>
-      <c r="AH11">
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="AK11">
         <v>877.77777779999997</v>
       </c>
-      <c r="BO11">
+      <c r="BR11">
         <v>42.860670050000003</v>
       </c>
     </row>
-    <row r="12" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -2788,14 +2911,17 @@
         <v>42934</v>
       </c>
       <c r="C12" s="4"/>
-      <c r="AH12">
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="AK12">
         <v>1111.666667</v>
       </c>
-      <c r="BO12">
+      <c r="BR12">
         <v>104.08329999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -2803,122 +2929,125 @@
         <v>42909</v>
       </c>
       <c r="C13" s="4"/>
-      <c r="D13">
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13">
         <v>41</v>
       </c>
-      <c r="E13">
+      <c r="H13">
         <v>41</v>
       </c>
-      <c r="F13">
+      <c r="I13">
         <v>3.6666666669999999</v>
       </c>
-      <c r="H13">
+      <c r="K13">
         <v>0.56501726699999999</v>
       </c>
-      <c r="I13">
+      <c r="L13">
         <v>28.669284189999999</v>
       </c>
-      <c r="J13">
+      <c r="M13">
         <v>17.366666670000001</v>
       </c>
-      <c r="L13">
+      <c r="O13">
         <v>17.366666670000001</v>
       </c>
-      <c r="M13">
+      <c r="P13">
         <v>12.16666667</v>
       </c>
-      <c r="Q13">
+      <c r="T13">
         <v>29.533333329999998</v>
       </c>
-      <c r="R13">
+      <c r="U13">
         <v>5.3513595260000004</v>
       </c>
-      <c r="T13">
+      <c r="W13">
         <v>2.557780186</v>
       </c>
-      <c r="X13">
+      <c r="AA13">
         <v>0.92831271999999998</v>
       </c>
-      <c r="Z13">
+      <c r="AC13">
         <v>0.31247847400000001</v>
       </c>
-      <c r="AD13">
+      <c r="AG13">
         <v>1.240791193</v>
       </c>
-      <c r="AE13">
+      <c r="AH13">
         <v>1.660832965</v>
       </c>
-      <c r="AF13">
+      <c r="AI13">
         <v>32509.90871</v>
       </c>
-      <c r="AG13">
+      <c r="AJ13">
         <v>32509.90871</v>
       </c>
-      <c r="AH13">
+      <c r="AK13">
         <v>600</v>
       </c>
-      <c r="AI13">
+      <c r="AL13">
         <v>118.33333330000001</v>
       </c>
-      <c r="AK13">
+      <c r="AN13">
         <v>2.6457513110000002</v>
       </c>
-      <c r="AL13">
+      <c r="AO13">
         <v>2.6457513110000002</v>
       </c>
-      <c r="AM13">
+      <c r="AP13">
         <v>0.57735026899999997</v>
       </c>
-      <c r="AO13">
+      <c r="AR13">
         <v>7.2568472999999994E-2</v>
       </c>
-      <c r="AP13">
+      <c r="AS13">
         <v>0.63868976399999999</v>
       </c>
-      <c r="AQ13">
+      <c r="AT13">
         <v>0.75718777900000001</v>
       </c>
-      <c r="AS13">
+      <c r="AV13">
         <v>0.75718777900000001</v>
       </c>
-      <c r="AT13">
+      <c r="AW13">
         <v>1.908751774</v>
       </c>
-      <c r="AX13">
+      <c r="BA13">
         <v>26.65207934</v>
       </c>
-      <c r="AY13">
+      <c r="BB13">
         <v>0.213327875</v>
       </c>
-      <c r="BA13">
+      <c r="BD13">
         <v>0.10142232299999999</v>
       </c>
-      <c r="BE13">
+      <c r="BH13">
         <v>1.1554798999999999E-2</v>
       </c>
-      <c r="BG13">
+      <c r="BJ13">
         <v>6.0073020999999997E-2</v>
       </c>
-      <c r="BK13">
+      <c r="BN13">
         <v>6.5997679000000004E-2</v>
       </c>
-      <c r="BL13">
+      <c r="BO13">
         <v>0.20978332699999999</v>
       </c>
-      <c r="BM13">
+      <c r="BP13">
         <v>3518.26377</v>
       </c>
-      <c r="BN13">
+      <c r="BQ13">
         <v>3518.26377</v>
       </c>
-      <c r="BO13">
+      <c r="BR13">
         <v>17.63834207</v>
       </c>
-      <c r="BP13">
+      <c r="BS13">
         <v>4.407066296</v>
       </c>
     </row>
-    <row r="14" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -2926,122 +3055,125 @@
         <v>42926</v>
       </c>
       <c r="C14" s="4"/>
-      <c r="D14">
+      <c r="D14" s="4"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14">
         <v>36.333333330000002</v>
       </c>
-      <c r="E14">
+      <c r="H14">
         <v>32.666666669999998</v>
       </c>
-      <c r="F14">
+      <c r="I14">
         <v>7.1133333329999999</v>
       </c>
-      <c r="H14">
+      <c r="K14">
         <v>1.333144933</v>
       </c>
-      <c r="I14">
+      <c r="L14">
         <v>24.658185629999998</v>
       </c>
-      <c r="J14">
+      <c r="M14">
         <v>60.45</v>
       </c>
-      <c r="L14">
+      <c r="O14">
         <v>60.45</v>
       </c>
-      <c r="M14">
+      <c r="P14">
         <v>47.576666670000002</v>
       </c>
-      <c r="Q14">
+      <c r="T14">
         <v>108.02666670000001</v>
       </c>
-      <c r="R14">
+      <c r="U14">
         <v>5.5619044300000002</v>
       </c>
-      <c r="T14">
+      <c r="W14">
         <v>2.2197982469999999</v>
       </c>
-      <c r="X14">
+      <c r="AA14">
         <v>3.3607650140000001</v>
       </c>
-      <c r="Z14">
+      <c r="AC14">
         <v>1.050690216</v>
       </c>
-      <c r="AD14">
+      <c r="AG14">
         <v>4.4114552299999996</v>
       </c>
-      <c r="AE14">
+      <c r="AH14">
         <v>2.591035186</v>
       </c>
-      <c r="AF14">
+      <c r="AI14">
         <v>21961.912329999999</v>
       </c>
-      <c r="AG14">
+      <c r="AJ14">
         <v>21961.912329999999</v>
       </c>
-      <c r="AH14">
+      <c r="AK14">
         <v>858.33333330000005</v>
       </c>
-      <c r="AI14">
+      <c r="AL14">
         <v>237.78</v>
       </c>
-      <c r="AK14">
+      <c r="AN14">
         <v>2.5166114780000002</v>
       </c>
-      <c r="AL14">
+      <c r="AO14">
         <v>7.0945988849999999</v>
       </c>
-      <c r="AM14">
+      <c r="AP14">
         <v>0.96417494999999998</v>
       </c>
-      <c r="AO14">
+      <c r="AR14">
         <v>0.27197959799999999</v>
       </c>
-      <c r="AP14">
+      <c r="AS14">
         <v>3.0724990559999998</v>
       </c>
-      <c r="AQ14">
+      <c r="AT14">
         <v>2.3404059479999999</v>
       </c>
-      <c r="AS14">
+      <c r="AV14">
         <v>2.3404059479999999</v>
       </c>
-      <c r="AT14">
+      <c r="AW14">
         <v>3.6065126279999999</v>
       </c>
-      <c r="AX14">
+      <c r="BA14">
         <v>14.75273986</v>
       </c>
-      <c r="AY14">
+      <c r="BB14">
         <v>0.10581093699999999</v>
       </c>
-      <c r="BA14">
+      <c r="BD14">
         <v>0.225253958</v>
       </c>
-      <c r="BE14">
+      <c r="BH14">
         <v>8.4158015000000003E-2</v>
       </c>
-      <c r="BG14">
+      <c r="BJ14">
         <v>3.0301444E-2</v>
       </c>
-      <c r="BK14">
+      <c r="BN14">
         <v>0.111229473</v>
       </c>
-      <c r="BL14">
+      <c r="BO14">
         <v>0.51737233100000002</v>
       </c>
-      <c r="BM14">
+      <c r="BP14">
         <v>3761.7168099999999</v>
       </c>
-      <c r="BN14">
+      <c r="BQ14">
         <v>3761.7168099999999</v>
       </c>
-      <c r="BO14">
+      <c r="BR14">
         <v>59.231185480000001</v>
       </c>
-      <c r="BP14">
+      <c r="BS14">
         <v>42.861361389999999</v>
       </c>
     </row>
-    <row r="15" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>4</v>
       </c>
@@ -3049,158 +3181,161 @@
         <v>42942</v>
       </c>
       <c r="C15" s="4"/>
-      <c r="D15">
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15">
         <v>36.333333330000002</v>
       </c>
-      <c r="E15">
+      <c r="H15">
         <v>34</v>
       </c>
-      <c r="F15">
+      <c r="I15">
         <v>13.78</v>
       </c>
-      <c r="H15">
+      <c r="K15">
         <v>2.870000133</v>
       </c>
-      <c r="I15">
+      <c r="L15">
         <v>29.498674009999998</v>
       </c>
-      <c r="J15">
+      <c r="M15">
         <v>106.4666667</v>
       </c>
-      <c r="K15">
+      <c r="N15">
         <v>3.95</v>
       </c>
-      <c r="L15">
+      <c r="O15">
         <v>110.41666669999999</v>
       </c>
-      <c r="M15">
+      <c r="P15">
         <v>136.7333333</v>
       </c>
-      <c r="N15">
+      <c r="Q15">
         <v>0.81666666700000001</v>
       </c>
-      <c r="Q15">
+      <c r="T15">
         <v>247.96666669999999</v>
       </c>
-      <c r="R15">
+      <c r="U15">
         <v>5.6759546600000004</v>
       </c>
-      <c r="S15">
+      <c r="V15">
         <v>2.2230339849999998</v>
       </c>
-      <c r="T15">
+      <c r="W15">
         <v>1.49628977</v>
       </c>
-      <c r="U15">
+      <c r="X15">
         <v>3.4290581539999998</v>
       </c>
-      <c r="X15">
+      <c r="AA15">
         <v>6.0370028959999997</v>
       </c>
-      <c r="Y15">
+      <c r="AB15">
         <v>9.2586599000000006E-2</v>
       </c>
-      <c r="Z15">
+      <c r="AC15">
         <v>2.0423830540000001</v>
       </c>
-      <c r="AA15">
+      <c r="AD15">
         <v>2.5147903999999999E-2</v>
       </c>
-      <c r="AD15">
+      <c r="AG15">
         <v>8.1971204530000001</v>
       </c>
-      <c r="AE15">
+      <c r="AH15">
         <v>2.1404846100000001</v>
       </c>
-      <c r="AF15">
+      <c r="AI15">
         <v>26939.467619999999</v>
       </c>
-      <c r="AG15">
+      <c r="AJ15">
         <v>26034.953669999999</v>
       </c>
-      <c r="AH15">
+      <c r="AK15">
         <v>1153.333333</v>
       </c>
-      <c r="AI15">
+      <c r="AL15">
         <v>510</v>
       </c>
-      <c r="AK15">
+      <c r="AN15">
         <v>2.5166114780000002</v>
       </c>
-      <c r="AL15">
+      <c r="AO15">
         <v>5.2915026220000003</v>
       </c>
-      <c r="AM15">
+      <c r="AP15">
         <v>1.168888361</v>
       </c>
-      <c r="AO15">
+      <c r="AR15">
         <v>0.43784565800000003</v>
       </c>
-      <c r="AP15">
+      <c r="AS15">
         <v>0.89697609499999997</v>
       </c>
-      <c r="AQ15">
+      <c r="AT15">
         <v>6.709942871</v>
       </c>
-      <c r="AR15">
+      <c r="AU15">
         <v>2.4864633519999999</v>
       </c>
-      <c r="AS15">
+      <c r="AV15">
         <v>7.3607630940000002</v>
       </c>
-      <c r="AT15">
+      <c r="AW15">
         <v>11.00378723</v>
       </c>
-      <c r="AU15">
+      <c r="AX15">
         <v>0.59651767200000005</v>
       </c>
-      <c r="AX15">
+      <c r="BA15">
         <v>147.6010953</v>
       </c>
-      <c r="AY15">
+      <c r="BB15">
         <v>0.34234834800000002</v>
       </c>
-      <c r="AZ15">
+      <c r="BC15">
         <v>0.388470392</v>
       </c>
-      <c r="BA15">
+      <c r="BD15">
         <v>4.9557148000000002E-2</v>
       </c>
-      <c r="BB15">
+      <c r="BE15">
         <v>0.71820184499999995</v>
       </c>
-      <c r="BE15">
+      <c r="BH15">
         <v>0.41912551599999998</v>
       </c>
-      <c r="BF15">
+      <c r="BI15">
         <v>6.2015540000000001E-2</v>
       </c>
-      <c r="BG15">
+      <c r="BJ15">
         <v>9.9778357999999998E-2</v>
       </c>
-      <c r="BH15">
+      <c r="BK15">
         <v>1.6461156000000001E-2</v>
       </c>
-      <c r="BK15">
+      <c r="BN15">
         <v>0.41153527699999998</v>
       </c>
-      <c r="BL15">
+      <c r="BO15">
         <v>0.37967192900000002</v>
       </c>
-      <c r="BM15">
+      <c r="BP15">
         <v>3588.6822590000002</v>
       </c>
-      <c r="BN15">
+      <c r="BQ15">
         <v>4087.9392079999998</v>
       </c>
-      <c r="BO15">
+      <c r="BR15">
         <v>93.852721500000001</v>
       </c>
-      <c r="BP15">
+      <c r="BS15">
         <v>83.735230939999994</v>
       </c>
     </row>
-    <row r="16" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -3208,161 +3343,164 @@
         <v>42951</v>
       </c>
       <c r="C16" s="4"/>
-      <c r="D16">
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16">
         <v>36.333333330000002</v>
       </c>
-      <c r="E16">
+      <c r="H16">
         <v>38.333333330000002</v>
       </c>
-      <c r="F16">
+      <c r="I16">
         <v>15.61</v>
       </c>
-      <c r="G16">
+      <c r="J16">
         <v>36.776666669999997</v>
       </c>
-      <c r="H16">
+      <c r="K16">
         <v>4.6754084669999996</v>
       </c>
-      <c r="I16">
+      <c r="L16">
         <v>23.288884029999998</v>
       </c>
-      <c r="J16">
+      <c r="M16">
         <v>166.5</v>
       </c>
-      <c r="K16">
+      <c r="N16">
         <v>3.766666667</v>
       </c>
-      <c r="L16">
+      <c r="O16">
         <v>170.2666667</v>
       </c>
-      <c r="M16">
+      <c r="P16">
         <v>256.60000000000002</v>
       </c>
-      <c r="N16">
+      <c r="Q16">
         <v>19.666666670000001</v>
       </c>
-      <c r="Q16">
+      <c r="T16">
         <v>446.53333329999998</v>
       </c>
-      <c r="R16">
+      <c r="U16">
         <v>4.7166145640000003</v>
       </c>
-      <c r="S16">
+      <c r="V16">
         <v>2.4504482350000001</v>
       </c>
-      <c r="T16">
+      <c r="W16">
         <v>1.330648343</v>
       </c>
-      <c r="U16">
+      <c r="X16">
         <v>3.5</v>
       </c>
-      <c r="X16">
+      <c r="AA16">
         <v>7.7601181229999998</v>
       </c>
-      <c r="Y16">
+      <c r="AB16">
         <v>9.6129725999999999E-2</v>
       </c>
-      <c r="Z16">
+      <c r="AC16">
         <v>3.3425547560000002</v>
       </c>
-      <c r="AA16">
+      <c r="AD16">
         <v>0.68833333299999999</v>
       </c>
-      <c r="AD16">
+      <c r="AG16">
         <v>11.88713594</v>
       </c>
-      <c r="AE16">
+      <c r="AH16">
         <v>1.6701437029999999</v>
       </c>
-      <c r="AF16">
+      <c r="AI16">
         <v>28207.598379999999</v>
       </c>
-      <c r="AG16">
+      <c r="AJ16">
         <v>27540.923060000001</v>
       </c>
-      <c r="AH16">
+      <c r="AK16">
         <v>1235</v>
       </c>
-      <c r="AI16">
+      <c r="AL16">
         <v>665.55333329999996</v>
       </c>
-      <c r="AK16">
+      <c r="AN16">
         <v>2.5166114780000002</v>
       </c>
-      <c r="AL16">
+      <c r="AO16">
         <v>2.0816659990000002</v>
       </c>
-      <c r="AM16">
+      <c r="AP16">
         <v>0.67178865700000001</v>
       </c>
-      <c r="AN16">
+      <c r="AQ16">
         <v>2.1444191130000001</v>
       </c>
-      <c r="AO16">
+      <c r="AR16">
         <v>0.75047234600000001</v>
       </c>
-      <c r="AP16">
+      <c r="AS16">
         <v>0.71532856499999997</v>
       </c>
-      <c r="AQ16">
+      <c r="AT16">
         <v>32.922332849999997</v>
       </c>
-      <c r="AR16">
+      <c r="AU16">
         <v>1.4047538340000001</v>
       </c>
-      <c r="AS16">
+      <c r="AV16">
         <v>31.731582580000001</v>
       </c>
-      <c r="AT16">
+      <c r="AW16">
         <v>62.276881750000001</v>
       </c>
-      <c r="AU16">
+      <c r="AX16">
         <v>8.0002083309999996</v>
       </c>
-      <c r="AX16">
+      <c r="BA16">
         <v>1015.488716</v>
       </c>
-      <c r="AY16">
+      <c r="BB16">
         <v>0.42883606299999999</v>
       </c>
-      <c r="AZ16">
+      <c r="BC16">
         <v>0.48703883199999998</v>
       </c>
-      <c r="BA16">
+      <c r="BD16">
         <v>0.20050975200000001</v>
       </c>
-      <c r="BE16">
+      <c r="BH16">
         <v>0.77755899100000003</v>
       </c>
-      <c r="BF16">
+      <c r="BI16">
         <v>4.7494438999999999E-2</v>
       </c>
-      <c r="BG16">
+      <c r="BJ16">
         <v>0.404080877</v>
       </c>
-      <c r="BH16">
+      <c r="BK16">
         <v>0.28000729200000002</v>
       </c>
-      <c r="BK16">
+      <c r="BN16">
         <v>1.401819975</v>
       </c>
-      <c r="BL16">
+      <c r="BO16">
         <v>0.101699416</v>
       </c>
-      <c r="BM16">
+      <c r="BP16">
         <v>992.64098639999997</v>
       </c>
-      <c r="BN16">
+      <c r="BQ16">
         <v>668.4282283</v>
       </c>
-      <c r="BO16">
+      <c r="BR16">
         <v>86.746757860000002</v>
       </c>
-      <c r="BP16">
+      <c r="BS16">
         <v>110.67036469999999</v>
       </c>
     </row>
-    <row r="17" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>4</v>
       </c>
@@ -3370,158 +3508,161 @@
         <v>42968</v>
       </c>
       <c r="C17" s="4"/>
-      <c r="D17">
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17">
         <v>36.333333330000002</v>
       </c>
-      <c r="E17">
+      <c r="H17">
         <v>35</v>
       </c>
-      <c r="F17">
+      <c r="I17">
         <v>16.39</v>
       </c>
-      <c r="G17">
+      <c r="J17">
         <v>50</v>
       </c>
-      <c r="H17">
+      <c r="K17">
         <v>5.2218760670000002</v>
       </c>
-      <c r="I17">
+      <c r="L17">
         <v>26.034529389999999</v>
       </c>
-      <c r="J17">
+      <c r="M17">
         <v>177.59</v>
       </c>
-      <c r="K17">
+      <c r="N17">
         <v>4.8566666669999998</v>
       </c>
-      <c r="L17">
+      <c r="O17">
         <v>182.44666670000001</v>
       </c>
-      <c r="M17">
+      <c r="P17">
         <v>306.48333330000003</v>
       </c>
-      <c r="N17">
+      <c r="Q17">
         <v>137.35666670000001</v>
       </c>
-      <c r="Q17">
+      <c r="T17">
         <v>626.28666670000007</v>
       </c>
-      <c r="R17">
+      <c r="U17">
         <v>4.7927247680000002</v>
       </c>
-      <c r="S17">
+      <c r="V17">
         <v>2.4406307140000001</v>
       </c>
-      <c r="T17">
+      <c r="W17">
         <v>1.375053326</v>
       </c>
-      <c r="U17">
+      <c r="X17">
         <v>3.5871027309999999</v>
       </c>
-      <c r="X17">
+      <c r="AA17">
         <v>8.4749179560000005</v>
       </c>
-      <c r="Y17">
+      <c r="AB17">
         <v>0.112247159</v>
       </c>
-      <c r="Z17">
+      <c r="AC17">
         <v>4.1794316409999999</v>
       </c>
-      <c r="AA17">
+      <c r="AD17">
         <v>4.9122820190000001</v>
       </c>
-      <c r="AD17">
+      <c r="AG17">
         <v>17.678878780000002</v>
       </c>
-      <c r="AE17">
+      <c r="AH17">
         <v>1.622554703</v>
       </c>
-      <c r="AF17">
+      <c r="AI17">
         <v>29646.15581</v>
       </c>
-      <c r="AG17">
+      <c r="AJ17">
         <v>28857.855530000001</v>
       </c>
-      <c r="AI17">
+      <c r="AL17">
         <v>733.33333330000005</v>
       </c>
-      <c r="AK17">
+      <c r="AN17">
         <v>2.5166114780000002</v>
       </c>
-      <c r="AL17">
+      <c r="AO17">
         <v>1.7320508080000001</v>
       </c>
-      <c r="AM17">
+      <c r="AP17">
         <v>0.348281495</v>
       </c>
-      <c r="AN17">
+      <c r="AQ17">
         <v>10.440306509999999</v>
       </c>
-      <c r="AO17">
+      <c r="AR17">
         <v>8.9865407999999994E-2</v>
       </c>
-      <c r="AP17">
+      <c r="AS17">
         <v>1.8305064879999999</v>
       </c>
-      <c r="AQ17">
+      <c r="AT17">
         <v>19.2779667</v>
       </c>
-      <c r="AR17">
+      <c r="AU17">
         <v>2.2501851780000002</v>
       </c>
-      <c r="AS17">
+      <c r="AV17">
         <v>19.828346710000002</v>
       </c>
-      <c r="AT17">
+      <c r="AW17">
         <v>37.884209550000001</v>
       </c>
-      <c r="AU17">
+      <c r="AX17">
         <v>20.123949249999999</v>
       </c>
-      <c r="AX17">
+      <c r="BA17">
         <v>741.52028519999999</v>
       </c>
-      <c r="AY17">
+      <c r="BB17">
         <v>0.32390440599999998</v>
       </c>
-      <c r="AZ17">
+      <c r="BC17">
         <v>0.44870957700000003</v>
       </c>
-      <c r="BA17">
+      <c r="BD17">
         <v>0.30498844600000002</v>
       </c>
-      <c r="BB17">
+      <c r="BE17">
         <v>0.113142141</v>
       </c>
-      <c r="BE17">
+      <c r="BH17">
         <v>0.53440854000000004</v>
       </c>
-      <c r="BF17">
+      <c r="BI17">
         <v>3.5300312E-2</v>
       </c>
-      <c r="BG17">
+      <c r="BJ17">
         <v>0.90320213199999999</v>
       </c>
-      <c r="BH17">
+      <c r="BK17">
         <v>0.55779815600000004</v>
       </c>
-      <c r="BK17">
+      <c r="BN17">
         <v>1.258361353</v>
       </c>
-      <c r="BL17">
+      <c r="BO17">
         <v>8.7457088000000002E-2</v>
       </c>
-      <c r="BM17">
+      <c r="BP17">
         <v>3364.5618420000001</v>
       </c>
-      <c r="BN17">
+      <c r="BQ17">
         <v>3278.8751830000001</v>
       </c>
-      <c r="BP17">
+      <c r="BS17">
         <v>106.5078506</v>
       </c>
     </row>
-    <row r="18" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>4</v>
       </c>
@@ -3529,158 +3670,161 @@
         <v>42983</v>
       </c>
       <c r="C18" s="4"/>
-      <c r="D18">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18">
         <v>36.333333330000002</v>
       </c>
-      <c r="E18">
+      <c r="H18">
         <v>37.666666669999998</v>
       </c>
-      <c r="F18">
+      <c r="I18">
         <v>16.39</v>
       </c>
-      <c r="G18">
+      <c r="J18">
         <v>37.166666669999998</v>
       </c>
-      <c r="H18">
+      <c r="K18">
         <v>4.4241513330000002</v>
       </c>
-      <c r="I18">
+      <c r="L18">
         <v>22.268321570000001</v>
       </c>
-      <c r="J18">
+      <c r="M18">
         <v>174.93</v>
       </c>
-      <c r="K18">
+      <c r="N18">
         <v>14.956666670000001</v>
       </c>
-      <c r="L18">
+      <c r="O18">
         <v>189.88666670000001</v>
       </c>
-      <c r="M18">
+      <c r="P18">
         <v>315.51666669999997</v>
       </c>
-      <c r="N18">
+      <c r="Q18">
         <v>298.65333329999999</v>
       </c>
-      <c r="Q18">
+      <c r="T18">
         <v>804.05666670000005</v>
       </c>
-      <c r="R18">
+      <c r="U18">
         <v>3.4432400859999999</v>
       </c>
-      <c r="S18">
+      <c r="V18">
         <v>1.938536008</v>
       </c>
-      <c r="T18">
+      <c r="W18">
         <v>0.93853016700000003</v>
       </c>
-      <c r="U18">
+      <c r="X18">
         <v>3.5966654619999998</v>
       </c>
-      <c r="X18">
+      <c r="AA18">
         <v>5.9953915029999996</v>
       </c>
-      <c r="Y18">
+      <c r="AB18">
         <v>0.29116908899999999</v>
       </c>
-      <c r="Z18">
+      <c r="AC18">
         <v>2.9563275170000001</v>
       </c>
-      <c r="AA18">
+      <c r="AD18">
         <v>10.73565777</v>
       </c>
-      <c r="AD18">
+      <c r="AG18">
         <v>19.978545879999999</v>
       </c>
-      <c r="AE18">
+      <c r="AH18">
         <v>1.362412132</v>
       </c>
-      <c r="AF18">
+      <c r="AI18">
         <v>25470.01368</v>
       </c>
-      <c r="AG18">
+      <c r="AJ18">
         <v>23475.8786</v>
       </c>
-      <c r="AI18">
+      <c r="AL18">
         <v>733.33333330000005</v>
       </c>
-      <c r="AK18">
+      <c r="AN18">
         <v>2.5166114780000002</v>
       </c>
-      <c r="AL18">
+      <c r="AO18">
         <v>1.1547005379999999</v>
       </c>
-      <c r="AM18">
+      <c r="AP18">
         <v>0.348281495</v>
       </c>
-      <c r="AN18">
+      <c r="AQ18">
         <v>5.7518113089999998</v>
       </c>
-      <c r="AO18">
+      <c r="AR18">
         <v>0.28243780600000001</v>
       </c>
-      <c r="AP18">
+      <c r="AS18">
         <v>1.309851638</v>
       </c>
-      <c r="AQ18">
+      <c r="AT18">
         <v>14.148851540000001</v>
       </c>
-      <c r="AR18">
+      <c r="AU18">
         <v>10.21833809</v>
       </c>
-      <c r="AS18">
+      <c r="AV18">
         <v>18.289954439999999</v>
       </c>
-      <c r="AT18">
+      <c r="AW18">
         <v>12.678459419999999</v>
       </c>
-      <c r="AU18">
+      <c r="AX18">
         <v>15.767594409999999</v>
       </c>
-      <c r="AX18">
+      <c r="BA18">
         <v>415.57733739999998</v>
       </c>
-      <c r="AY18">
+      <c r="BB18">
         <v>0.40941188499999998</v>
       </c>
-      <c r="AZ18">
+      <c r="BC18">
         <v>0.40461825099999998</v>
       </c>
-      <c r="BA18">
+      <c r="BD18">
         <v>0.17834109300000001</v>
       </c>
-      <c r="BB18">
+      <c r="BE18">
         <v>0.17916147299999999</v>
       </c>
-      <c r="BE18">
+      <c r="BH18">
         <v>0.49556551900000001</v>
       </c>
-      <c r="BF18">
+      <c r="BI18">
         <v>0.21661079899999999</v>
       </c>
-      <c r="BG18">
+      <c r="BJ18">
         <v>0.53461416900000003</v>
       </c>
-      <c r="BH18">
+      <c r="BK18">
         <v>0.66098231100000004</v>
       </c>
-      <c r="BK18">
+      <c r="BN18">
         <v>0.43763847</v>
       </c>
-      <c r="BL18">
+      <c r="BO18">
         <v>0.18807691900000001</v>
       </c>
-      <c r="BM18">
+      <c r="BP18">
         <v>3456.5980880000002</v>
       </c>
-      <c r="BN18">
+      <c r="BQ18">
         <v>3152.3957850000002</v>
       </c>
-      <c r="BP18">
+      <c r="BS18">
         <v>106.5078506</v>
       </c>
     </row>
-    <row r="19" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>4</v>
       </c>
@@ -3688,170 +3832,173 @@
         <v>42997</v>
       </c>
       <c r="C19" s="4"/>
-      <c r="D19">
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19">
         <v>36.333333330000002</v>
       </c>
-      <c r="E19">
+      <c r="H19">
         <v>31</v>
       </c>
-      <c r="F19">
+      <c r="I19">
         <v>16.39</v>
       </c>
-      <c r="G19">
+      <c r="J19">
         <v>40</v>
       </c>
-      <c r="J19">
+      <c r="M19">
         <v>19.223333329999999</v>
       </c>
-      <c r="K19">
+      <c r="N19">
         <v>21.49</v>
       </c>
-      <c r="L19">
+      <c r="O19">
         <v>40.713333329999998</v>
       </c>
-      <c r="M19">
+      <c r="P19">
         <v>219.25</v>
       </c>
-      <c r="N19">
+      <c r="Q19">
         <v>387.29</v>
       </c>
-      <c r="O19">
+      <c r="R19">
         <v>108.9866667</v>
       </c>
-      <c r="P19">
+      <c r="S19">
         <v>278.30333330000002</v>
       </c>
-      <c r="Q19">
+      <c r="T19">
         <v>647.25333330000001</v>
       </c>
-      <c r="R19">
+      <c r="U19">
         <v>2.3521679240000002</v>
       </c>
-      <c r="S19">
+      <c r="V19">
         <v>1.6860892380000001</v>
       </c>
-      <c r="T19">
+      <c r="W19">
         <v>0.52212872099999996</v>
       </c>
-      <c r="U19">
+      <c r="X19">
         <v>4.5911583289999998</v>
       </c>
-      <c r="V19">
+      <c r="Y19">
         <v>0.93376227199999995</v>
       </c>
-      <c r="W19">
+      <c r="Z19">
         <v>6.0332436559999998</v>
       </c>
-      <c r="X19">
+      <c r="AA19">
         <v>0.43640024599999999</v>
       </c>
-      <c r="Y19">
+      <c r="AB19">
         <v>0.35975561299999997</v>
       </c>
-      <c r="Z19">
+      <c r="AC19">
         <v>1.14375928</v>
       </c>
-      <c r="AA19">
+      <c r="AD19">
         <v>17.7300304</v>
       </c>
-      <c r="AB19">
+      <c r="AE19">
         <v>1.0196174790000001</v>
       </c>
-      <c r="AC19">
+      <c r="AF19">
         <v>16.71041292</v>
       </c>
-      <c r="AD19">
+      <c r="AG19">
         <v>19.669945540000001</v>
       </c>
-      <c r="AI19">
+      <c r="AL19">
         <v>733.33333330000005</v>
       </c>
-      <c r="AJ19">
+      <c r="AM19">
         <v>47.663444439999999</v>
       </c>
-      <c r="AK19">
+      <c r="AN19">
         <v>2.5166114780000002</v>
       </c>
-      <c r="AL19">
+      <c r="AO19">
         <v>3.4641016150000001</v>
       </c>
-      <c r="AM19">
+      <c r="AP19">
         <v>0.348281495</v>
       </c>
-      <c r="AN19">
+      <c r="AQ19">
         <v>4.67</v>
       </c>
-      <c r="AQ19">
+      <c r="AT19">
         <v>15.94061898</v>
       </c>
-      <c r="AR19">
+      <c r="AU19">
         <v>10.5</v>
       </c>
-      <c r="AS19">
+      <c r="AV19">
         <v>25.78087146</v>
       </c>
-      <c r="AT19">
+      <c r="AW19">
         <v>11.883181390000001</v>
       </c>
-      <c r="AU19">
+      <c r="AX19">
         <v>53.30703518</v>
       </c>
-      <c r="AV19">
+      <c r="AY19">
         <v>11.006317879999999</v>
       </c>
-      <c r="AW19">
+      <c r="AZ19">
         <v>42.300721430000003</v>
       </c>
-      <c r="AX19">
+      <c r="BA19">
         <v>750.10421499999995</v>
       </c>
-      <c r="AY19">
+      <c r="BB19">
         <v>0.205624793</v>
       </c>
-      <c r="AZ19">
+      <c r="BC19">
         <v>8.6981791000000003E-2</v>
       </c>
-      <c r="BA19">
+      <c r="BD19">
         <v>6.4591645000000003E-2</v>
       </c>
-      <c r="BB19">
+      <c r="BE19">
         <v>0.247615847</v>
       </c>
-      <c r="BC19">
+      <c r="BF19">
         <v>0.16779386900000001</v>
       </c>
-      <c r="BD19">
+      <c r="BG19">
         <v>0.35224639200000002</v>
       </c>
-      <c r="BE19">
+      <c r="BH19">
         <v>0.33582984900000001</v>
       </c>
-      <c r="BF19">
+      <c r="BI19">
         <v>0.17449678199999999</v>
       </c>
-      <c r="BG19">
+      <c r="BJ19">
         <v>0.14542123200000001</v>
       </c>
-      <c r="BH19">
+      <c r="BK19">
         <v>2.0032270049999998</v>
       </c>
-      <c r="BI19">
+      <c r="BL19">
         <v>0.215670792</v>
       </c>
-      <c r="BJ19">
+      <c r="BM19">
         <v>1.8231119410000001</v>
       </c>
-      <c r="BK19">
+      <c r="BN19">
         <v>2.316815096</v>
       </c>
-      <c r="BP19">
+      <c r="BS19">
         <v>106.5078506</v>
       </c>
-      <c r="BQ19">
+      <c r="BT19">
         <v>7.2446063140000003</v>
       </c>
     </row>
-    <row r="20" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>4</v>
       </c>
@@ -3861,20 +4008,23 @@
       <c r="C20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="P20">
+      <c r="D20" s="4"/>
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="S20">
         <v>308.80134229999999</v>
       </c>
-      <c r="AJ20">
+      <c r="AM20">
         <v>52.886666669999997</v>
       </c>
-      <c r="AW20">
+      <c r="AZ20">
         <v>14.451823940000001</v>
       </c>
-      <c r="BQ20">
+      <c r="BT20">
         <v>2.4750824900000001</v>
       </c>
     </row>
-    <row r="21" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>4</v>
       </c>
@@ -3882,14 +4032,17 @@
         <v>42916</v>
       </c>
       <c r="C21" s="4"/>
-      <c r="AH21">
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="AK21">
         <v>818.88888889999998</v>
       </c>
-      <c r="BO21">
+      <c r="BR21">
         <v>10.18350154</v>
       </c>
     </row>
-    <row r="22" spans="1:69" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>4</v>
       </c>
@@ -3897,11 +4050,422 @@
         <v>42934</v>
       </c>
       <c r="C22" s="4"/>
-      <c r="AH22">
+      <c r="D22" s="4"/>
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="AK22">
         <v>971.66666669999995</v>
       </c>
-      <c r="BO22">
+      <c r="BR22">
         <v>99.068578939999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D23" s="5">
+        <v>6</v>
+      </c>
+      <c r="E23" s="5">
+        <v>21</v>
+      </c>
+      <c r="F23" s="5">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D24" s="5">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5">
+        <v>26</v>
+      </c>
+      <c r="F24" s="5">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="25" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="5">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5">
+        <v>30</v>
+      </c>
+      <c r="F25" s="5">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D26" s="5">
+        <v>6</v>
+      </c>
+      <c r="E26" s="5">
+        <v>33</v>
+      </c>
+      <c r="F26" s="5">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" s="5">
+        <v>6</v>
+      </c>
+      <c r="E27" s="5">
+        <v>37</v>
+      </c>
+      <c r="F27" s="5">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="28" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" s="5">
+        <v>6</v>
+      </c>
+      <c r="E28" s="5">
+        <v>40</v>
+      </c>
+      <c r="F28" s="5">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="29" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D29" s="5">
+        <v>6</v>
+      </c>
+      <c r="E29" s="5">
+        <v>67</v>
+      </c>
+      <c r="F29" s="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="5">
+        <v>6</v>
+      </c>
+      <c r="E30" s="5">
+        <v>72</v>
+      </c>
+      <c r="F30" s="5">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D31" s="5">
+        <v>13</v>
+      </c>
+      <c r="E31" s="5">
+        <v>40</v>
+      </c>
+      <c r="F31" s="5">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="32" spans="1:72" x14ac:dyDescent="0.55000000000000004">
+      <c r="A32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="5">
+        <v>13</v>
+      </c>
+      <c r="E32" s="5">
+        <v>43</v>
+      </c>
+      <c r="F32" s="5">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" t="s">
+        <v>92</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D33" s="5">
+        <v>13</v>
+      </c>
+      <c r="E33" s="5">
+        <v>43</v>
+      </c>
+      <c r="F33" s="5">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D34" s="5">
+        <v>13</v>
+      </c>
+      <c r="E34" s="5">
+        <v>44</v>
+      </c>
+      <c r="F34" s="5">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D35" s="5">
+        <v>13</v>
+      </c>
+      <c r="E35" s="5">
+        <v>48</v>
+      </c>
+      <c r="F35" s="5">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>95</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D36" s="5">
+        <v>13</v>
+      </c>
+      <c r="E36" s="5">
+        <v>53</v>
+      </c>
+      <c r="F36" s="5">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" s="5">
+        <v>13</v>
+      </c>
+      <c r="E37" s="5">
+        <v>71</v>
+      </c>
+      <c r="F37" s="5">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>97</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D38" s="5">
+        <v>13</v>
+      </c>
+      <c r="E38" s="5">
+        <v>73</v>
+      </c>
+      <c r="F38" s="5">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>98</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D39" s="5">
+        <v>7</v>
+      </c>
+      <c r="E39" s="5">
+        <v>34</v>
+      </c>
+      <c r="F39" s="5">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>99</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D40" s="5">
+        <v>7</v>
+      </c>
+      <c r="E40" s="5">
+        <v>35</v>
+      </c>
+      <c r="F40" s="5">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>100</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" s="5">
+        <v>7</v>
+      </c>
+      <c r="E41" s="5">
+        <v>38</v>
+      </c>
+      <c r="F41" s="5">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>101</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D42" s="5">
+        <v>7</v>
+      </c>
+      <c r="E42" s="5">
+        <v>40</v>
+      </c>
+      <c r="F42" s="5">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>102</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D43" s="5">
+        <v>7</v>
+      </c>
+      <c r="E43" s="5">
+        <v>41</v>
+      </c>
+      <c r="F43" s="5">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>103</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D44" s="5">
+        <v>7</v>
+      </c>
+      <c r="E44" s="5">
+        <v>49</v>
+      </c>
+      <c r="F44" s="5">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>104</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D45" s="5">
+        <v>7</v>
+      </c>
+      <c r="E45" s="5">
+        <v>60</v>
+      </c>
+      <c r="F45" s="5">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D46" s="5">
+        <v>7</v>
+      </c>
+      <c r="E46" s="5">
+        <v>62</v>
+      </c>
+      <c r="F46" s="5">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
work on phenology model
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CDDBE5-3B30-45A8-A569-D5908102FDFD}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{270F067E-F6B3-4ED6-8B5B-BD6578412767}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="112">
   <si>
     <t>SimulationName</t>
   </si>
@@ -278,70 +278,88 @@
     <t>Arkansas2001CvLambert_MG0</t>
   </si>
   <si>
-    <t>Arkansas2001CvIA1006_MG01</t>
-  </si>
-  <si>
-    <t>Arkansas2001CvIA2008_MG02</t>
-  </si>
-  <si>
-    <t>Arkansas2001CvMacon_MG03</t>
-  </si>
-  <si>
-    <t>Arkansas2001CvPioneer94B01_MG04</t>
-  </si>
-  <si>
-    <t>Arkansas2001CvHutcheson_MG05</t>
-  </si>
-  <si>
-    <t>Arkansas2001CvNK622_MG06</t>
-  </si>
-  <si>
     <t>Arkansas2002CvTrial_MG00</t>
   </si>
   <si>
     <t>Arkansas2002CvLambert_MG0</t>
   </si>
   <si>
-    <t>Arkansas2002CvIA1006_MG01</t>
-  </si>
-  <si>
-    <t>Arkansas2002CvIA2008_MG02</t>
-  </si>
-  <si>
-    <t>Arkansas2002CvMacon_MG03</t>
-  </si>
-  <si>
-    <t>Arkansas2002CvPioneer94B01_MG04</t>
-  </si>
-  <si>
-    <t>Arkansas2002CvHutcheson_MG05</t>
-  </si>
-  <si>
-    <t>Arkansas2002CvNK622_MG06</t>
-  </si>
-  <si>
     <t>Arkansas2003CvTrial_MG00</t>
   </si>
   <si>
     <t>Arkansas2003CvLambert_MG0</t>
   </si>
   <si>
-    <t>Arkansas2003CvIA1006_MG01</t>
-  </si>
-  <si>
-    <t>Arkansas2003CvIA2008_MG02</t>
-  </si>
-  <si>
-    <t>Arkansas2003CvMacon_MG03</t>
-  </si>
-  <si>
-    <t>Arkansas2003CvPioneer94B01_MG04</t>
-  </si>
-  <si>
-    <t>Arkansas2003CvHutcheson_MG05</t>
-  </si>
-  <si>
-    <t>Arkansas2003CvNK622_MG06</t>
+    <t>Indiana2006SowMar30</t>
+  </si>
+  <si>
+    <t>Indiana2006SowApr13</t>
+  </si>
+  <si>
+    <t>Indiana2006SowApr27</t>
+  </si>
+  <si>
+    <t>Indiana2006SowMay10</t>
+  </si>
+  <si>
+    <t>Indiana2006SowMay30</t>
+  </si>
+  <si>
+    <t>Indiana2006SowJun06</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvIA1006_MG10</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvIA2008_MG20</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvMacon_MG30</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvPioneer94B01_MG40</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvHutcheson_MG50</t>
+  </si>
+  <si>
+    <t>Arkansas2001CvNK622_MG60</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvIA1006_MG10</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvIA2008_MG20</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvMacon_MG30</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvPioneer94B01_MG40</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvHutcheson_MG50</t>
+  </si>
+  <si>
+    <t>Arkansas2002CvNK622_MG60</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvIA1006_MG10</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvIA2008_MG20</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvMacon_MG30</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvPioneer94B01_MG40</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvHutcheson_MG50</t>
+  </si>
+  <si>
+    <t>Arkansas2003CvNK622_MG60</t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1431,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
-  <dimension ref="A1:BT46"/>
+  <dimension ref="A1:BT54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23:C46"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -4096,7 +4114,7 @@
     </row>
     <row r="25" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>77</v>
@@ -4113,7 +4131,7 @@
     </row>
     <row r="26" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>77</v>
@@ -4130,7 +4148,7 @@
     </row>
     <row r="27" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>77</v>
@@ -4147,7 +4165,7 @@
     </row>
     <row r="28" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>77</v>
@@ -4164,7 +4182,7 @@
     </row>
     <row r="29" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>77</v>
@@ -4181,7 +4199,7 @@
     </row>
     <row r="30" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>77</v>
@@ -4198,7 +4216,7 @@
     </row>
     <row r="31" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>77</v>
@@ -4215,7 +4233,7 @@
     </row>
     <row r="32" spans="1:72" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>77</v>
@@ -4230,9 +4248,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>77</v>
@@ -4247,9 +4265,9 @@
         <v>91</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>77</v>
@@ -4264,9 +4282,9 @@
         <v>103</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>77</v>
@@ -4281,9 +4299,9 @@
         <v>112</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>77</v>
@@ -4298,9 +4316,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>77</v>
@@ -4315,9 +4333,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>77</v>
@@ -4332,9 +4350,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>77</v>
@@ -4349,9 +4367,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>77</v>
@@ -4366,9 +4384,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>77</v>
@@ -4383,9 +4401,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>77</v>
@@ -4400,9 +4418,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>77</v>
@@ -4417,9 +4435,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>77</v>
@@ -4434,9 +4452,9 @@
         <v>116</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>77</v>
@@ -4451,9 +4469,9 @@
         <v>140</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>77</v>
@@ -4467,6 +4485,150 @@
       <c r="F46" s="5">
         <v>140</v>
       </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D47" s="5">
+        <v>22</v>
+      </c>
+      <c r="E47" s="5">
+        <v>84</v>
+      </c>
+      <c r="F47" s="5">
+        <v>167</v>
+      </c>
+      <c r="S47" s="5">
+        <v>430</v>
+      </c>
+      <c r="T47" s="5"/>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D48" s="5">
+        <v>20</v>
+      </c>
+      <c r="E48" s="5">
+        <v>71</v>
+      </c>
+      <c r="F48" s="5">
+        <v>159</v>
+      </c>
+      <c r="S48" s="5">
+        <v>410</v>
+      </c>
+      <c r="T48" s="5"/>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>90</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="5">
+        <v>14</v>
+      </c>
+      <c r="E49" s="5">
+        <v>64</v>
+      </c>
+      <c r="F49" s="5">
+        <v>148</v>
+      </c>
+      <c r="S49" s="5">
+        <v>400</v>
+      </c>
+      <c r="T49" s="5"/>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>91</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D50" s="5">
+        <v>16</v>
+      </c>
+      <c r="E50" s="5">
+        <v>55</v>
+      </c>
+      <c r="F50" s="5">
+        <v>139</v>
+      </c>
+      <c r="S50" s="5">
+        <v>410</v>
+      </c>
+      <c r="T50" s="5"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>92</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D51" s="5">
+        <v>11</v>
+      </c>
+      <c r="E51" s="5">
+        <v>44</v>
+      </c>
+      <c r="F51" s="5">
+        <v>125</v>
+      </c>
+      <c r="S51" s="5">
+        <v>320</v>
+      </c>
+      <c r="T51" s="5"/>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>93</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D52" s="5">
+        <v>16</v>
+      </c>
+      <c r="E52" s="5">
+        <v>43</v>
+      </c>
+      <c r="F52" s="5">
+        <v>118</v>
+      </c>
+      <c r="S52" s="5">
+        <v>300</v>
+      </c>
+      <c r="T52" s="5"/>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5"/>
+      <c r="S53" s="5">
+        <v>440</v>
+      </c>
+      <c r="T53" s="5"/>
+    </row>
+    <row r="54" spans="1:20" x14ac:dyDescent="0.55000000000000004">
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5"/>
+      <c r="S54" s="5">
+        <v>440</v>
+      </c>
+      <c r="T54" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
working on plant nitrogen
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F329E3-B3CE-42F3-B1A5-9C82E191CF4E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A506F8-F5B9-47D3-A647-5471CB225495}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedOLD" sheetId="13" r:id="rId1"/>
@@ -78,48 +78,6 @@
   </si>
   <si>
     <t>plants-small</t>
-  </si>
-  <si>
-    <t>PodGreenWt</t>
-  </si>
-  <si>
-    <t>LeafGreennconc</t>
-  </si>
-  <si>
-    <t>LeafSenescednconc</t>
-  </si>
-  <si>
-    <t>StemGreennconc</t>
-  </si>
-  <si>
-    <t>FruitTotalnconc</t>
-  </si>
-  <si>
-    <t>PodGreennconc</t>
-  </si>
-  <si>
-    <t>GrainGrainnconc</t>
-  </si>
-  <si>
-    <t>leafGreenN</t>
-  </si>
-  <si>
-    <t>leafSenescedN</t>
-  </si>
-  <si>
-    <t>StemTotalN</t>
-  </si>
-  <si>
-    <t>FruitGreenN</t>
-  </si>
-  <si>
-    <t>PodGreenN</t>
-  </si>
-  <si>
-    <t>grain_n</t>
-  </si>
-  <si>
-    <t>green_biomass_n</t>
   </si>
   <si>
     <t>SLN_apsim</t>
@@ -559,6 +517,48 @@
   <si>
     <t>Indiana2007SowJun07CvPioneer92MGI_MG26</t>
   </si>
+  <si>
+    <t>Soybean.Leaf.Live.N</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.Dead.N</t>
+  </si>
+  <si>
+    <t>Soybean.Pod.N</t>
+  </si>
+  <si>
+    <t>Soybean.Stem.N</t>
+  </si>
+  <si>
+    <t>Soybean.Pod.Nconc</t>
+  </si>
+  <si>
+    <t>Soybean.Stem.NConc</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.Dead.NConc</t>
+  </si>
+  <si>
+    <t>Soybean.Leaf.Live.NConc</t>
+  </si>
+  <si>
+    <t>Soybean.Shell.NConc</t>
+  </si>
+  <si>
+    <t>Soybean.Grain.N</t>
+  </si>
+  <si>
+    <t>Soybean.Shell.Wt</t>
+  </si>
+  <si>
+    <t>Soybean.Grain.NConc</t>
+  </si>
+  <si>
+    <t>Soybean.Shell.N</t>
+  </si>
+  <si>
+    <t>Soybean.AboveGround.N</t>
+  </si>
 </sst>
 </file>
 
@@ -1659,9 +1659,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
   <dimension ref="A1:BV114"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A96" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
+    <sheetView topLeftCell="Z1" workbookViewId="0">
+      <pane ySplit="576" topLeftCell="A19" activePane="bottomLeft"/>
+      <selection activeCell="W1" sqref="W1:W1048576"/>
+      <selection pane="bottomLeft" activeCell="AN23" sqref="AN23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1683,6 +1684,9 @@
     <col min="20" max="20" width="11.68359375" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.05078125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="21.83984375" customWidth="1"/>
+    <col min="23" max="23" width="20.3671875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.41796875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="17.5234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:74" x14ac:dyDescent="0.55000000000000004">
@@ -1696,13 +1700,13 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="F1" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -1711,202 +1715,202 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="J1" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="K1" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="L1" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="M1" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="N1" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="O1" t="s">
         <v>12</v>
       </c>
       <c r="P1" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="Q1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="R1" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="S1" t="s">
         <v>6</v>
       </c>
       <c r="T1" t="s">
-        <v>17</v>
+        <v>173</v>
       </c>
       <c r="U1" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="V1" t="s">
         <v>7</v>
       </c>
       <c r="W1" t="s">
+        <v>170</v>
+      </c>
+      <c r="X1" t="s">
+        <v>169</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>171</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>175</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>172</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AK1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AL1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AM1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AN1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AO1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AP1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AQ1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AR1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AS1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AT1" t="s">
         <v>27</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AU1" t="s">
         <v>28</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AV1" t="s">
         <v>29</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AW1" t="s">
         <v>30</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AX1" t="s">
         <v>31</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AY1" t="s">
         <v>32</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AZ1" t="s">
         <v>33</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="BA1" t="s">
         <v>34</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="BB1" t="s">
         <v>35</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="BC1" t="s">
         <v>36</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="BD1" t="s">
         <v>37</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="BE1" t="s">
         <v>38</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="BF1" t="s">
         <v>39</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="BG1" t="s">
         <v>40</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="BH1" t="s">
         <v>41</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="BI1" t="s">
         <v>42</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="BJ1" t="s">
         <v>43</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="BK1" t="s">
         <v>44</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BL1" t="s">
         <v>45</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="BM1" t="s">
         <v>46</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BN1" t="s">
         <v>47</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BO1" t="s">
         <v>48</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BP1" t="s">
         <v>49</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BQ1" t="s">
         <v>50</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BR1" t="s">
         <v>51</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BS1" t="s">
         <v>52</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BT1" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BU1" t="s">
         <v>54</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BV1" t="s">
         <v>55</v>
-      </c>
-      <c r="BI1" t="s">
-        <v>56</v>
-      </c>
-      <c r="BJ1" t="s">
-        <v>57</v>
-      </c>
-      <c r="BK1" t="s">
-        <v>58</v>
-      </c>
-      <c r="BL1" t="s">
-        <v>59</v>
-      </c>
-      <c r="BM1" t="s">
-        <v>60</v>
-      </c>
-      <c r="BN1" t="s">
-        <v>61</v>
-      </c>
-      <c r="BO1" t="s">
-        <v>62</v>
-      </c>
-      <c r="BP1" t="s">
-        <v>63</v>
-      </c>
-      <c r="BQ1" t="s">
-        <v>64</v>
-      </c>
-      <c r="BR1" t="s">
-        <v>65</v>
-      </c>
-      <c r="BS1" t="s">
-        <v>66</v>
-      </c>
-      <c r="BT1" t="s">
-        <v>67</v>
-      </c>
-      <c r="BU1" t="s">
-        <v>68</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:74" x14ac:dyDescent="0.55000000000000004">
@@ -1952,10 +1956,10 @@
         <v>12.3</v>
       </c>
       <c r="W2">
-        <v>4.6311446829999996</v>
+        <v>4.6311446829999998E-2</v>
       </c>
       <c r="Y2">
-        <v>2.0514227950000001</v>
+        <v>2.0514227950000002E-2</v>
       </c>
       <c r="AC2">
         <v>0.34375607200000002</v>
@@ -2079,10 +2083,10 @@
         <v>50.3</v>
       </c>
       <c r="W3">
-        <v>5.0692481989999996</v>
+        <v>5.0692481989999996E-2</v>
       </c>
       <c r="Y3">
-        <v>1.8245937029999999</v>
+        <v>1.8245937029999999E-2</v>
       </c>
       <c r="AC3">
         <v>1.476158393</v>
@@ -2209,10 +2213,10 @@
         <v>180.85</v>
       </c>
       <c r="W4">
-        <v>5.2969261809999999</v>
+        <v>5.2969261810000001E-2</v>
       </c>
       <c r="Y4">
-        <v>1.830695073</v>
+        <v>1.830695073E-2</v>
       </c>
       <c r="AC4">
         <v>4.8199299030000002</v>
@@ -2352,16 +2356,16 @@
         <v>374.8</v>
       </c>
       <c r="W5">
-        <v>5.2664065359999999</v>
+        <v>5.2664065359999998E-2</v>
       </c>
       <c r="X5">
-        <v>2.4026684359999999</v>
+        <v>2.4026684359999998E-2</v>
       </c>
       <c r="Y5">
-        <v>1.5933583579999999</v>
+        <v>1.5933583580000001E-2</v>
       </c>
       <c r="Z5">
-        <v>3.462394953</v>
+        <v>3.4623949530000003E-2</v>
       </c>
       <c r="AC5">
         <v>7.4919406620000002</v>
@@ -2528,16 +2532,16 @@
         <v>523.70000000000005</v>
       </c>
       <c r="W6">
-        <v>4.9020051960000002</v>
+        <v>4.9020051960000005E-2</v>
       </c>
       <c r="X6">
-        <v>2.7312035560000001</v>
+        <v>2.731203556E-2</v>
       </c>
       <c r="Y6">
-        <v>1.4922018850000001</v>
+        <v>1.4922018850000001E-2</v>
       </c>
       <c r="Z6">
-        <v>3.4</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="AC6">
         <v>8.395316459</v>
@@ -2701,16 +2705,16 @@
         <v>722.85333330000003</v>
       </c>
       <c r="W7">
-        <v>4.5780029300000002</v>
+        <v>4.5780029300000004E-2</v>
       </c>
       <c r="X7">
-        <v>2.434477131</v>
+        <v>2.4344771309999999E-2</v>
       </c>
       <c r="Y7">
-        <v>1.360071177</v>
+        <v>1.3600711770000001E-2</v>
       </c>
       <c r="Z7">
-        <v>3.3245203499999998</v>
+        <v>3.3245203500000001E-2</v>
       </c>
       <c r="AC7">
         <v>8.3967630989999993</v>
@@ -2871,16 +2875,16 @@
         <v>898.0133333</v>
       </c>
       <c r="W8">
-        <v>2.7464925450000002</v>
+        <v>2.746492545E-2</v>
       </c>
       <c r="X8">
-        <v>1.897563656</v>
+        <v>1.8975636559999998E-2</v>
       </c>
       <c r="Y8">
-        <v>0.81153414599999996</v>
+        <v>8.1153414599999998E-3</v>
       </c>
       <c r="Z8">
-        <v>3.87950778</v>
+        <v>3.8795077800000001E-2</v>
       </c>
       <c r="AC8">
         <v>4.4259175710000003</v>
@@ -3037,22 +3041,22 @@
         <v>688.29333329999997</v>
       </c>
       <c r="W9">
-        <v>2.2859224079999998</v>
+        <v>2.2859224079999997E-2</v>
       </c>
       <c r="X9">
-        <v>1.7393941879999999</v>
+        <v>1.739394188E-2</v>
       </c>
       <c r="Y9">
-        <v>0.490818898</v>
+        <v>4.9081889800000004E-3</v>
       </c>
       <c r="Z9">
-        <v>4.4114886699999998</v>
+        <v>4.4114886699999994E-2</v>
       </c>
       <c r="AA9">
-        <v>0.79016911999999995</v>
+        <v>7.9016911999999998E-3</v>
       </c>
       <c r="AB9">
-        <v>5.8392753600000002</v>
+        <v>5.3927535999999998E-2</v>
       </c>
       <c r="AC9">
         <v>0.36035655300000002</v>
@@ -3171,7 +3175,7 @@
         <v>43026</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -3268,10 +3272,10 @@
         <v>29.533333329999998</v>
       </c>
       <c r="W13">
-        <v>5.3513595260000004</v>
+        <v>5.3513595260000005E-2</v>
       </c>
       <c r="Y13">
-        <v>2.557780186</v>
+        <v>2.5577801859999999E-2</v>
       </c>
       <c r="AC13">
         <v>0.92831271999999998</v>
@@ -3398,10 +3402,10 @@
         <v>108.02666670000001</v>
       </c>
       <c r="W14">
-        <v>5.5619044300000002</v>
+        <v>5.5619044300000003E-2</v>
       </c>
       <c r="Y14">
-        <v>2.2197982469999999</v>
+        <v>2.2197982469999999E-2</v>
       </c>
       <c r="AC14">
         <v>3.3607650140000001</v>
@@ -3534,16 +3538,16 @@
         <v>247.96666669999999</v>
       </c>
       <c r="W15">
-        <v>5.6759546600000004</v>
+        <v>5.6759546600000002E-2</v>
       </c>
       <c r="X15">
-        <v>2.2230339849999998</v>
+        <v>2.2230339849999999E-2</v>
       </c>
       <c r="Y15">
-        <v>1.49628977</v>
+        <v>1.49628977E-2</v>
       </c>
       <c r="Z15">
-        <v>3.4290581539999998</v>
+        <v>3.4290581539999997E-2</v>
       </c>
       <c r="AC15">
         <v>6.0370028959999997</v>
@@ -3707,16 +3711,16 @@
         <v>446.53333329999998</v>
       </c>
       <c r="W16">
-        <v>4.7166145640000003</v>
+        <v>4.7166145640000004E-2</v>
       </c>
       <c r="X16">
-        <v>2.4504482350000001</v>
+        <v>2.4504482350000002E-2</v>
       </c>
       <c r="Y16">
-        <v>1.330648343</v>
+        <v>1.330648343E-2</v>
       </c>
       <c r="Z16">
-        <v>3.5</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AC16">
         <v>7.7601181229999998</v>
@@ -3880,16 +3884,16 @@
         <v>626.28666670000007</v>
       </c>
       <c r="W17">
-        <v>4.7927247680000002</v>
+        <v>4.792724768E-2</v>
       </c>
       <c r="X17">
-        <v>2.4406307140000001</v>
+        <v>2.440630714E-2</v>
       </c>
       <c r="Y17">
-        <v>1.375053326</v>
+        <v>1.375053326E-2</v>
       </c>
       <c r="Z17">
-        <v>3.5871027309999999</v>
+        <v>3.5871027309999998E-2</v>
       </c>
       <c r="AC17">
         <v>8.4749179560000005</v>
@@ -4050,16 +4054,16 @@
         <v>804.05666670000005</v>
       </c>
       <c r="W18">
-        <v>3.4432400859999999</v>
+        <v>3.4432400859999997E-2</v>
       </c>
       <c r="X18">
-        <v>1.938536008</v>
+        <v>1.938536008E-2</v>
       </c>
       <c r="Y18">
-        <v>0.93853016700000003</v>
+        <v>9.3853016700000003E-3</v>
       </c>
       <c r="Z18">
-        <v>3.5966654619999998</v>
+        <v>3.5966654619999996E-2</v>
       </c>
       <c r="AC18">
         <v>5.9953915029999996</v>
@@ -4216,22 +4220,22 @@
         <v>647.25333330000001</v>
       </c>
       <c r="W19">
-        <v>2.3521679240000002</v>
+        <v>2.3521679240000003E-2</v>
       </c>
       <c r="X19">
-        <v>1.6860892380000001</v>
+        <v>1.6860892380000003E-2</v>
       </c>
       <c r="Y19">
-        <v>0.52212872099999996</v>
+        <v>5.2212872099999998E-3</v>
       </c>
       <c r="Z19">
-        <v>4.5911583289999998</v>
+        <v>4.5911583289999995E-2</v>
       </c>
       <c r="AA19">
-        <v>0.93376227199999995</v>
+        <v>9.3376227199999991E-3</v>
       </c>
       <c r="AB19">
-        <v>6.0332436559999998</v>
+        <v>6.0332436560000001E-2</v>
       </c>
       <c r="AC19">
         <v>0.43640024599999999</v>
@@ -4350,7 +4354,7 @@
         <v>43026</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -4406,7 +4410,7 @@
     </row>
     <row r="23" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B23" s="4">
         <v>42898</v>
@@ -4445,30 +4449,6 @@
       <c r="V23">
         <v>14.855333330000001</v>
       </c>
-      <c r="AC23">
-        <v>0</v>
-      </c>
-      <c r="AD23">
-        <v>0</v>
-      </c>
-      <c r="AE23">
-        <v>0</v>
-      </c>
-      <c r="AF23">
-        <v>0</v>
-      </c>
-      <c r="AG23">
-        <v>0</v>
-      </c>
-      <c r="AH23">
-        <v>0</v>
-      </c>
-      <c r="AI23">
-        <v>0</v>
-      </c>
-      <c r="AJ23">
-        <v>0</v>
-      </c>
       <c r="AK23">
         <v>38030.98921</v>
       </c>
@@ -4547,7 +4527,7 @@
     </row>
     <row r="24" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B24" s="4">
         <v>42915</v>
@@ -4586,30 +4566,6 @@
       <c r="V24">
         <v>73.633333329999999</v>
       </c>
-      <c r="AC24">
-        <v>0</v>
-      </c>
-      <c r="AD24">
-        <v>0</v>
-      </c>
-      <c r="AE24">
-        <v>0</v>
-      </c>
-      <c r="AF24">
-        <v>0</v>
-      </c>
-      <c r="AG24">
-        <v>0</v>
-      </c>
-      <c r="AH24">
-        <v>0</v>
-      </c>
-      <c r="AI24">
-        <v>0</v>
-      </c>
-      <c r="AJ24">
-        <v>0</v>
-      </c>
       <c r="AK24">
         <v>22159.869739999998</v>
       </c>
@@ -4688,7 +4644,7 @@
     </row>
     <row r="25" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B25" s="4">
         <v>42929</v>
@@ -4727,30 +4683,6 @@
       <c r="V25">
         <v>148.93333329999999</v>
       </c>
-      <c r="AC25">
-        <v>0</v>
-      </c>
-      <c r="AD25">
-        <v>0</v>
-      </c>
-      <c r="AE25">
-        <v>0</v>
-      </c>
-      <c r="AF25">
-        <v>0</v>
-      </c>
-      <c r="AG25">
-        <v>0</v>
-      </c>
-      <c r="AH25">
-        <v>0</v>
-      </c>
-      <c r="AI25">
-        <v>0</v>
-      </c>
-      <c r="AJ25">
-        <v>0</v>
-      </c>
       <c r="AK25">
         <v>23266.329870000001</v>
       </c>
@@ -4832,7 +4764,7 @@
     </row>
     <row r="26" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B26" s="4">
         <v>42943</v>
@@ -4877,30 +4809,6 @@
       <c r="V26">
         <v>308.06666669999998</v>
       </c>
-      <c r="AC26">
-        <v>0</v>
-      </c>
-      <c r="AD26">
-        <v>0</v>
-      </c>
-      <c r="AE26">
-        <v>0</v>
-      </c>
-      <c r="AF26">
-        <v>0</v>
-      </c>
-      <c r="AG26">
-        <v>0</v>
-      </c>
-      <c r="AH26">
-        <v>0</v>
-      </c>
-      <c r="AI26">
-        <v>0</v>
-      </c>
-      <c r="AJ26">
-        <v>0</v>
-      </c>
       <c r="AK26">
         <v>28154.005659999999</v>
       </c>
@@ -4988,7 +4896,7 @@
     </row>
     <row r="27" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B27" s="4">
         <v>42957</v>
@@ -5036,30 +4944,6 @@
       <c r="V27">
         <v>508.78</v>
       </c>
-      <c r="AC27">
-        <v>0</v>
-      </c>
-      <c r="AD27">
-        <v>0</v>
-      </c>
-      <c r="AE27">
-        <v>0</v>
-      </c>
-      <c r="AF27">
-        <v>0</v>
-      </c>
-      <c r="AG27">
-        <v>0</v>
-      </c>
-      <c r="AH27">
-        <v>0</v>
-      </c>
-      <c r="AI27">
-        <v>0</v>
-      </c>
-      <c r="AJ27">
-        <v>0</v>
-      </c>
       <c r="AK27">
         <v>27123.857769999999</v>
       </c>
@@ -5150,7 +5034,7 @@
     </row>
     <row r="28" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B28" s="4">
         <v>42975</v>
@@ -5198,30 +5082,6 @@
       <c r="V28">
         <v>696.32333329999994</v>
       </c>
-      <c r="AC28">
-        <v>0</v>
-      </c>
-      <c r="AD28">
-        <v>0</v>
-      </c>
-      <c r="AE28">
-        <v>0</v>
-      </c>
-      <c r="AF28">
-        <v>0</v>
-      </c>
-      <c r="AG28">
-        <v>0</v>
-      </c>
-      <c r="AH28">
-        <v>0</v>
-      </c>
-      <c r="AI28">
-        <v>0</v>
-      </c>
-      <c r="AJ28">
-        <v>0</v>
-      </c>
       <c r="AK28">
         <v>24539.78052</v>
       </c>
@@ -5306,7 +5166,7 @@
     </row>
     <row r="29" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B29" s="4">
         <v>42993</v>
@@ -5350,27 +5210,6 @@
       <c r="V29">
         <v>752.1</v>
       </c>
-      <c r="AC29">
-        <v>0</v>
-      </c>
-      <c r="AD29">
-        <v>0</v>
-      </c>
-      <c r="AE29">
-        <v>0</v>
-      </c>
-      <c r="AF29">
-        <v>0</v>
-      </c>
-      <c r="AG29">
-        <v>0</v>
-      </c>
-      <c r="AH29">
-        <v>0</v>
-      </c>
-      <c r="AI29">
-        <v>0</v>
-      </c>
       <c r="AO29">
         <v>57.915900379999997</v>
       </c>
@@ -5437,7 +5276,7 @@
     </row>
     <row r="30" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B30" s="4">
         <v>43028</v>
@@ -5448,27 +5287,6 @@
       <c r="U30">
         <v>378.40134230000001</v>
       </c>
-      <c r="AC30">
-        <v>0</v>
-      </c>
-      <c r="AD30">
-        <v>0</v>
-      </c>
-      <c r="AE30">
-        <v>0</v>
-      </c>
-      <c r="AF30">
-        <v>0</v>
-      </c>
-      <c r="AG30">
-        <v>0</v>
-      </c>
-      <c r="AH30">
-        <v>0</v>
-      </c>
-      <c r="AI30">
-        <v>0</v>
-      </c>
       <c r="AO30">
         <v>64.806666669999998</v>
       </c>
@@ -5502,7 +5320,7 @@
     </row>
     <row r="31" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B31" s="4">
         <v>42898</v>
@@ -5516,27 +5334,6 @@
       <c r="H31">
         <v>25.666666670000001</v>
       </c>
-      <c r="AC31">
-        <v>0</v>
-      </c>
-      <c r="AD31">
-        <v>0</v>
-      </c>
-      <c r="AE31">
-        <v>0</v>
-      </c>
-      <c r="AF31">
-        <v>0</v>
-      </c>
-      <c r="AG31">
-        <v>0</v>
-      </c>
-      <c r="AH31">
-        <v>0</v>
-      </c>
-      <c r="AI31">
-        <v>0</v>
-      </c>
       <c r="AM31">
         <v>220.1333333</v>
       </c>
@@ -5576,7 +5373,7 @@
     </row>
     <row r="32" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B32" s="4">
         <v>42915</v>
@@ -5615,30 +5412,6 @@
       <c r="V32">
         <v>28.366666670000001</v>
       </c>
-      <c r="AC32">
-        <v>0</v>
-      </c>
-      <c r="AD32">
-        <v>0</v>
-      </c>
-      <c r="AE32">
-        <v>0</v>
-      </c>
-      <c r="AF32">
-        <v>0</v>
-      </c>
-      <c r="AG32">
-        <v>0</v>
-      </c>
-      <c r="AH32">
-        <v>0</v>
-      </c>
-      <c r="AI32">
-        <v>0</v>
-      </c>
-      <c r="AJ32">
-        <v>0</v>
-      </c>
       <c r="AK32">
         <v>18761.898669999999</v>
       </c>
@@ -5717,7 +5490,7 @@
     </row>
     <row r="33" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B33" s="4">
         <v>42929</v>
@@ -5756,30 +5529,6 @@
       <c r="V33">
         <v>75.483333329999994</v>
       </c>
-      <c r="AC33">
-        <v>0</v>
-      </c>
-      <c r="AD33">
-        <v>0</v>
-      </c>
-      <c r="AE33">
-        <v>0</v>
-      </c>
-      <c r="AF33">
-        <v>0</v>
-      </c>
-      <c r="AG33">
-        <v>0</v>
-      </c>
-      <c r="AH33">
-        <v>0</v>
-      </c>
-      <c r="AI33">
-        <v>0</v>
-      </c>
-      <c r="AJ33">
-        <v>0</v>
-      </c>
       <c r="AK33">
         <v>22983.122050000002</v>
       </c>
@@ -5861,7 +5610,7 @@
     </row>
     <row r="34" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B34" s="4">
         <v>42943</v>
@@ -5906,30 +5655,6 @@
       <c r="V34">
         <v>235.8</v>
       </c>
-      <c r="AC34">
-        <v>0</v>
-      </c>
-      <c r="AD34">
-        <v>0</v>
-      </c>
-      <c r="AE34">
-        <v>0</v>
-      </c>
-      <c r="AF34">
-        <v>0</v>
-      </c>
-      <c r="AG34">
-        <v>0</v>
-      </c>
-      <c r="AH34">
-        <v>0</v>
-      </c>
-      <c r="AI34">
-        <v>0</v>
-      </c>
-      <c r="AJ34">
-        <v>0</v>
-      </c>
       <c r="AK34">
         <v>33565.220029999997</v>
       </c>
@@ -6017,7 +5742,7 @@
     </row>
     <row r="35" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B35" s="4">
         <v>42957</v>
@@ -6065,30 +5790,6 @@
       <c r="V35">
         <v>391.19666669999998</v>
       </c>
-      <c r="AC35">
-        <v>0</v>
-      </c>
-      <c r="AD35">
-        <v>0</v>
-      </c>
-      <c r="AE35">
-        <v>0</v>
-      </c>
-      <c r="AF35">
-        <v>0</v>
-      </c>
-      <c r="AG35">
-        <v>0</v>
-      </c>
-      <c r="AH35">
-        <v>0</v>
-      </c>
-      <c r="AI35">
-        <v>0</v>
-      </c>
-      <c r="AJ35">
-        <v>0</v>
-      </c>
       <c r="AK35">
         <v>27930.12355</v>
       </c>
@@ -6179,7 +5880,7 @@
     </row>
     <row r="36" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B36" s="4">
         <v>42975</v>
@@ -6227,30 +5928,6 @@
       <c r="V36">
         <v>642.03333299999997</v>
       </c>
-      <c r="AC36">
-        <v>0</v>
-      </c>
-      <c r="AD36">
-        <v>0</v>
-      </c>
-      <c r="AE36">
-        <v>0</v>
-      </c>
-      <c r="AF36">
-        <v>0</v>
-      </c>
-      <c r="AG36">
-        <v>0</v>
-      </c>
-      <c r="AH36">
-        <v>0</v>
-      </c>
-      <c r="AI36">
-        <v>0</v>
-      </c>
-      <c r="AJ36">
-        <v>0</v>
-      </c>
       <c r="AK36">
         <v>26258.566169999998</v>
       </c>
@@ -6332,7 +6009,7 @@
     </row>
     <row r="37" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B37" s="4">
         <v>42993</v>
@@ -6376,27 +6053,6 @@
       <c r="V37">
         <v>740.49</v>
       </c>
-      <c r="AC37">
-        <v>0</v>
-      </c>
-      <c r="AD37">
-        <v>0</v>
-      </c>
-      <c r="AE37">
-        <v>0</v>
-      </c>
-      <c r="AF37">
-        <v>0</v>
-      </c>
-      <c r="AG37">
-        <v>0</v>
-      </c>
-      <c r="AH37">
-        <v>0</v>
-      </c>
-      <c r="AI37">
-        <v>0</v>
-      </c>
       <c r="AO37">
         <v>48.302260539999999</v>
       </c>
@@ -6463,7 +6119,7 @@
     </row>
     <row r="38" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B38" s="4">
         <v>43028</v>
@@ -6474,27 +6130,6 @@
       <c r="U38">
         <v>337.5872483</v>
       </c>
-      <c r="AC38">
-        <v>0</v>
-      </c>
-      <c r="AD38">
-        <v>0</v>
-      </c>
-      <c r="AE38">
-        <v>0</v>
-      </c>
-      <c r="AF38">
-        <v>0</v>
-      </c>
-      <c r="AG38">
-        <v>0</v>
-      </c>
-      <c r="AH38">
-        <v>0</v>
-      </c>
-      <c r="AI38">
-        <v>0</v>
-      </c>
       <c r="AO38">
         <v>57.816666669999996</v>
       </c>
@@ -6528,10 +6163,10 @@
     </row>
     <row r="39" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D39" s="5">
         <v>6</v>
@@ -6545,10 +6180,10 @@
     </row>
     <row r="40" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D40" s="5">
         <v>6</v>
@@ -6562,10 +6197,10 @@
     </row>
     <row r="41" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D41" s="5">
         <v>6</v>
@@ -6579,10 +6214,10 @@
     </row>
     <row r="42" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D42" s="5">
         <v>6</v>
@@ -6596,10 +6231,10 @@
     </row>
     <row r="43" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D43" s="5">
         <v>6</v>
@@ -6613,10 +6248,10 @@
     </row>
     <row r="44" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D44" s="5">
         <v>6</v>
@@ -6630,10 +6265,10 @@
     </row>
     <row r="45" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D45" s="5">
         <v>6</v>
@@ -6647,10 +6282,10 @@
     </row>
     <row r="46" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D46" s="5">
         <v>6</v>
@@ -6664,10 +6299,10 @@
     </row>
     <row r="47" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D47" s="5">
         <v>13</v>
@@ -6681,10 +6316,10 @@
     </row>
     <row r="48" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D48" s="5">
         <v>13</v>
@@ -6698,10 +6333,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D49" s="5">
         <v>13</v>
@@ -6715,10 +6350,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D50" s="5">
         <v>13</v>
@@ -6732,10 +6367,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D51" s="5">
         <v>13</v>
@@ -6749,10 +6384,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D52" s="5">
         <v>13</v>
@@ -6766,10 +6401,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D53" s="5">
         <v>13</v>
@@ -6783,10 +6418,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D54" s="5">
         <v>13</v>
@@ -6800,10 +6435,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D55" s="5">
         <v>7</v>
@@ -6817,10 +6452,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D56" s="5">
         <v>7</v>
@@ -6834,10 +6469,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D57" s="5">
         <v>7</v>
@@ -6851,10 +6486,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D58" s="5">
         <v>7</v>
@@ -6868,10 +6503,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D59" s="5">
         <v>7</v>
@@ -6885,10 +6520,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D60" s="5">
         <v>7</v>
@@ -6902,10 +6537,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D61" s="5">
         <v>7</v>
@@ -6919,10 +6554,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D62" s="5">
         <v>7</v>
@@ -6936,10 +6571,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5">
@@ -6949,10 +6584,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5">
@@ -6962,10 +6597,10 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E65" s="5">
         <v>52</v>
@@ -6973,10 +6608,10 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E66" s="5">
         <v>52</v>
@@ -6984,10 +6619,10 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E67" s="5">
         <v>42</v>
@@ -6995,10 +6630,10 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E68" s="5">
         <v>42</v>
@@ -7006,10 +6641,10 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E69" s="5">
         <v>56</v>
@@ -7017,10 +6652,10 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E70" s="5">
         <v>55</v>
@@ -7028,10 +6663,10 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E71" s="5">
         <v>39</v>
@@ -7039,10 +6674,10 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E72" s="5">
         <v>40</v>
@@ -7050,10 +6685,10 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E73" s="5">
         <v>58</v>
@@ -7061,10 +6696,10 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E74" s="5">
         <v>60</v>
@@ -7072,10 +6707,10 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E75" s="5">
         <v>38</v>
@@ -7083,10 +6718,10 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E76" s="5">
         <v>41</v>
@@ -7094,10 +6729,10 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E77" s="5">
         <v>55</v>
@@ -7105,10 +6740,10 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="E78" s="5">
         <v>58</v>
@@ -7116,10 +6751,10 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="6" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D79" s="5">
         <v>22</v>
@@ -7136,10 +6771,10 @@
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="6" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D80" s="5">
         <v>20</v>
@@ -7156,10 +6791,10 @@
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="6" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D81" s="5">
         <v>14</v>
@@ -7176,10 +6811,10 @@
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="7" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D82" s="5">
         <v>16</v>
@@ -7196,10 +6831,10 @@
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="7" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D83" s="5">
         <v>11</v>
@@ -7216,10 +6851,10 @@
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="7" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D84" s="5">
         <v>16</v>
@@ -7236,10 +6871,10 @@
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="6" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D85" s="5">
         <v>31</v>
@@ -7256,10 +6891,10 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="6" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D86" s="5">
         <v>25</v>
@@ -7276,10 +6911,10 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="6" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D87" s="5">
         <v>9</v>
@@ -7296,10 +6931,10 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="7" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D88" s="5">
         <v>9</v>
@@ -7316,10 +6951,10 @@
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="7" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D89" s="5">
         <v>9</v>
@@ -7336,10 +6971,10 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="7" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D90" s="5">
         <v>11</v>
@@ -7356,10 +6991,10 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="6" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D91" s="5">
         <v>22</v>
@@ -7376,10 +7011,10 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="6" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D92" s="5">
         <v>20</v>
@@ -7396,10 +7031,10 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="6" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D93" s="5">
         <v>14</v>
@@ -7416,10 +7051,10 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="7" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D94" s="5">
         <v>16</v>
@@ -7436,10 +7071,10 @@
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="7" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D95" s="5">
         <v>11</v>
@@ -7456,10 +7091,10 @@
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="7" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D96" s="5">
         <v>16</v>
@@ -7476,10 +7111,10 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="6" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D97" s="5">
         <v>31</v>
@@ -7496,10 +7131,10 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="6" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D98" s="5">
         <v>25</v>
@@ -7516,10 +7151,10 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="6" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D99" s="5">
         <v>9</v>
@@ -7536,10 +7171,10 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="7" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D100" s="5">
         <v>9</v>
@@ -7556,10 +7191,10 @@
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="7" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D101" s="5">
         <v>9</v>
@@ -7576,10 +7211,10 @@
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="7" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D102" s="5">
         <v>11</v>
@@ -7596,10 +7231,10 @@
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="6" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D103" s="5">
         <v>22</v>
@@ -7616,10 +7251,10 @@
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="6" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D104" s="5">
         <v>20</v>
@@ -7636,10 +7271,10 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="6" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D105" s="5">
         <v>14</v>
@@ -7656,10 +7291,10 @@
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="7" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D106" s="5">
         <v>16</v>
@@ -7676,10 +7311,10 @@
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="7" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D107" s="5">
         <v>11</v>
@@ -7696,10 +7331,10 @@
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="7" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D108" s="5">
         <v>16</v>
@@ -7716,10 +7351,10 @@
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="6" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D109" s="5">
         <v>31</v>
@@ -7736,10 +7371,10 @@
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="6" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D110" s="5">
         <v>25</v>
@@ -7756,10 +7391,10 @@
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="6" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D111" s="5">
         <v>9</v>
@@ -7776,10 +7411,10 @@
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="7" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D112" s="5">
         <v>9</v>
@@ -7796,10 +7431,10 @@
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="7" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D113" s="5">
         <v>9</v>
@@ -7816,10 +7451,10 @@
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="7" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="D114" s="5">
         <v>11</v>
@@ -7860,10 +7495,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9593,8 +9228,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFA9B49-2792-48D3-82BC-E629331E59DB}">
   <dimension ref="A1:M576"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+      <selection activeCell="C300" sqref="C300:F404"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -9602,6 +9237,10 @@
     <col min="1" max="1" width="16.3125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.26171875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7890625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.5234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="25.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -9612,25 +9251,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="E1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="G1" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="H1" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="M1" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -9642,7 +9281,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="M2" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -11021,7 +10660,7 @@
         <v>950.91666999999995</v>
       </c>
       <c r="H122" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="J122" s="4"/>
     </row>
@@ -11048,7 +10687,7 @@
         <v>942</v>
       </c>
       <c r="H123" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="J123" s="4"/>
     </row>
@@ -11426,7 +11065,7 @@
         <v>1134.4166700000001</v>
       </c>
       <c r="H137" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="J137" s="4"/>
     </row>
@@ -15123,18 +14762,6 @@
       <c r="B300" s="4">
         <v>42737</v>
       </c>
-      <c r="C300">
-        <v>0.18492</v>
-      </c>
-      <c r="D300">
-        <v>4.4549999999999999E-2</v>
-      </c>
-      <c r="E300">
-        <v>0.17358000000000001</v>
-      </c>
-      <c r="F300">
-        <v>4.1009999999999998E-2</v>
-      </c>
       <c r="M300" s="4"/>
     </row>
     <row r="301" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -15144,18 +14771,6 @@
       <c r="B301" s="4">
         <v>42738</v>
       </c>
-      <c r="C301">
-        <v>0.18683</v>
-      </c>
-      <c r="D301">
-        <v>4.0890000000000003E-2</v>
-      </c>
-      <c r="E301">
-        <v>0.17624999999999999</v>
-      </c>
-      <c r="F301">
-        <v>3.7010000000000001E-2</v>
-      </c>
     </row>
     <row r="302" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A302" t="s">
@@ -15164,18 +14779,6 @@
       <c r="B302" s="4">
         <v>42739</v>
       </c>
-      <c r="C302">
-        <v>0.17674999999999999</v>
-      </c>
-      <c r="D302">
-        <v>5.5149999999999998E-2</v>
-      </c>
-      <c r="E302">
-        <v>0.16508</v>
-      </c>
-      <c r="F302">
-        <v>5.2209999999999999E-2</v>
-      </c>
     </row>
     <row r="303" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A303" t="s">
@@ -15184,18 +14787,6 @@
       <c r="B303" s="4">
         <v>42740</v>
       </c>
-      <c r="C303">
-        <v>0.17041999999999999</v>
-      </c>
-      <c r="D303">
-        <v>5.398E-2</v>
-      </c>
-      <c r="E303">
-        <v>0.15978999999999999</v>
-      </c>
-      <c r="F303">
-        <v>5.3330000000000002E-2</v>
-      </c>
     </row>
     <row r="304" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A304" t="s">
@@ -15204,1938 +14795,774 @@
       <c r="B304" s="4">
         <v>42741</v>
       </c>
-      <c r="C304">
-        <v>0.16458</v>
-      </c>
-      <c r="D304">
-        <v>5.4449999999999998E-2</v>
-      </c>
-      <c r="E304">
-        <v>0.15520999999999999</v>
-      </c>
-      <c r="F304">
-        <v>5.6509999999999998E-2</v>
-      </c>
-    </row>
-    <row r="305" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="305" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A305" t="s">
         <v>4</v>
       </c>
       <c r="B305" s="4">
         <v>42742</v>
       </c>
-      <c r="C305">
-        <v>0.15404000000000001</v>
-      </c>
-      <c r="D305">
-        <v>3.8240000000000003E-2</v>
-      </c>
-      <c r="E305">
-        <v>0.14588000000000001</v>
-      </c>
-      <c r="F305">
-        <v>4.1779999999999998E-2</v>
-      </c>
-    </row>
-    <row r="306" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="306" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A306" t="s">
         <v>4</v>
       </c>
       <c r="B306" s="4">
         <v>42743</v>
       </c>
-      <c r="C306">
-        <v>0.13553999999999999</v>
-      </c>
-      <c r="D306">
-        <v>1.491E-2</v>
-      </c>
-      <c r="E306">
-        <v>0.12992000000000001</v>
-      </c>
-      <c r="F306">
-        <v>2.2159999999999999E-2</v>
-      </c>
-    </row>
-    <row r="307" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="307" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A307" t="s">
         <v>4</v>
       </c>
       <c r="B307" s="4">
         <v>42744</v>
       </c>
-      <c r="C307">
-        <v>0.13083</v>
-      </c>
-      <c r="D307">
-        <v>6.13E-3</v>
-      </c>
-      <c r="E307">
-        <v>0.12642</v>
-      </c>
-      <c r="F307">
-        <v>1.438E-2</v>
-      </c>
-    </row>
-    <row r="308" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="308" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A308" t="s">
         <v>4</v>
       </c>
       <c r="B308" s="4">
         <v>42745</v>
       </c>
-      <c r="C308">
-        <v>0.13408</v>
-      </c>
-      <c r="D308">
-        <v>7.1000000000000002E-4</v>
-      </c>
-      <c r="E308">
-        <v>0.12962000000000001</v>
-      </c>
-      <c r="F308">
-        <v>8.0700000000000008E-3</v>
-      </c>
-    </row>
-    <row r="309" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="309" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A309" t="s">
         <v>4</v>
       </c>
       <c r="B309" s="4">
         <v>42746</v>
       </c>
-      <c r="C309">
-        <v>0.13567000000000001</v>
-      </c>
-      <c r="D309">
-        <v>4.6999999999999999E-4</v>
-      </c>
-      <c r="E309">
-        <v>0.13083</v>
-      </c>
-      <c r="F309">
-        <v>7.7799999999999996E-3</v>
-      </c>
-    </row>
-    <row r="310" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="310" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A310" t="s">
         <v>4</v>
       </c>
       <c r="B310" s="4">
         <v>42747</v>
       </c>
-      <c r="C310">
-        <v>0.13145999999999999</v>
-      </c>
-      <c r="D310">
-        <v>3.48E-3</v>
-      </c>
-      <c r="E310">
-        <v>0.12662999999999999</v>
-      </c>
-      <c r="F310">
-        <v>1.1730000000000001E-2</v>
-      </c>
-    </row>
-    <row r="311" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="311" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A311" t="s">
         <v>4</v>
       </c>
       <c r="B311" s="4">
         <v>42748</v>
       </c>
-      <c r="C311">
-        <v>0.12828999999999999</v>
-      </c>
-      <c r="D311">
-        <v>2.5300000000000001E-3</v>
-      </c>
-      <c r="E311">
-        <v>0.12379</v>
-      </c>
-      <c r="F311">
-        <v>1.125E-2</v>
-      </c>
-    </row>
-    <row r="312" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="312" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A312" t="s">
         <v>4</v>
       </c>
       <c r="B312" s="4">
         <v>42749</v>
       </c>
-      <c r="C312">
-        <v>0.12778999999999999</v>
-      </c>
-      <c r="D312">
-        <v>8.8000000000000003E-4</v>
-      </c>
-      <c r="E312">
-        <v>0.12346</v>
-      </c>
-      <c r="F312">
-        <v>7.6E-3</v>
-      </c>
-    </row>
-    <row r="313" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="313" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A313" t="s">
         <v>4</v>
       </c>
       <c r="B313" s="4">
         <v>42750</v>
       </c>
-      <c r="C313">
-        <v>0.13045999999999999</v>
-      </c>
-      <c r="D313">
-        <v>3.3600000000000001E-3</v>
-      </c>
-      <c r="E313">
-        <v>0.12570999999999999</v>
-      </c>
-      <c r="F313">
-        <v>5.4799999999999996E-3</v>
-      </c>
-    </row>
-    <row r="314" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="314" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A314" t="s">
         <v>4</v>
       </c>
       <c r="B314" s="4">
         <v>42751</v>
       </c>
-      <c r="C314">
-        <v>0.13746</v>
-      </c>
-      <c r="D314">
-        <v>1.3600000000000001E-3</v>
-      </c>
-      <c r="E314">
-        <v>0.12867000000000001</v>
-      </c>
-      <c r="F314">
-        <v>4.2399999999999998E-3</v>
-      </c>
-    </row>
-    <row r="315" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="315" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A315" t="s">
         <v>4</v>
       </c>
       <c r="B315" s="4">
         <v>42752</v>
       </c>
-      <c r="C315">
-        <v>0.14896000000000001</v>
-      </c>
-      <c r="D315">
-        <v>1.5730000000000001E-2</v>
-      </c>
-      <c r="E315">
-        <v>0.13475000000000001</v>
-      </c>
-      <c r="F315">
-        <v>1.65E-3</v>
-      </c>
-    </row>
-    <row r="316" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="316" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A316" t="s">
         <v>4</v>
       </c>
       <c r="B316" s="4">
         <v>42753</v>
       </c>
-      <c r="C316">
-        <v>0.15645999999999999</v>
-      </c>
-      <c r="D316">
-        <v>1.137E-2</v>
-      </c>
-      <c r="E316">
-        <v>0.14549999999999999</v>
-      </c>
-      <c r="F316">
-        <v>2.7100000000000002E-3</v>
-      </c>
-    </row>
-    <row r="317" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="317" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A317" t="s">
         <v>4</v>
       </c>
       <c r="B317" s="4">
         <v>42754</v>
       </c>
-      <c r="C317">
-        <v>0.16163</v>
-      </c>
-      <c r="D317">
-        <v>4.5399999999999998E-3</v>
-      </c>
-      <c r="E317">
-        <v>0.16067000000000001</v>
-      </c>
-      <c r="F317">
-        <v>1.308E-2</v>
-      </c>
-    </row>
-    <row r="318" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="318" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A318" t="s">
         <v>4</v>
       </c>
       <c r="B318" s="4">
         <v>42755</v>
       </c>
-      <c r="C318">
-        <v>0.16433</v>
-      </c>
-      <c r="D318">
-        <v>4.6999999999999999E-4</v>
-      </c>
-      <c r="E318">
-        <v>0.16375000000000001</v>
-      </c>
-      <c r="F318">
-        <v>1.355E-2</v>
-      </c>
-    </row>
-    <row r="319" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="319" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A319" t="s">
         <v>4</v>
       </c>
       <c r="B319" s="4">
         <v>42756</v>
       </c>
-      <c r="C319">
-        <v>0.20316999999999999</v>
-      </c>
-      <c r="D319">
-        <v>4.7730000000000002E-2</v>
-      </c>
-      <c r="E319">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="F319">
-        <v>1.155E-2</v>
-      </c>
-    </row>
-    <row r="320" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="320" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A320" t="s">
         <v>4</v>
       </c>
       <c r="B320" s="4">
         <v>42757</v>
       </c>
-      <c r="C320">
-        <v>0.24324999999999999</v>
-      </c>
-      <c r="D320">
-        <v>9.6990000000000007E-2</v>
-      </c>
-      <c r="E320">
-        <v>0.17821000000000001</v>
-      </c>
-      <c r="F320">
-        <v>4.0699999999999998E-3</v>
-      </c>
-    </row>
-    <row r="321" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="321" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A321" t="s">
         <v>4</v>
       </c>
       <c r="B321" s="4">
         <v>42758</v>
       </c>
-      <c r="C321">
-        <v>0.24442</v>
-      </c>
-      <c r="D321">
-        <v>9.5579999999999998E-2</v>
-      </c>
-      <c r="E321">
-        <v>0.183</v>
-      </c>
-      <c r="F321">
-        <v>8.1999999999999998E-4</v>
-      </c>
-    </row>
-    <row r="322" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="322" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A322" t="s">
         <v>4</v>
       </c>
       <c r="B322" s="4">
         <v>42759</v>
       </c>
-      <c r="C322">
-        <v>0.23921000000000001</v>
-      </c>
-      <c r="D322">
-        <v>8.3970000000000003E-2</v>
-      </c>
-      <c r="E322">
-        <v>0.18583</v>
-      </c>
-      <c r="F322">
-        <v>1.1800000000000001E-3</v>
-      </c>
-    </row>
-    <row r="323" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="323" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A323" t="s">
         <v>4</v>
       </c>
       <c r="B323" s="4">
         <v>42760</v>
       </c>
-      <c r="C323">
-        <v>0.23333000000000001</v>
-      </c>
-      <c r="D323">
-        <v>7.2599999999999998E-2</v>
-      </c>
-      <c r="E323">
-        <v>0.18546000000000001</v>
-      </c>
-      <c r="F323">
-        <v>2.3E-3</v>
-      </c>
-    </row>
-    <row r="324" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="324" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A324" t="s">
         <v>4</v>
       </c>
       <c r="B324" s="4">
         <v>42761</v>
       </c>
-      <c r="C324">
-        <v>0.23188</v>
-      </c>
-      <c r="D324">
-        <v>6.087E-2</v>
-      </c>
-      <c r="E324">
-        <v>0.18667</v>
-      </c>
-      <c r="F324">
-        <v>4.6999999999999999E-4</v>
-      </c>
-    </row>
-    <row r="325" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="325" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A325" t="s">
         <v>4</v>
       </c>
       <c r="B325" s="4">
         <v>42762</v>
       </c>
-      <c r="C325">
-        <v>0.22608</v>
-      </c>
-      <c r="D325">
-        <v>4.4670000000000001E-2</v>
-      </c>
-      <c r="E325">
-        <v>0.18754000000000001</v>
-      </c>
-      <c r="F325">
-        <v>1.5900000000000001E-3</v>
-      </c>
-    </row>
-    <row r="326" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="326" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A326" t="s">
         <v>4</v>
       </c>
       <c r="B326" s="4">
         <v>42763</v>
       </c>
-      <c r="C326">
-        <v>0.21879000000000001</v>
-      </c>
-      <c r="D326">
-        <v>2.3980000000000001E-2</v>
-      </c>
-      <c r="E326">
-        <v>0.18754000000000001</v>
-      </c>
-      <c r="F326">
-        <v>4.6600000000000001E-3</v>
-      </c>
-    </row>
-    <row r="327" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="327" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A327" t="s">
         <v>4</v>
       </c>
       <c r="B327" s="4">
         <v>42764</v>
       </c>
-      <c r="C327">
-        <v>0.21812000000000001</v>
-      </c>
-      <c r="D327">
-        <v>8.43E-3</v>
-      </c>
-      <c r="E327">
-        <v>0.18792</v>
-      </c>
-      <c r="F327">
-        <v>7.4200000000000004E-3</v>
-      </c>
-    </row>
-    <row r="328" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="328" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A328" t="s">
         <v>4</v>
       </c>
       <c r="B328" s="4">
         <v>42765</v>
       </c>
-      <c r="C328">
-        <v>0.222</v>
-      </c>
-      <c r="D328">
-        <v>4.6999999999999999E-4</v>
-      </c>
-      <c r="E328">
-        <v>0.18975</v>
-      </c>
-      <c r="F328">
-        <v>8.8400000000000006E-3</v>
-      </c>
-    </row>
-    <row r="329" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="329" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A329" t="s">
         <v>4</v>
       </c>
       <c r="B329" s="4">
         <v>42766</v>
       </c>
-      <c r="C329">
-        <v>0.24437999999999999</v>
-      </c>
-      <c r="D329">
-        <v>1.3729999999999999E-2</v>
-      </c>
-      <c r="E329">
-        <v>0.19525000000000001</v>
-      </c>
-      <c r="F329">
-        <v>1.025E-2</v>
-      </c>
-    </row>
-    <row r="330" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="330" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A330" t="s">
         <v>4</v>
       </c>
       <c r="B330" s="4">
         <v>42767</v>
       </c>
-      <c r="C330">
-        <v>0.23604</v>
-      </c>
-      <c r="D330">
-        <v>2.445E-2</v>
-      </c>
-      <c r="E330">
-        <v>0.20041999999999999</v>
-      </c>
-      <c r="F330">
-        <v>1.414E-2</v>
-      </c>
-    </row>
-    <row r="331" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="331" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A331" t="s">
         <v>4</v>
       </c>
       <c r="B331" s="4">
         <v>42768</v>
       </c>
-      <c r="C331">
-        <v>0.21912000000000001</v>
-      </c>
-      <c r="D331">
-        <v>1.585E-2</v>
-      </c>
-      <c r="E331">
-        <v>0.20716999999999999</v>
-      </c>
-      <c r="F331">
-        <v>2.5219999999999999E-2</v>
-      </c>
-    </row>
-    <row r="332" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="332" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A332" t="s">
         <v>4</v>
       </c>
       <c r="B332" s="4">
         <v>42769</v>
       </c>
-      <c r="C332">
-        <v>0.18521000000000001</v>
-      </c>
-      <c r="D332">
-        <v>2.7400000000000001E-2</v>
-      </c>
-      <c r="E332">
-        <v>0.18337999999999999</v>
-      </c>
-      <c r="F332">
-        <v>5.3800000000000001E-2</v>
-      </c>
-    </row>
-    <row r="333" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="333" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A333" t="s">
         <v>4</v>
       </c>
       <c r="B333" s="4">
         <v>42770</v>
       </c>
-      <c r="C333">
-        <v>0.17038</v>
-      </c>
-      <c r="D333">
-        <v>2.9760000000000002E-2</v>
-      </c>
-      <c r="E333">
-        <v>0.16866999999999999</v>
-      </c>
-      <c r="F333">
-        <v>5.4919999999999997E-2</v>
-      </c>
-    </row>
-    <row r="334" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="334" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A334" t="s">
         <v>4</v>
       </c>
       <c r="B334" s="4">
         <v>42771</v>
       </c>
-      <c r="C334">
-        <v>0.16603999999999999</v>
-      </c>
-      <c r="D334">
-        <v>1.797E-2</v>
-      </c>
-      <c r="E334">
-        <v>0.1615</v>
-      </c>
-      <c r="F334">
-        <v>3.8769999999999999E-2</v>
-      </c>
-    </row>
-    <row r="335" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="335" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A335" t="s">
         <v>4</v>
       </c>
       <c r="B335" s="4">
         <v>42772</v>
       </c>
-      <c r="C335">
-        <v>0.16578999999999999</v>
-      </c>
-      <c r="D335">
-        <v>1.4670000000000001E-2</v>
-      </c>
-      <c r="E335">
-        <v>0.15987000000000001</v>
-      </c>
-      <c r="F335">
-        <v>3.4000000000000002E-2</v>
-      </c>
-    </row>
-    <row r="336" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="336" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A336" t="s">
         <v>4</v>
       </c>
       <c r="B336" s="4">
         <v>42773</v>
       </c>
-      <c r="C336">
-        <v>0.16838</v>
-      </c>
-      <c r="D336">
-        <v>1.008E-2</v>
-      </c>
-      <c r="E336">
-        <v>0.16142000000000001</v>
-      </c>
-      <c r="F336">
-        <v>3.005E-2</v>
-      </c>
-    </row>
-    <row r="337" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="337" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A337" t="s">
         <v>4</v>
       </c>
       <c r="B337" s="4">
         <v>42774</v>
       </c>
-      <c r="C337">
-        <v>0.17183000000000001</v>
-      </c>
-      <c r="D337">
-        <v>1.025E-2</v>
-      </c>
-      <c r="E337">
-        <v>0.16583000000000001</v>
-      </c>
-      <c r="F337">
-        <v>2.6280000000000001E-2</v>
-      </c>
-    </row>
-    <row r="338" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="338" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A338" t="s">
         <v>4</v>
       </c>
       <c r="B338" s="4">
         <v>42775</v>
       </c>
-      <c r="C338">
-        <v>0.16941999999999999</v>
-      </c>
-      <c r="D338">
-        <v>2.0389999999999998E-2</v>
-      </c>
-      <c r="E338">
-        <v>0.16388</v>
-      </c>
-      <c r="F338">
-        <v>2.9989999999999999E-2</v>
-      </c>
-    </row>
-    <row r="339" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="339" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A339" t="s">
         <v>4</v>
       </c>
       <c r="B339" s="4">
         <v>42776</v>
       </c>
-      <c r="C339">
-        <v>0.16778999999999999</v>
-      </c>
-      <c r="D339">
-        <v>2.3279999999999999E-2</v>
-      </c>
-      <c r="E339">
-        <v>0.15892000000000001</v>
-      </c>
-      <c r="F339">
-        <v>3.2059999999999998E-2</v>
-      </c>
-    </row>
-    <row r="340" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="340" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A340" t="s">
         <v>4</v>
       </c>
       <c r="B340" s="4">
         <v>42777</v>
       </c>
-      <c r="C340">
-        <v>0.17021</v>
-      </c>
-      <c r="D340">
-        <v>1.55E-2</v>
-      </c>
-      <c r="E340">
-        <v>0.15892000000000001</v>
-      </c>
-      <c r="F340">
-        <v>2.487E-2</v>
-      </c>
-    </row>
-    <row r="341" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="341" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A341" t="s">
         <v>4</v>
       </c>
       <c r="B341" s="4">
         <v>42778</v>
       </c>
-      <c r="C341">
-        <v>0.17554</v>
-      </c>
-      <c r="D341">
-        <v>1.055E-2</v>
-      </c>
-      <c r="E341">
-        <v>0.16220999999999999</v>
-      </c>
-      <c r="F341">
-        <v>2.0449999999999999E-2</v>
-      </c>
-    </row>
-    <row r="342" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="342" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A342" t="s">
         <v>4</v>
       </c>
       <c r="B342" s="4">
         <v>42779</v>
       </c>
-      <c r="C342">
-        <v>0.18074999999999999</v>
-      </c>
-      <c r="D342">
-        <v>7.7799999999999996E-3</v>
-      </c>
-      <c r="E342">
-        <v>0.16661999999999999</v>
-      </c>
-      <c r="F342">
-        <v>1.609E-2</v>
-      </c>
-    </row>
-    <row r="343" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="343" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A343" t="s">
         <v>4</v>
       </c>
       <c r="B343" s="4">
         <v>42780</v>
       </c>
-      <c r="C343">
-        <v>0.18392</v>
-      </c>
-      <c r="D343">
-        <v>6.9499999999999996E-3</v>
-      </c>
-      <c r="E343">
-        <v>0.16975000000000001</v>
-      </c>
-      <c r="F343">
-        <v>1.332E-2</v>
-      </c>
-    </row>
-    <row r="344" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="344" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A344" t="s">
         <v>4</v>
       </c>
       <c r="B344" s="4">
         <v>42781</v>
       </c>
-      <c r="C344">
-        <v>0.18725</v>
-      </c>
-      <c r="D344">
-        <v>5.8900000000000003E-3</v>
-      </c>
-      <c r="E344">
-        <v>0.17321</v>
-      </c>
-      <c r="F344">
-        <v>9.3699999999999999E-3</v>
-      </c>
-    </row>
-    <row r="345" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="345" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A345" t="s">
         <v>4</v>
       </c>
       <c r="B345" s="4">
         <v>42782</v>
       </c>
-      <c r="C345">
-        <v>0.18975</v>
-      </c>
-      <c r="D345">
-        <v>3.5400000000000002E-3</v>
-      </c>
-      <c r="E345">
-        <v>0.17616999999999999</v>
-      </c>
-      <c r="F345">
-        <v>5.4200000000000003E-3</v>
-      </c>
-    </row>
-    <row r="346" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="346" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A346" t="s">
         <v>4</v>
       </c>
       <c r="B346" s="4">
         <v>42783</v>
       </c>
-      <c r="C346">
-        <v>0.20924999999999999</v>
-      </c>
-      <c r="D346">
-        <v>2.4160000000000001E-2</v>
-      </c>
-      <c r="E346">
-        <v>0.19433</v>
-      </c>
-      <c r="F346">
-        <v>2.0150000000000001E-2</v>
-      </c>
-    </row>
-    <row r="347" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="347" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A347" t="s">
         <v>4</v>
       </c>
       <c r="B347" s="4">
         <v>42784</v>
       </c>
-      <c r="C347">
-        <v>0.24004</v>
-      </c>
-      <c r="D347">
-        <v>6.6530000000000006E-2</v>
-      </c>
-      <c r="E347">
-        <v>0.22267000000000001</v>
-      </c>
-      <c r="F347">
-        <v>5.8340000000000003E-2</v>
-      </c>
-    </row>
-    <row r="348" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="348" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A348" t="s">
         <v>4</v>
       </c>
       <c r="B348" s="4">
         <v>42785</v>
       </c>
-      <c r="C348">
-        <v>0.23924999999999999</v>
-      </c>
-      <c r="D348">
-        <v>6.2810000000000005E-2</v>
-      </c>
-      <c r="E348">
-        <v>0.22103999999999999</v>
-      </c>
-      <c r="F348">
-        <v>5.5449999999999999E-2</v>
-      </c>
-    </row>
-    <row r="349" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="349" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A349" t="s">
         <v>4</v>
       </c>
       <c r="B349" s="4">
         <v>42786</v>
       </c>
-      <c r="C349">
-        <v>0.24732999999999999</v>
-      </c>
-      <c r="D349">
-        <v>4.3020000000000003E-2</v>
-      </c>
-      <c r="E349">
-        <v>0.22287999999999999</v>
-      </c>
-      <c r="F349">
-        <v>4.1779999999999998E-2</v>
-      </c>
-    </row>
-    <row r="350" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="350" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A350" t="s">
         <v>4</v>
       </c>
       <c r="B350" s="4">
         <v>42787</v>
       </c>
-      <c r="C350">
-        <v>0.24192</v>
-      </c>
-      <c r="D350">
-        <v>3.099E-2</v>
-      </c>
-      <c r="E350">
-        <v>0.2215</v>
-      </c>
-      <c r="F350">
-        <v>3.4880000000000001E-2</v>
-      </c>
-    </row>
-    <row r="351" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="351" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A351" t="s">
         <v>4</v>
       </c>
       <c r="B351" s="4">
         <v>42788</v>
       </c>
-      <c r="C351">
-        <v>0.23471</v>
-      </c>
-      <c r="D351">
-        <v>2.7400000000000001E-2</v>
-      </c>
-      <c r="E351">
-        <v>0.21662000000000001</v>
-      </c>
-      <c r="F351">
-        <v>3.2590000000000001E-2</v>
-      </c>
-    </row>
-    <row r="352" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="352" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A352" t="s">
         <v>4</v>
       </c>
       <c r="B352" s="4">
         <v>42789</v>
       </c>
-      <c r="C352">
-        <v>0.23</v>
-      </c>
-      <c r="D352">
-        <v>2.64E-2</v>
-      </c>
-      <c r="E352">
-        <v>0.21357999999999999</v>
-      </c>
-      <c r="F352">
-        <v>3.0519999999999999E-2</v>
-      </c>
-    </row>
-    <row r="353" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A353" t="s">
         <v>4</v>
       </c>
       <c r="B353" s="4">
         <v>42790</v>
       </c>
-      <c r="C353">
-        <v>0.22525000000000001</v>
-      </c>
-      <c r="D353">
-        <v>3.0519999999999999E-2</v>
-      </c>
-      <c r="E353">
-        <v>0.20849999999999999</v>
-      </c>
-      <c r="F353">
-        <v>3.0759999999999999E-2</v>
-      </c>
-    </row>
-    <row r="354" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A354" t="s">
         <v>4</v>
       </c>
       <c r="B354" s="4">
         <v>42791</v>
       </c>
-      <c r="C354">
-        <v>0.22661999999999999</v>
-      </c>
-      <c r="D354">
-        <v>2.4570000000000002E-2</v>
-      </c>
-      <c r="E354">
-        <v>0.21317</v>
-      </c>
-      <c r="F354">
-        <v>3.2289999999999999E-2</v>
-      </c>
-    </row>
-    <row r="355" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A355" t="s">
         <v>4</v>
       </c>
       <c r="B355" s="4">
         <v>42792</v>
       </c>
-      <c r="C355">
-        <v>0.22761999999999999</v>
-      </c>
-      <c r="D355">
-        <v>2.6689999999999998E-2</v>
-      </c>
-      <c r="E355">
-        <v>0.21232999999999999</v>
-      </c>
-      <c r="F355">
-        <v>3.1469999999999998E-2</v>
-      </c>
-    </row>
-    <row r="356" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A356" t="s">
         <v>4</v>
       </c>
       <c r="B356" s="4">
         <v>42793</v>
       </c>
-      <c r="C356">
-        <v>0.22946</v>
-      </c>
-      <c r="D356">
-        <v>2.6460000000000001E-2</v>
-      </c>
-      <c r="E356">
-        <v>0.21346000000000001</v>
-      </c>
-      <c r="F356">
-        <v>3.2469999999999999E-2</v>
-      </c>
-    </row>
-    <row r="357" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A357" t="s">
         <v>4</v>
       </c>
       <c r="B357" s="4">
         <v>42794</v>
       </c>
-      <c r="C357">
-        <v>0.22928999999999999</v>
-      </c>
-      <c r="D357">
-        <v>2.7279999999999999E-2</v>
-      </c>
-      <c r="E357">
-        <v>0.21221000000000001</v>
-      </c>
-      <c r="F357">
-        <v>3.1530000000000002E-2</v>
-      </c>
-    </row>
-    <row r="358" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A358" t="s">
         <v>4</v>
       </c>
       <c r="B358" s="4">
         <v>42795</v>
       </c>
-      <c r="C358">
-        <v>0.22796</v>
-      </c>
-      <c r="D358">
-        <v>2.622E-2</v>
-      </c>
-      <c r="E358">
-        <v>0.21162</v>
-      </c>
-      <c r="F358">
-        <v>3.0349999999999999E-2</v>
-      </c>
-    </row>
-    <row r="359" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A359" t="s">
         <v>4</v>
       </c>
       <c r="B359" s="4">
         <v>42796</v>
       </c>
-      <c r="C359">
-        <v>0.22578999999999999</v>
-      </c>
-      <c r="D359">
-        <v>2.375E-2</v>
-      </c>
-      <c r="E359">
-        <v>0.21092</v>
-      </c>
-      <c r="F359">
-        <v>2.9819999999999999E-2</v>
-      </c>
-    </row>
-    <row r="360" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A360" t="s">
         <v>4</v>
       </c>
       <c r="B360" s="4">
         <v>42797</v>
       </c>
-      <c r="C360">
-        <v>0.22320999999999999</v>
-      </c>
-      <c r="D360">
-        <v>2.1389999999999999E-2</v>
-      </c>
-      <c r="E360">
-        <v>0.20916999999999999</v>
-      </c>
-      <c r="F360">
-        <v>2.911E-2</v>
-      </c>
-    </row>
-    <row r="361" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A361" t="s">
         <v>4</v>
       </c>
       <c r="B361" s="4">
         <v>42798</v>
       </c>
-      <c r="C361">
-        <v>0.22192000000000001</v>
-      </c>
-      <c r="D361">
-        <v>2.1569999999999999E-2</v>
-      </c>
-      <c r="E361">
-        <v>0.20771000000000001</v>
-      </c>
-      <c r="F361">
-        <v>2.8340000000000001E-2</v>
-      </c>
-    </row>
-    <row r="362" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A362" t="s">
         <v>4</v>
       </c>
       <c r="B362" s="4">
         <v>42799</v>
       </c>
-      <c r="C362">
-        <v>0.22217000000000001</v>
-      </c>
-      <c r="D362">
-        <v>2.2859999999999998E-2</v>
-      </c>
-      <c r="E362">
-        <v>0.20729</v>
-      </c>
-      <c r="F362">
-        <v>2.7869999999999999E-2</v>
-      </c>
-    </row>
-    <row r="363" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A363" t="s">
         <v>4</v>
       </c>
       <c r="B363" s="4">
         <v>42800</v>
       </c>
-      <c r="C363">
-        <v>0.22262000000000001</v>
-      </c>
-      <c r="D363">
-        <v>2.375E-2</v>
-      </c>
-      <c r="E363">
-        <v>0.20754</v>
-      </c>
-      <c r="F363">
-        <v>2.7990000000000001E-2</v>
-      </c>
-    </row>
-    <row r="364" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A364" t="s">
         <v>4</v>
       </c>
       <c r="B364" s="4">
         <v>42801</v>
       </c>
-      <c r="C364">
-        <v>0.22458</v>
-      </c>
-      <c r="D364">
-        <v>2.605E-2</v>
-      </c>
-      <c r="E364">
-        <v>0.20829</v>
-      </c>
-      <c r="F364">
-        <v>2.775E-2</v>
-      </c>
-    </row>
-    <row r="365" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A365" t="s">
         <v>4</v>
       </c>
       <c r="B365" s="4">
         <v>42802</v>
       </c>
-      <c r="C365">
-        <v>0.22275</v>
-      </c>
-      <c r="D365">
-        <v>2.3689999999999999E-2</v>
-      </c>
-      <c r="E365">
-        <v>0.20854</v>
-      </c>
-      <c r="F365">
-        <v>2.8230000000000002E-2</v>
-      </c>
-    </row>
-    <row r="366" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A366" t="s">
         <v>4</v>
       </c>
       <c r="B366" s="4">
         <v>42803</v>
       </c>
-      <c r="C366">
-        <v>0.22153999999999999</v>
-      </c>
-      <c r="D366">
-        <v>2.2689999999999998E-2</v>
-      </c>
-      <c r="E366">
-        <v>0.20788000000000001</v>
-      </c>
-      <c r="F366">
-        <v>2.8580000000000001E-2</v>
-      </c>
-    </row>
-    <row r="367" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A367" t="s">
         <v>4</v>
       </c>
       <c r="B367" s="4">
         <v>42804</v>
       </c>
-      <c r="C367">
-        <v>0.22033</v>
-      </c>
-      <c r="D367">
-        <v>2.086E-2</v>
-      </c>
-      <c r="E367">
-        <v>0.20716999999999999</v>
-      </c>
-      <c r="F367">
-        <v>2.8170000000000001E-2</v>
-      </c>
-    </row>
-    <row r="368" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A368" t="s">
         <v>4</v>
       </c>
       <c r="B368" s="4">
         <v>42805</v>
       </c>
-      <c r="C368">
-        <v>0.21892</v>
-      </c>
-      <c r="D368">
-        <v>2.0979999999999999E-2</v>
-      </c>
-      <c r="E368">
-        <v>0.20621</v>
-      </c>
-      <c r="F368">
-        <v>2.8580000000000001E-2</v>
-      </c>
-    </row>
-    <row r="369" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A369" t="s">
         <v>4</v>
       </c>
       <c r="B369" s="4">
         <v>42806</v>
       </c>
-      <c r="C369">
-        <v>0.21808</v>
-      </c>
-      <c r="D369">
-        <v>2.0150000000000001E-2</v>
-      </c>
-      <c r="E369">
-        <v>0.20533000000000001</v>
-      </c>
-      <c r="F369">
-        <v>2.793E-2</v>
-      </c>
-    </row>
-    <row r="370" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A370" t="s">
         <v>4</v>
       </c>
       <c r="B370" s="4">
         <v>42807</v>
       </c>
-      <c r="C370">
-        <v>0.21795999999999999</v>
-      </c>
-      <c r="D370">
-        <v>2.2329999999999999E-2</v>
-      </c>
-      <c r="E370">
-        <v>0.20441999999999999</v>
-      </c>
-      <c r="F370">
-        <v>2.6870000000000002E-2</v>
-      </c>
-    </row>
-    <row r="371" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A371" t="s">
         <v>4</v>
       </c>
       <c r="B371" s="4">
         <v>42808</v>
       </c>
-      <c r="C371">
-        <v>0.21596000000000001</v>
-      </c>
-      <c r="D371">
-        <v>2.0330000000000001E-2</v>
-      </c>
-      <c r="E371">
-        <v>0.20374999999999999</v>
-      </c>
-      <c r="F371">
-        <v>2.699E-2</v>
-      </c>
-    </row>
-    <row r="372" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A372" t="s">
         <v>4</v>
       </c>
       <c r="B372" s="4">
         <v>42809</v>
       </c>
-      <c r="C372">
-        <v>0.21238000000000001</v>
-      </c>
-      <c r="D372">
-        <v>1.6559999999999998E-2</v>
-      </c>
-      <c r="E372">
-        <v>0.20166999999999999</v>
-      </c>
-      <c r="F372">
-        <v>2.605E-2</v>
-      </c>
-    </row>
-    <row r="373" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A373" t="s">
         <v>4</v>
       </c>
       <c r="B373" s="4">
         <v>42810</v>
       </c>
-      <c r="C373">
-        <v>0.21242</v>
-      </c>
-      <c r="D373">
-        <v>1.7319999999999999E-2</v>
-      </c>
-      <c r="E373">
-        <v>0.20041999999999999</v>
-      </c>
-      <c r="F373">
-        <v>2.5930000000000002E-2</v>
-      </c>
-    </row>
-    <row r="374" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A374" t="s">
         <v>4</v>
       </c>
       <c r="B374" s="4">
         <v>42811</v>
       </c>
-      <c r="C374">
-        <v>0.21492</v>
-      </c>
-      <c r="D374">
-        <v>2.2159999999999999E-2</v>
-      </c>
-      <c r="E374">
-        <v>0.20196</v>
-      </c>
-      <c r="F374">
-        <v>2.6579999999999999E-2</v>
-      </c>
-    </row>
-    <row r="375" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A375" t="s">
         <v>4</v>
       </c>
       <c r="B375" s="4">
         <v>42812</v>
       </c>
-      <c r="C375">
-        <v>0.21592</v>
-      </c>
-      <c r="D375">
-        <v>2.121E-2</v>
-      </c>
-      <c r="E375">
-        <v>0.20291999999999999</v>
-      </c>
-      <c r="F375">
-        <v>2.6749999999999999E-2</v>
-      </c>
-    </row>
-    <row r="376" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A376" t="s">
         <v>4</v>
       </c>
       <c r="B376" s="4">
         <v>42813</v>
       </c>
-      <c r="C376">
-        <v>0.21612000000000001</v>
-      </c>
-      <c r="D376">
-        <v>2.1270000000000001E-2</v>
-      </c>
-      <c r="E376">
-        <v>0.20324999999999999</v>
-      </c>
-      <c r="F376">
-        <v>2.6159999999999999E-2</v>
-      </c>
-    </row>
-    <row r="377" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A377" t="s">
         <v>4</v>
       </c>
       <c r="B377" s="4">
         <v>42814</v>
       </c>
-      <c r="C377">
-        <v>0.21733</v>
-      </c>
-      <c r="D377">
-        <v>2.1569999999999999E-2</v>
-      </c>
-      <c r="E377">
-        <v>0.20391999999999999</v>
-      </c>
-      <c r="F377">
-        <v>2.6280000000000001E-2</v>
-      </c>
-    </row>
-    <row r="378" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A378" t="s">
         <v>4</v>
       </c>
       <c r="B378" s="4">
         <v>42815</v>
       </c>
-      <c r="C378">
-        <v>0.21754000000000001</v>
-      </c>
-      <c r="D378">
-        <v>2.0570000000000001E-2</v>
-      </c>
-      <c r="E378">
-        <v>0.20391999999999999</v>
-      </c>
-      <c r="F378">
-        <v>2.5340000000000001E-2</v>
-      </c>
-    </row>
-    <row r="379" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A379" t="s">
         <v>4</v>
       </c>
       <c r="B379" s="4">
         <v>42816</v>
       </c>
-      <c r="C379">
-        <v>0.21621000000000001</v>
-      </c>
-      <c r="D379">
-        <v>1.95E-2</v>
-      </c>
-      <c r="E379">
-        <v>0.20333000000000001</v>
-      </c>
-      <c r="F379">
-        <v>2.4979999999999999E-2</v>
-      </c>
-    </row>
-    <row r="380" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A380" t="s">
         <v>4</v>
       </c>
       <c r="B380" s="4">
         <v>42817</v>
       </c>
-      <c r="C380">
-        <v>0.2155</v>
-      </c>
-      <c r="D380">
-        <v>1.968E-2</v>
-      </c>
-      <c r="E380">
-        <v>0.20279</v>
-      </c>
-      <c r="F380">
-        <v>2.5159999999999998E-2</v>
-      </c>
-    </row>
-    <row r="381" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A381" t="s">
         <v>4</v>
       </c>
       <c r="B381" s="4">
         <v>42818</v>
       </c>
-      <c r="C381">
-        <v>0.21512000000000001</v>
-      </c>
-      <c r="D381">
-        <v>2.1739999999999999E-2</v>
-      </c>
-      <c r="E381">
-        <v>0.20188</v>
-      </c>
-      <c r="F381">
-        <v>2.41E-2</v>
-      </c>
-    </row>
-    <row r="382" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A382" t="s">
         <v>4</v>
       </c>
       <c r="B382" s="4">
         <v>42819</v>
       </c>
-      <c r="C382">
-        <v>0.22558</v>
-      </c>
-      <c r="D382">
-        <v>3.406E-2</v>
-      </c>
-      <c r="E382">
-        <v>0.21182999999999999</v>
-      </c>
-      <c r="F382">
-        <v>3.099E-2</v>
-      </c>
-    </row>
-    <row r="383" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A383" t="s">
         <v>4</v>
       </c>
       <c r="B383" s="4">
         <v>42820</v>
       </c>
-      <c r="C383">
-        <v>0.23183000000000001</v>
-      </c>
-      <c r="D383">
-        <v>2.9819999999999999E-2</v>
-      </c>
-      <c r="E383">
-        <v>0.21737999999999999</v>
-      </c>
-      <c r="F383">
-        <v>3.1640000000000001E-2</v>
-      </c>
-    </row>
-    <row r="384" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A384" t="s">
         <v>4</v>
       </c>
       <c r="B384" s="4">
         <v>42821</v>
       </c>
-      <c r="C384">
-        <v>0.23116999999999999</v>
-      </c>
-      <c r="D384">
-        <v>2.699E-2</v>
-      </c>
-      <c r="E384">
-        <v>0.21425</v>
-      </c>
-      <c r="F384">
-        <v>2.9340000000000001E-2</v>
-      </c>
-    </row>
-    <row r="385" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A385" t="s">
         <v>4</v>
       </c>
       <c r="B385" s="4">
         <v>42822</v>
       </c>
-      <c r="C385">
-        <v>0.22858000000000001</v>
-      </c>
-      <c r="D385">
-        <v>2.64E-2</v>
-      </c>
-      <c r="E385">
-        <v>0.21246000000000001</v>
-      </c>
-      <c r="F385">
-        <v>2.7990000000000001E-2</v>
-      </c>
-    </row>
-    <row r="386" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A386" t="s">
         <v>4</v>
       </c>
       <c r="B386" s="4">
         <v>42823</v>
       </c>
-      <c r="C386">
-        <v>0.23211999999999999</v>
-      </c>
-      <c r="D386">
-        <v>3.2469999999999999E-2</v>
-      </c>
-      <c r="E386">
-        <v>0.22275</v>
-      </c>
-      <c r="F386">
-        <v>3.7949999999999998E-2</v>
-      </c>
-    </row>
-    <row r="387" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A387" t="s">
         <v>4</v>
       </c>
       <c r="B387" s="4">
         <v>42824</v>
       </c>
-      <c r="C387">
-        <v>0.23654</v>
-      </c>
-      <c r="D387">
-        <v>3.1050000000000001E-2</v>
-      </c>
-      <c r="E387">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="F387">
-        <v>5.0319999999999997E-2</v>
-      </c>
-    </row>
-    <row r="388" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="388" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A388" t="s">
         <v>4</v>
       </c>
       <c r="B388" s="4">
         <v>42825</v>
       </c>
-      <c r="C388">
-        <v>0.23241999999999999</v>
-      </c>
-      <c r="D388">
-        <v>2.6159999999999999E-2</v>
-      </c>
-      <c r="E388">
-        <v>0.22878999999999999</v>
-      </c>
-      <c r="F388">
-        <v>4.7320000000000001E-2</v>
-      </c>
-    </row>
-    <row r="389" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="389" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A389" t="s">
         <v>4</v>
       </c>
       <c r="B389" s="4">
         <v>42826</v>
       </c>
-      <c r="C389">
-        <v>0.23008000000000001</v>
-      </c>
-      <c r="D389">
-        <v>2.4979999999999999E-2</v>
-      </c>
-      <c r="E389">
-        <v>0.22608</v>
-      </c>
-      <c r="F389">
-        <v>4.5370000000000001E-2</v>
-      </c>
-    </row>
-    <row r="390" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="390" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A390" t="s">
         <v>4</v>
       </c>
       <c r="B390" s="4">
         <v>42827</v>
       </c>
-      <c r="C390">
-        <v>0.22825000000000001</v>
-      </c>
-      <c r="D390">
-        <v>2.4979999999999999E-2</v>
-      </c>
-      <c r="E390">
-        <v>0.22417000000000001</v>
-      </c>
-      <c r="F390">
-        <v>4.3839999999999997E-2</v>
-      </c>
-    </row>
-    <row r="391" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="391" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A391" t="s">
         <v>4</v>
       </c>
       <c r="B391" s="4">
         <v>42828</v>
       </c>
-      <c r="C391">
-        <v>0.23221</v>
-      </c>
-      <c r="D391">
-        <v>3.0460000000000001E-2</v>
-      </c>
-      <c r="E391">
-        <v>0.22733</v>
-      </c>
-      <c r="F391">
-        <v>4.7140000000000001E-2</v>
-      </c>
-    </row>
-    <row r="392" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="392" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A392" t="s">
         <v>4</v>
       </c>
       <c r="B392" s="4">
         <v>42829</v>
       </c>
-      <c r="C392">
-        <v>0.23621</v>
-      </c>
-      <c r="D392">
-        <v>2.9520000000000001E-2</v>
-      </c>
-      <c r="E392">
-        <v>0.23021</v>
-      </c>
-      <c r="F392">
-        <v>4.437E-2</v>
-      </c>
-    </row>
-    <row r="393" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="393" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A393" t="s">
         <v>4</v>
       </c>
       <c r="B393" s="4">
         <v>42830</v>
       </c>
-      <c r="C393">
-        <v>0.23279</v>
-      </c>
-      <c r="D393">
-        <v>2.6100000000000002E-2</v>
-      </c>
-      <c r="E393">
-        <v>0.22725000000000001</v>
-      </c>
-      <c r="F393">
-        <v>4.231E-2</v>
-      </c>
-    </row>
-    <row r="394" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="394" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A394" t="s">
         <v>4</v>
       </c>
       <c r="B394" s="4">
         <v>42831</v>
       </c>
-      <c r="C394">
-        <v>0.23083000000000001</v>
-      </c>
-      <c r="D394">
-        <v>2.392E-2</v>
-      </c>
-      <c r="E394">
-        <v>0.22567000000000001</v>
-      </c>
-      <c r="F394">
-        <v>4.1959999999999997E-2</v>
-      </c>
-    </row>
-    <row r="395" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="395" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A395" t="s">
         <v>4</v>
       </c>
       <c r="B395" s="4">
         <v>42832</v>
       </c>
-      <c r="C395">
-        <v>0.22950000000000001</v>
-      </c>
-      <c r="D395">
-        <v>2.1569999999999999E-2</v>
-      </c>
-      <c r="E395">
-        <v>0.22470999999999999</v>
-      </c>
-      <c r="F395">
-        <v>4.2130000000000001E-2</v>
-      </c>
-    </row>
-    <row r="396" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="396" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A396" t="s">
         <v>4</v>
       </c>
       <c r="B396" s="4">
         <v>42833</v>
       </c>
-      <c r="C396">
-        <v>0.22911999999999999</v>
-      </c>
-      <c r="D396">
-        <v>2.1739999999999999E-2</v>
-      </c>
-      <c r="E396">
-        <v>0.22378999999999999</v>
-      </c>
-      <c r="F396">
-        <v>4.2009999999999999E-2</v>
-      </c>
-    </row>
-    <row r="397" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="397" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A397" t="s">
         <v>4</v>
       </c>
       <c r="B397" s="4">
         <v>42834</v>
       </c>
-      <c r="C397">
-        <v>0.22992000000000001</v>
-      </c>
-      <c r="D397">
-        <v>2.2509999999999999E-2</v>
-      </c>
-      <c r="E397">
-        <v>0.22428999999999999</v>
-      </c>
-      <c r="F397">
-        <v>4.1419999999999998E-2</v>
-      </c>
-    </row>
-    <row r="398" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="398" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A398" t="s">
         <v>4</v>
       </c>
       <c r="B398" s="4">
         <v>42835</v>
       </c>
-      <c r="C398">
-        <v>0.22978999999999999</v>
-      </c>
-      <c r="D398">
-        <v>2.198E-2</v>
-      </c>
-      <c r="E398">
-        <v>0.22450000000000001</v>
-      </c>
-      <c r="F398">
-        <v>4.0309999999999999E-2</v>
-      </c>
-    </row>
-    <row r="399" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="399" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A399" t="s">
         <v>4</v>
       </c>
       <c r="B399" s="4">
         <v>42836</v>
       </c>
-      <c r="C399">
-        <v>0.22821</v>
-      </c>
-      <c r="D399">
-        <v>2.104E-2</v>
-      </c>
-      <c r="E399">
-        <v>0.22292000000000001</v>
-      </c>
-      <c r="F399">
-        <v>3.9359999999999999E-2</v>
-      </c>
-    </row>
-    <row r="400" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+    </row>
+    <row r="400" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A400" t="s">
         <v>4</v>
       </c>
       <c r="B400" s="4">
         <v>42837</v>
       </c>
-      <c r="C400">
-        <v>0.224</v>
-      </c>
-      <c r="D400">
-        <v>1.558E-2</v>
-      </c>
-      <c r="E400">
-        <v>0.20874999999999999</v>
-      </c>
-      <c r="F400">
-        <v>3.6119999999999999E-2</v>
-      </c>
     </row>
     <row r="401" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A401" t="s">
@@ -17144,18 +15571,6 @@
       <c r="B401" s="4">
         <v>42838</v>
       </c>
-      <c r="C401">
-        <v>0.22467000000000001</v>
-      </c>
-      <c r="D401">
-        <v>1.566E-2</v>
-      </c>
-      <c r="E401">
-        <v>0.20860999999999999</v>
-      </c>
-      <c r="F401">
-        <v>3.5720000000000002E-2</v>
-      </c>
     </row>
     <row r="402" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A402" t="s">
@@ -17164,18 +15579,6 @@
       <c r="B402" s="4">
         <v>42839</v>
       </c>
-      <c r="C402">
-        <v>0.22594</v>
-      </c>
-      <c r="D402">
-        <v>1.448E-2</v>
-      </c>
-      <c r="E402">
-        <v>0.20916999999999999</v>
-      </c>
-      <c r="F402">
-        <v>3.5580000000000001E-2</v>
-      </c>
     </row>
     <row r="403" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A403" t="s">
@@ -17184,18 +15587,6 @@
       <c r="B403" s="4">
         <v>42840</v>
       </c>
-      <c r="C403">
-        <v>0.22917000000000001</v>
-      </c>
-      <c r="D403">
-        <v>1.6490000000000001E-2</v>
-      </c>
-      <c r="E403">
-        <v>0.20749999999999999</v>
-      </c>
-      <c r="F403">
-        <v>3.9609999999999999E-2</v>
-      </c>
     </row>
     <row r="404" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A404" t="s">
@@ -17203,18 +15594,6 @@
       </c>
       <c r="B404" s="4">
         <v>42841</v>
-      </c>
-      <c r="C404">
-        <v>0.23091999999999999</v>
-      </c>
-      <c r="D404">
-        <v>1.762E-2</v>
-      </c>
-      <c r="E404">
-        <v>0.20996999999999999</v>
-      </c>
-      <c r="F404">
-        <v>4.0030000000000003E-2</v>
       </c>
     </row>
     <row r="405" spans="1:6" x14ac:dyDescent="0.55000000000000004">
@@ -20685,16 +19064,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="E1" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
added root depth graph
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0A506F8-F5B9-47D3-A647-5471CB225495}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84C8B367-840A-4DA8-A823-989AE0E5C4E5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ObservedOLD" sheetId="13" r:id="rId1"/>
@@ -87,9 +87,6 @@
   </si>
   <si>
     <t>SLA_apsim_total</t>
-  </si>
-  <si>
-    <t>Root_in</t>
   </si>
   <si>
     <t>Height</t>
@@ -559,6 +556,9 @@
   <si>
     <t>Soybean.AboveGround.N</t>
   </si>
+  <si>
+    <t>Soybean.Root.Depth</t>
+  </si>
 </sst>
 </file>
 
@@ -1659,10 +1659,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
   <dimension ref="A1:BV114"/>
   <sheetViews>
-    <sheetView topLeftCell="Z1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A19" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" topLeftCell="Z1" workbookViewId="0">
+      <pane ySplit="576" activePane="bottomLeft"/>
       <selection activeCell="W1" sqref="W1:W1048576"/>
-      <selection pane="bottomLeft" activeCell="AN23" sqref="AN23"/>
+      <selection pane="bottomLeft" activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1700,13 +1700,13 @@
         <v>14</v>
       </c>
       <c r="D1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E1" t="s">
         <v>63</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>64</v>
-      </c>
-      <c r="F1" t="s">
-        <v>65</v>
       </c>
       <c r="G1" t="s">
         <v>15</v>
@@ -1715,85 +1715,85 @@
         <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="J1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K1" t="s">
+        <v>89</v>
+      </c>
+      <c r="L1" t="s">
+        <v>55</v>
+      </c>
+      <c r="M1" t="s">
+        <v>91</v>
+      </c>
+      <c r="N1" t="s">
         <v>90</v>
-      </c>
-      <c r="L1" t="s">
-        <v>56</v>
-      </c>
-      <c r="M1" t="s">
-        <v>92</v>
-      </c>
-      <c r="N1" t="s">
-        <v>91</v>
       </c>
       <c r="O1" t="s">
         <v>12</v>
       </c>
       <c r="P1" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q1" t="s">
         <v>57</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>58</v>
-      </c>
-      <c r="R1" t="s">
-        <v>59</v>
       </c>
       <c r="S1" t="s">
         <v>6</v>
       </c>
       <c r="T1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="U1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V1" t="s">
         <v>7</v>
       </c>
       <c r="W1" t="s">
+        <v>169</v>
+      </c>
+      <c r="X1" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>167</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>166</v>
+      </c>
+      <c r="AA1" t="s">
         <v>170</v>
       </c>
-      <c r="X1" t="s">
-        <v>169</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>168</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>167</v>
-      </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
+        <v>173</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>162</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>163</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>165</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>164</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>174</v>
+      </c>
+      <c r="AH1" t="s">
         <v>171</v>
       </c>
-      <c r="AB1" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>166</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>165</v>
-      </c>
-      <c r="AG1" t="s">
+      <c r="AI1" t="s">
         <v>175</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>172</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>176</v>
       </c>
       <c r="AJ1" t="s">
         <v>17</v>
@@ -1805,112 +1805,112 @@
         <v>19</v>
       </c>
       <c r="AM1" t="s">
+        <v>176</v>
+      </c>
+      <c r="AN1" t="s">
         <v>20</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>21</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>22</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>23</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>24</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>25</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>26</v>
       </c>
-      <c r="AT1" t="s">
+      <c r="AU1" t="s">
         <v>27</v>
       </c>
-      <c r="AU1" t="s">
+      <c r="AV1" t="s">
         <v>28</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>29</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>30</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="AY1" t="s">
         <v>31</v>
       </c>
-      <c r="AY1" t="s">
+      <c r="AZ1" t="s">
         <v>32</v>
       </c>
-      <c r="AZ1" t="s">
+      <c r="BA1" t="s">
         <v>33</v>
       </c>
-      <c r="BA1" t="s">
+      <c r="BB1" t="s">
         <v>34</v>
       </c>
-      <c r="BB1" t="s">
+      <c r="BC1" t="s">
         <v>35</v>
       </c>
-      <c r="BC1" t="s">
+      <c r="BD1" t="s">
         <v>36</v>
       </c>
-      <c r="BD1" t="s">
+      <c r="BE1" t="s">
         <v>37</v>
       </c>
-      <c r="BE1" t="s">
+      <c r="BF1" t="s">
         <v>38</v>
       </c>
-      <c r="BF1" t="s">
+      <c r="BG1" t="s">
         <v>39</v>
       </c>
-      <c r="BG1" t="s">
+      <c r="BH1" t="s">
         <v>40</v>
       </c>
-      <c r="BH1" t="s">
+      <c r="BI1" t="s">
         <v>41</v>
       </c>
-      <c r="BI1" t="s">
+      <c r="BJ1" t="s">
         <v>42</v>
       </c>
-      <c r="BJ1" t="s">
+      <c r="BK1" t="s">
         <v>43</v>
       </c>
-      <c r="BK1" t="s">
+      <c r="BL1" t="s">
         <v>44</v>
       </c>
-      <c r="BL1" t="s">
+      <c r="BM1" t="s">
         <v>45</v>
       </c>
-      <c r="BM1" t="s">
+      <c r="BN1" t="s">
         <v>46</v>
       </c>
-      <c r="BN1" t="s">
+      <c r="BO1" t="s">
         <v>47</v>
       </c>
-      <c r="BO1" t="s">
+      <c r="BP1" t="s">
         <v>48</v>
       </c>
-      <c r="BP1" t="s">
+      <c r="BQ1" t="s">
         <v>49</v>
       </c>
-      <c r="BQ1" t="s">
+      <c r="BR1" t="s">
         <v>50</v>
       </c>
-      <c r="BR1" t="s">
+      <c r="BS1" t="s">
         <v>51</v>
       </c>
-      <c r="BS1" t="s">
+      <c r="BT1" t="s">
         <v>52</v>
       </c>
-      <c r="BT1" t="s">
+      <c r="BU1" t="s">
         <v>53</v>
       </c>
-      <c r="BU1" t="s">
+      <c r="BV1" t="s">
         <v>54</v>
-      </c>
-      <c r="BV1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:74" x14ac:dyDescent="0.55000000000000004">
@@ -3175,7 +3175,7 @@
         <v>43026</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
@@ -4354,7 +4354,7 @@
         <v>43026</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D20" s="4"/>
       <c r="E20" s="4"/>
@@ -4410,7 +4410,7 @@
     </row>
     <row r="23" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B23" s="4">
         <v>42898</v>
@@ -4527,7 +4527,7 @@
     </row>
     <row r="24" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B24" s="4">
         <v>42915</v>
@@ -4644,7 +4644,7 @@
     </row>
     <row r="25" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B25" s="4">
         <v>42929</v>
@@ -4764,7 +4764,7 @@
     </row>
     <row r="26" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B26" s="4">
         <v>42943</v>
@@ -4896,7 +4896,7 @@
     </row>
     <row r="27" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B27" s="4">
         <v>42957</v>
@@ -5034,7 +5034,7 @@
     </row>
     <row r="28" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B28" s="4">
         <v>42975</v>
@@ -5166,7 +5166,7 @@
     </row>
     <row r="29" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B29" s="4">
         <v>42993</v>
@@ -5276,7 +5276,7 @@
     </row>
     <row r="30" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B30" s="4">
         <v>43028</v>
@@ -5320,7 +5320,7 @@
     </row>
     <row r="31" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B31" s="4">
         <v>42898</v>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="32" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B32" s="4">
         <v>42915</v>
@@ -5490,7 +5490,7 @@
     </row>
     <row r="33" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B33" s="4">
         <v>42929</v>
@@ -5610,7 +5610,7 @@
     </row>
     <row r="34" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B34" s="4">
         <v>42943</v>
@@ -5742,7 +5742,7 @@
     </row>
     <row r="35" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B35" s="4">
         <v>42957</v>
@@ -5880,7 +5880,7 @@
     </row>
     <row r="36" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B36" s="4">
         <v>42975</v>
@@ -6009,7 +6009,7 @@
     </row>
     <row r="37" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B37" s="4">
         <v>42993</v>
@@ -6119,7 +6119,7 @@
     </row>
     <row r="38" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B38" s="4">
         <v>43028</v>
@@ -6163,10 +6163,10 @@
     </row>
     <row r="39" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D39" s="5">
         <v>6</v>
@@ -6180,10 +6180,10 @@
     </row>
     <row r="40" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D40" s="5">
         <v>6</v>
@@ -6197,10 +6197,10 @@
     </row>
     <row r="41" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D41" s="5">
         <v>6</v>
@@ -6214,10 +6214,10 @@
     </row>
     <row r="42" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D42" s="5">
         <v>6</v>
@@ -6231,10 +6231,10 @@
     </row>
     <row r="43" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D43" s="5">
         <v>6</v>
@@ -6248,10 +6248,10 @@
     </row>
     <row r="44" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D44" s="5">
         <v>6</v>
@@ -6265,10 +6265,10 @@
     </row>
     <row r="45" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D45" s="5">
         <v>6</v>
@@ -6282,10 +6282,10 @@
     </row>
     <row r="46" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D46" s="5">
         <v>6</v>
@@ -6299,10 +6299,10 @@
     </row>
     <row r="47" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D47" s="5">
         <v>13</v>
@@ -6316,10 +6316,10 @@
     </row>
     <row r="48" spans="1:74" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D48" s="5">
         <v>13</v>
@@ -6333,10 +6333,10 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D49" s="5">
         <v>13</v>
@@ -6350,10 +6350,10 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D50" s="5">
         <v>13</v>
@@ -6367,10 +6367,10 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D51" s="5">
         <v>13</v>
@@ -6384,10 +6384,10 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D52" s="5">
         <v>13</v>
@@ -6401,10 +6401,10 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D53" s="5">
         <v>13</v>
@@ -6418,10 +6418,10 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D54" s="5">
         <v>13</v>
@@ -6435,10 +6435,10 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D55" s="5">
         <v>7</v>
@@ -6452,10 +6452,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D56" s="5">
         <v>7</v>
@@ -6469,10 +6469,10 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D57" s="5">
         <v>7</v>
@@ -6486,10 +6486,10 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D58" s="5">
         <v>7</v>
@@ -6503,10 +6503,10 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D59" s="5">
         <v>7</v>
@@ -6520,10 +6520,10 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D60" s="5">
         <v>7</v>
@@ -6537,10 +6537,10 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D61" s="5">
         <v>7</v>
@@ -6554,10 +6554,10 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62" s="5">
         <v>7</v>
@@ -6571,10 +6571,10 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="5">
@@ -6584,10 +6584,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D64" s="5"/>
       <c r="E64" s="5">
@@ -6597,10 +6597,10 @@
     </row>
     <row r="65" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E65" s="5">
         <v>52</v>
@@ -6608,10 +6608,10 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E66" s="5">
         <v>52</v>
@@ -6619,10 +6619,10 @@
     </row>
     <row r="67" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E67" s="5">
         <v>42</v>
@@ -6630,10 +6630,10 @@
     </row>
     <row r="68" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E68" s="5">
         <v>42</v>
@@ -6641,10 +6641,10 @@
     </row>
     <row r="69" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E69" s="5">
         <v>56</v>
@@ -6652,10 +6652,10 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E70" s="5">
         <v>55</v>
@@ -6663,10 +6663,10 @@
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E71" s="5">
         <v>39</v>
@@ -6674,10 +6674,10 @@
     </row>
     <row r="72" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A72" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E72" s="5">
         <v>40</v>
@@ -6685,10 +6685,10 @@
     </row>
     <row r="73" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A73" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E73" s="5">
         <v>58</v>
@@ -6696,10 +6696,10 @@
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A74" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E74" s="5">
         <v>60</v>
@@ -6707,10 +6707,10 @@
     </row>
     <row r="75" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A75" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E75" s="5">
         <v>38</v>
@@ -6718,10 +6718,10 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A76" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E76" s="5">
         <v>41</v>
@@ -6729,10 +6729,10 @@
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A77" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E77" s="5">
         <v>55</v>
@@ -6740,10 +6740,10 @@
     </row>
     <row r="78" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A78" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E78" s="5">
         <v>58</v>
@@ -6751,10 +6751,10 @@
     </row>
     <row r="79" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A79" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D79" s="5">
         <v>22</v>
@@ -6771,10 +6771,10 @@
     </row>
     <row r="80" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A80" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D80" s="5">
         <v>20</v>
@@ -6791,10 +6791,10 @@
     </row>
     <row r="81" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A81" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D81" s="5">
         <v>14</v>
@@ -6811,10 +6811,10 @@
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A82" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D82" s="5">
         <v>16</v>
@@ -6831,10 +6831,10 @@
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A83" s="7" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D83" s="5">
         <v>11</v>
@@ -6851,10 +6851,10 @@
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A84" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D84" s="5">
         <v>16</v>
@@ -6871,10 +6871,10 @@
     </row>
     <row r="85" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A85" s="6" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D85" s="5">
         <v>31</v>
@@ -6891,10 +6891,10 @@
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A86" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D86" s="5">
         <v>25</v>
@@ -6911,10 +6911,10 @@
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A87" s="6" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D87" s="5">
         <v>9</v>
@@ -6931,10 +6931,10 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A88" s="7" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D88" s="5">
         <v>9</v>
@@ -6951,10 +6951,10 @@
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A89" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D89" s="5">
         <v>9</v>
@@ -6971,10 +6971,10 @@
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A90" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D90" s="5">
         <v>11</v>
@@ -6991,10 +6991,10 @@
     </row>
     <row r="91" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A91" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D91" s="5">
         <v>22</v>
@@ -7011,10 +7011,10 @@
     </row>
     <row r="92" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A92" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D92" s="5">
         <v>20</v>
@@ -7031,10 +7031,10 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A93" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D93" s="5">
         <v>14</v>
@@ -7051,10 +7051,10 @@
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A94" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D94" s="5">
         <v>16</v>
@@ -7071,10 +7071,10 @@
     </row>
     <row r="95" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A95" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D95" s="5">
         <v>11</v>
@@ -7091,10 +7091,10 @@
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A96" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D96" s="5">
         <v>16</v>
@@ -7111,10 +7111,10 @@
     </row>
     <row r="97" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A97" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D97" s="5">
         <v>31</v>
@@ -7131,10 +7131,10 @@
     </row>
     <row r="98" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A98" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D98" s="5">
         <v>25</v>
@@ -7151,10 +7151,10 @@
     </row>
     <row r="99" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A99" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D99" s="5">
         <v>9</v>
@@ -7171,10 +7171,10 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A100" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D100" s="5">
         <v>9</v>
@@ -7191,10 +7191,10 @@
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A101" s="7" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D101" s="5">
         <v>9</v>
@@ -7211,10 +7211,10 @@
     </row>
     <row r="102" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A102" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D102" s="5">
         <v>11</v>
@@ -7231,10 +7231,10 @@
     </row>
     <row r="103" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A103" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D103" s="5">
         <v>22</v>
@@ -7251,10 +7251,10 @@
     </row>
     <row r="104" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A104" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D104" s="5">
         <v>20</v>
@@ -7271,10 +7271,10 @@
     </row>
     <row r="105" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A105" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D105" s="5">
         <v>14</v>
@@ -7291,10 +7291,10 @@
     </row>
     <row r="106" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A106" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D106" s="5">
         <v>16</v>
@@ -7311,10 +7311,10 @@
     </row>
     <row r="107" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A107" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D107" s="5">
         <v>11</v>
@@ -7331,10 +7331,10 @@
     </row>
     <row r="108" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A108" s="7" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D108" s="5">
         <v>16</v>
@@ -7351,10 +7351,10 @@
     </row>
     <row r="109" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A109" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D109" s="5">
         <v>31</v>
@@ -7371,10 +7371,10 @@
     </row>
     <row r="110" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A110" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D110" s="5">
         <v>25</v>
@@ -7391,10 +7391,10 @@
     </row>
     <row r="111" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A111" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D111" s="5">
         <v>9</v>
@@ -7411,10 +7411,10 @@
     </row>
     <row r="112" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A112" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D112" s="5">
         <v>9</v>
@@ -7431,10 +7431,10 @@
     </row>
     <row r="113" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A113" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D113" s="5">
         <v>9</v>
@@ -7451,10 +7451,10 @@
     </row>
     <row r="114" spans="1:21" x14ac:dyDescent="0.55000000000000004">
       <c r="A114" s="7" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D114" s="5">
         <v>11</v>
@@ -7495,10 +7495,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -9228,7 +9228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CFA9B49-2792-48D3-82BC-E629331E59DB}">
   <dimension ref="A1:M576"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A290" workbookViewId="0">
+    <sheetView topLeftCell="A290" workbookViewId="0">
       <selection activeCell="C300" sqref="C300:F404"/>
     </sheetView>
   </sheetViews>
@@ -9251,25 +9251,25 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" t="s">
+        <v>100</v>
+      </c>
+      <c r="E1" t="s">
         <v>98</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>101</v>
       </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>102</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>103</v>
       </c>
-      <c r="H1" t="s">
+      <c r="M1" t="s">
         <v>104</v>
-      </c>
-      <c r="M1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -9281,7 +9281,7 @@
       </c>
       <c r="J2" s="4"/>
       <c r="M2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -10660,7 +10660,7 @@
         <v>950.91666999999995</v>
       </c>
       <c r="H122" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J122" s="4"/>
     </row>
@@ -10687,7 +10687,7 @@
         <v>942</v>
       </c>
       <c r="H123" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J123" s="4"/>
     </row>
@@ -11065,7 +11065,7 @@
         <v>1134.4166700000001</v>
       </c>
       <c r="H137" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J137" s="4"/>
     </row>
@@ -19064,16 +19064,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D1" t="s">
         <v>107</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>109</v>
-      </c>
-      <c r="F1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">

</xml_diff>

<commit_message>
updated sutherland met file and new growth stage structure
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D90227-522F-437F-9D07-02DC62AD15A6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A650005-DCEC-4ECC-8A1C-5CDCF5F80CF6}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" firstSheet="2" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1835,10 +1835,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
   <dimension ref="A1:BZ249"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A233" activePane="bottomLeft"/>
-      <selection activeCell="C1" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A236" sqref="A236:E249"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <pane ySplit="576" topLeftCell="A23" activePane="bottomLeft"/>
+      <selection activeCell="X1" sqref="X1"/>
+      <selection pane="bottomLeft" activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -5222,6 +5222,10 @@
       <c r="L27">
         <v>33.666666669999998</v>
       </c>
+      <c r="M27">
+        <f t="shared" ref="M23:M38" si="5">L27*J27</f>
+        <v>1088.5555555511112</v>
+      </c>
       <c r="N27">
         <v>4.2919714000000004</v>
       </c>
@@ -5362,6 +5366,10 @@
       <c r="L28">
         <v>24.777777780000001</v>
       </c>
+      <c r="M28">
+        <f t="shared" si="5"/>
+        <v>718.55555562000006</v>
+      </c>
       <c r="N28">
         <v>3.6318666670000002</v>
       </c>
@@ -5496,6 +5504,10 @@
       <c r="L29">
         <v>33</v>
       </c>
+      <c r="M29">
+        <f t="shared" si="5"/>
+        <v>847.00000011000009</v>
+      </c>
       <c r="R29">
         <v>26.616666670000001</v>
       </c>
@@ -5513,6 +5525,10 @@
       </c>
       <c r="W29">
         <v>125.7166667</v>
+      </c>
+      <c r="X29">
+        <f>W29/M29</f>
+        <v>0.14842581662771329</v>
       </c>
       <c r="Y29">
         <v>338.16666670000001</v>
@@ -6084,6 +6100,10 @@
       <c r="L35">
         <v>21.444444440000002</v>
       </c>
+      <c r="M35">
+        <f t="shared" si="5"/>
+        <v>671.92592571518526</v>
+      </c>
       <c r="N35">
         <v>3.7738070669999999</v>
       </c>
@@ -6224,6 +6244,10 @@
       <c r="L36">
         <v>28.555555559999998</v>
       </c>
+      <c r="M36">
+        <f t="shared" si="5"/>
+        <v>951.85185190481479</v>
+      </c>
       <c r="N36">
         <v>4.0960799999999997</v>
       </c>
@@ -6355,6 +6379,10 @@
       <c r="L37">
         <v>39</v>
       </c>
+      <c r="M37">
+        <f t="shared" si="5"/>
+        <v>1014</v>
+      </c>
       <c r="R37">
         <v>72.08</v>
       </c>
@@ -6372,6 +6400,10 @@
       </c>
       <c r="W37">
         <v>118.78</v>
+      </c>
+      <c r="X37">
+        <f>W37/M37</f>
+        <v>0.11714003944773176</v>
       </c>
       <c r="Y37">
         <v>282.03333329999998</v>
@@ -9382,7 +9414,7 @@
         <v>0.74</v>
       </c>
       <c r="Q193" s="9">
-        <f t="shared" ref="Q193:Q233" si="5">N193*1000000/R193</f>
+        <f t="shared" ref="Q193:Q233" si="6">N193*1000000/R193</f>
         <v>38845.144356955381</v>
       </c>
       <c r="R193">
@@ -9422,7 +9454,7 @@
         <v>1.29</v>
       </c>
       <c r="Q194" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25313.97174254317</v>
       </c>
       <c r="R194">
@@ -9462,7 +9494,7 @@
         <v>2.3199999999999998</v>
       </c>
       <c r="Q195" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>26429.710640236957</v>
       </c>
       <c r="R195">
@@ -9502,7 +9534,7 @@
         <v>3.81</v>
       </c>
       <c r="Q196" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31127.450980392154</v>
       </c>
       <c r="R196">
@@ -9542,7 +9574,7 @@
         <v>5.96</v>
       </c>
       <c r="Q197" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33927.249957306318</v>
       </c>
       <c r="R197">
@@ -9594,7 +9626,7 @@
         <v>5.61</v>
       </c>
       <c r="Q198" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>33850.238339467811</v>
       </c>
       <c r="R198">
@@ -9646,7 +9678,7 @@
         <v>4.4400000000000004</v>
       </c>
       <c r="Q199" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>30498.694875669731</v>
       </c>
       <c r="R199">
@@ -9698,7 +9730,7 @@
         <v>1.68</v>
       </c>
       <c r="Q200" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27568.099770265835</v>
       </c>
       <c r="R200">
@@ -9758,6 +9790,10 @@
       </c>
       <c r="W201">
         <v>109.33</v>
+      </c>
+      <c r="X201" t="e">
+        <f>W201/M201</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y201">
         <v>370.94</v>
@@ -9795,7 +9831,7 @@
         <v>0.12</v>
       </c>
       <c r="Q203" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21126.760563380281</v>
       </c>
       <c r="R203">
@@ -9835,7 +9871,7 @@
         <v>0.31</v>
       </c>
       <c r="Q204" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35267.349260523326</v>
       </c>
       <c r="R204">
@@ -9875,7 +9911,7 @@
         <v>0.99</v>
       </c>
       <c r="Q205" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25621.118012422361</v>
       </c>
       <c r="R205">
@@ -9915,7 +9951,7 @@
         <v>1.48</v>
       </c>
       <c r="Q206" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29365.079365079368</v>
       </c>
       <c r="R206">
@@ -9955,7 +9991,7 @@
         <v>3.02</v>
       </c>
       <c r="Q207" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>29320.388349514564</v>
       </c>
       <c r="R207">
@@ -10007,7 +10043,7 @@
         <v>6.93</v>
       </c>
       <c r="Q208" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>50170.129588069212</v>
       </c>
       <c r="R208">
@@ -10059,7 +10095,7 @@
         <v>4.17</v>
       </c>
       <c r="Q209" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>31117.080814864563</v>
       </c>
       <c r="R209">
@@ -10111,7 +10147,7 @@
         <v>4.97</v>
       </c>
       <c r="Q210" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>39410.038854967883</v>
       </c>
       <c r="R210">
@@ -10163,7 +10199,7 @@
         <v>1.67</v>
       </c>
       <c r="Q211" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24598.615407276477</v>
       </c>
       <c r="R211">
@@ -10202,6 +10238,10 @@
       </c>
       <c r="W212">
         <v>99.48</v>
+      </c>
+      <c r="X212" t="e">
+        <f>W212/M212</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y212">
         <v>367.65</v>
@@ -10239,7 +10279,7 @@
         <v>0.12</v>
       </c>
       <c r="Q214" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>11583.011583011583</v>
       </c>
       <c r="R214">
@@ -10279,7 +10319,7 @@
         <v>0.74</v>
       </c>
       <c r="Q215" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27850.95972901769</v>
       </c>
       <c r="R215">
@@ -10319,7 +10359,7 @@
         <v>1.33</v>
       </c>
       <c r="Q216" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>23745.759685770397</v>
       </c>
       <c r="R216">
@@ -10390,7 +10430,7 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="Q218" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27430.762112499178</v>
       </c>
       <c r="R218">
@@ -10430,7 +10470,7 @@
         <v>7.22</v>
       </c>
       <c r="Q219" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42279.088832933179</v>
       </c>
       <c r="R219">
@@ -10482,7 +10522,7 @@
         <v>6</v>
       </c>
       <c r="Q220" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>35194.74425152511</v>
       </c>
       <c r="R220">
@@ -10534,7 +10574,7 @@
         <v>3.25</v>
       </c>
       <c r="Q221" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>20429.972340960521</v>
       </c>
       <c r="R221">
@@ -10586,7 +10626,7 @@
         <v>2.1</v>
       </c>
       <c r="Q222" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>27678.9244760775</v>
       </c>
       <c r="R222">
@@ -10625,6 +10665,10 @@
       </c>
       <c r="W223">
         <v>138.41</v>
+      </c>
+      <c r="X223" t="e">
+        <f>W223/M223</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y223">
         <v>462.61</v>
@@ -10662,7 +10706,7 @@
         <v>0.12</v>
       </c>
       <c r="Q225" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>17216.64275466284</v>
       </c>
       <c r="R225">
@@ -10702,7 +10746,7 @@
         <v>0.42</v>
       </c>
       <c r="Q226" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>25862.068965517243</v>
       </c>
       <c r="R226">
@@ -10773,7 +10817,7 @@
         <v>3.06</v>
       </c>
       <c r="Q228" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32387.806943268417</v>
       </c>
       <c r="R228">
@@ -10813,7 +10857,7 @@
         <v>5.91</v>
       </c>
       <c r="Q229" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>43475.062527585702</v>
       </c>
       <c r="R229">
@@ -10865,7 +10909,7 @@
         <v>7.32</v>
       </c>
       <c r="Q230" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>42620.087336244542</v>
       </c>
       <c r="R230">
@@ -10917,7 +10961,7 @@
         <v>4.9800000000000004</v>
       </c>
       <c r="Q231" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24619.339529365236</v>
       </c>
       <c r="R231">
@@ -10969,7 +11013,7 @@
         <v>4.49</v>
       </c>
       <c r="Q232" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40035.666518056176</v>
       </c>
       <c r="R232">
@@ -11009,7 +11053,7 @@
         <v>2.0299999999999998</v>
       </c>
       <c r="Q233" s="9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>53491.436100131745</v>
       </c>
       <c r="R233">
@@ -11048,6 +11092,10 @@
       </c>
       <c r="W234">
         <v>108.59</v>
+      </c>
+      <c r="X234" t="e">
+        <f>W234/M234</f>
+        <v>#DIV/0!</v>
       </c>
       <c r="Y234">
         <v>388.81</v>

</xml_diff>

<commit_message>
final version from Ames visit 2018
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69957711-C802-45BA-916B-40D008C0A395}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D21B3ACF-0C6F-4AD6-AA00-7529144A1B16}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="14" r:id="rId1"/>
@@ -1008,6 +1008,1480 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Observed!$Z$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Soybean.AboveGround.Wt</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Observed!$N$2:$N$234</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="232"/>
+                <c:pt idx="0">
+                  <c:v>0.18906666699999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.063767667</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.6299103330000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.5467477330000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.4898179999999996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.4933822670000003</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.3484526670000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.56501726699999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.333144933</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.870000133</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.6754084669999996</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.2218760670000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.4241513330000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.35698686699999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.95810446699999996</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1.6910712000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3.3258197329999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.2919714000000004</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3.6318666670000002</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.31231700000000001</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.89610920000000005</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3.1892269999999998</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.7738070669999999</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.0960799999999997</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>0.36252640515873402</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>1.65706142168406</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>2.4005498337359299</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>3.4464468005538702</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>4.6297213434540403</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5.1806062321228197</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5.1828298244372704</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>3.7833008217184299</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>2.2463942429173498</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>4.95254651856189E-2</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>1.8509991004558299</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>3.7213232395718499</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>5.5654898472796299</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>5.5681177291058104</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>5.1029017879703602</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>0.43436865139126002</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>0.44868050010612398</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>1.7156834008833699</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>2.2107359079836999</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>3.7524535319742398</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>4.3584835100415402</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>4.4146797521705201</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>3.64782340634128</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>3.0998494021568801</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>0.38039600157672898</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1.7981584612741099</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>2.5412425838142698</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>4.3573110704575502</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>4.6620240754404199</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>6.1475050283507997</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>3.9776832189530902</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>3.45724133051678</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>2.1673152144250398</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>0.59010097130555095</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>0.865826418298143</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>2.1045694822062</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>2.71019517076178</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>4.0585815502481299</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>3.5103245434055301</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>3.7322794853394501</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>2.5796905163787698</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>0.24532287571129699</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>1.96698976136811</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>3.9774810741972302</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>4.1717421845783704</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>3.4043602623838898</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>1.2348618845955499</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>2.3992699392924401</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>4.4933666527109004</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>6.89652239899518</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>7.4025800711743699</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>9.0776768892610402</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>8.6793227967343505</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>7.1780275277370702</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>5.12502616705045</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>4.8364559346870397</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>3.1582975716977102</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>0.53109953945990995</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>0.92121101109482895</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>4.33777737073477</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>5.1295399832530801</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>6.9137141511408799</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>6.4919667155118201</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>3.2030039773916599</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>6.2223937617751703</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>1.29</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>2.3199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>3.81</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>5.61</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>4.4400000000000004</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>1.68</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>0.31</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>0.99</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>1.48</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>3.02</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>6.93</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>4.17</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>1.67</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>0.12</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>0.74</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>1.33</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>4.1500000000000004</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>7.22</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>3.25</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>2.1</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>0.42</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>3.06</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>5.91</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>7.32</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>4.9800000000000004</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>2.0299999999999998</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Observed!$Q$2:$Q$234</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="232"/>
+                <c:pt idx="0">
+                  <c:v>25549.549594594591</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>36597.511475160842</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28900.113549450551</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24895.281227212148</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26139.052973774684</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24667.679467369173</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20837.10095400504</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32534.583506231364</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>22053.679619520262</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>26956.795229506322</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28080.531333333329</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>29404.110969086094</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>25290.981152460987</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>38626.581584072701</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22093.108384158866</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23411.230273346162</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>27807.857299331106</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>27164.949043826888</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>24385.309188606949</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>17914.933081819298</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>23205.244710987896</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32992.00344713821</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>27495.194297040794</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>26138.517819676141</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>34347.929212067291</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>37909.06206031816</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>41267.383030936362</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>37324.808003524799</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>40020.288634721081</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>35094.659940056139</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>32069.620549677846</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>31745.807010921511</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>34102.758793628491</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>45955.10799080845</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>23992.322456813821</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>38845.144356955381</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>25313.97174254317</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>26429.710640236957</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>31127.450980392154</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>33927.249957306318</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>33850.238339467811</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>30498.694875669731</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>27568.099770265835</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>21126.760563380281</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>35267.349260523326</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>25621.118012422361</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>29365.079365079368</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>29320.388349514564</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>50170.129588069212</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>31117.080814864563</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>39410.038854967883</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>24598.615407276477</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>11583.011583011583</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>27850.95972901769</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>23745.759685770397</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>27430.762112499178</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>42279.088832933179</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>35194.74425152511</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>20429.972340960521</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>27678.9244760775</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>25862.068965517243</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>32387.806943268417</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>43475.062527585702</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>42620.087336244542</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>24619.339529365236</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>40035.666518056176</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>53491.436100131745</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-667E-4EAE-9D25-E3F3B757E82C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="413476240"/>
+        <c:axId val="413474928"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="413476240"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413474928"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="413474928"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="413476240"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>944880</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>131445</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D03DC901-49D1-4580-8B2B-A4A6E82CBC00}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1331,10 +2805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
   <dimension ref="A1:BZ249"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="576" topLeftCell="A166" activePane="bottomLeft"/>
-      <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="Q179" sqref="Q179"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -10601,7 +12073,7 @@
       </c>
       <c r="Z224" s="11"/>
     </row>
-    <row r="225" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:36" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" t="s">
         <v>228</v>
       </c>
@@ -11084,6 +12556,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -23343,7 +24816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C38AC6CC-44CB-4FCE-B6C5-EB62C8EDED80}">
   <dimension ref="A1:AF15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>

</xml_diff>

<commit_message>
Added more Northern Aust Data
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{266756FD-8635-40FE-AD01-4DC3349E0803}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DCB818-5AF9-4829-8389-B61E1D629DA4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="309">
   <si>
     <t>SimulationName</t>
   </si>
@@ -927,15 +927,49 @@
   <si>
     <t>seeds_m2</t>
   </si>
+  <si>
+    <t>Murumbidgee2003SowDec09CvDjakal_furrow</t>
+  </si>
+  <si>
+    <t>Katherine1988WaterIrrigated</t>
+  </si>
+  <si>
+    <t>Katherine1988WaterRainfed</t>
+  </si>
+  <si>
+    <t>Katherine1989SowJan10</t>
+  </si>
+  <si>
+    <t>Katherine1989SowFeb07</t>
+  </si>
+  <si>
+    <t>Kununurra1980WaterWet</t>
+  </si>
+  <si>
+    <t>Kununurra1980WaterWetDry</t>
+  </si>
+  <si>
+    <t>Kununurra1980WaterDry</t>
+  </si>
+  <si>
+    <t>Kununurra1979WaterWet</t>
+  </si>
+  <si>
+    <t>Kununurra1979WaterDry</t>
+  </si>
+  <si>
+    <t>Kununurra1979WaterWetDry</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -956,6 +990,22 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="MS Sans Serif"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1001,10 +1051,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1030,9 +1081,13 @@
     <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_obs" xfId="1" xr:uid="{38A366B4-CF13-4E66-BB52-25551BEBB11D}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1368,14 +1423,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
-  <dimension ref="A1:CH249"/>
+  <dimension ref="A1:CH261"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="E242" workbookViewId="0">
+      <selection activeCell="H260" sqref="H260"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="43.3125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.20703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.26171875" customWidth="1"/>
     <col min="4" max="4" width="31.9453125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="31.9453125" customWidth="1"/>
@@ -11416,7 +11473,7 @@
       </c>
       <c r="Z224" s="11"/>
     </row>
-    <row r="225" spans="1:36" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:39" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A225" t="s">
         <v>228</v>
       </c>
@@ -11456,7 +11513,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="226" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A226" t="s">
         <v>228</v>
       </c>
@@ -11496,7 +11553,7 @@
         <v>0.26</v>
       </c>
     </row>
-    <row r="227" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A227" t="s">
         <v>228</v>
       </c>
@@ -11527,7 +11584,7 @@
         <v>1.1100000000000001</v>
       </c>
     </row>
-    <row r="228" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A228" t="s">
         <v>228</v>
       </c>
@@ -11567,7 +11624,7 @@
         <v>2.25</v>
       </c>
     </row>
-    <row r="229" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A229" t="s">
         <v>228</v>
       </c>
@@ -11619,7 +11676,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="230" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A230" t="s">
         <v>228</v>
       </c>
@@ -11671,7 +11728,7 @@
         <v>2.27</v>
       </c>
     </row>
-    <row r="231" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
         <v>228</v>
       </c>
@@ -11723,7 +11780,7 @@
         <v>7.03</v>
       </c>
     </row>
-    <row r="232" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A232" t="s">
         <v>228</v>
       </c>
@@ -11763,7 +11820,7 @@
         <v>15.98</v>
       </c>
     </row>
-    <row r="233" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A233" t="s">
         <v>228</v>
       </c>
@@ -11794,7 +11851,7 @@
         <v>751.68999999999994</v>
       </c>
     </row>
-    <row r="234" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A234" t="s">
         <v>228</v>
       </c>
@@ -11829,7 +11886,7 @@
         <v>709.66000000000008</v>
       </c>
     </row>
-    <row r="235" spans="1:36" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A235" t="s">
         <v>228</v>
       </c>
@@ -11841,61 +11898,589 @@
         <v>365.9</v>
       </c>
     </row>
-    <row r="236" spans="1:36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B236" s="4"/>
-      <c r="C236" s="12"/>
-    </row>
-    <row r="237" spans="1:36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B237" s="4"/>
-      <c r="C237" s="12"/>
-    </row>
-    <row r="238" spans="1:36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B238" s="4"/>
-      <c r="C238" s="12"/>
-    </row>
-    <row r="239" spans="1:36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B239" s="4"/>
-      <c r="C239" s="12"/>
-    </row>
-    <row r="240" spans="1:36" x14ac:dyDescent="0.55000000000000004">
-      <c r="B240" s="4"/>
-      <c r="C240" s="12"/>
-    </row>
-    <row r="241" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B241" s="4"/>
-      <c r="C241" s="12"/>
-    </row>
-    <row r="242" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B242" s="4"/>
-      <c r="C242" s="12"/>
-    </row>
-    <row r="243" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B243" s="4"/>
-      <c r="C243" s="12"/>
-    </row>
-    <row r="244" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B244" s="4"/>
-      <c r="C244" s="12"/>
-    </row>
-    <row r="245" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B245" s="4"/>
-      <c r="C245" s="12"/>
-    </row>
-    <row r="246" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B246" s="4"/>
-      <c r="C246" s="12"/>
-    </row>
-    <row r="247" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B247" s="4"/>
-      <c r="C247" s="12"/>
-    </row>
-    <row r="248" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B248" s="4"/>
-      <c r="C248" s="12"/>
-    </row>
-    <row r="249" spans="2:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="B249" s="4"/>
-      <c r="C249" s="12"/>
+    <row r="236" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A236" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B236" s="4">
+        <f>DATE(1988,1,5)+C236</f>
+        <v>32169.434782608696</v>
+      </c>
+      <c r="C236" s="15">
+        <v>22.434782608695599</v>
+      </c>
+      <c r="Y236">
+        <v>0</v>
+      </c>
+      <c r="Z236" s="17">
+        <v>51.3374903903647</v>
+      </c>
+      <c r="AM236" s="17">
+        <v>1.7214661406969001</v>
+      </c>
+    </row>
+    <row r="237" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A237" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B237" s="4">
+        <f t="shared" ref="B237:B249" si="14">DATE(1988,1,5)+C237</f>
+        <v>32179.521739130436</v>
+      </c>
+      <c r="C237" s="15">
+        <v>32.521739130434703</v>
+      </c>
+      <c r="Y237">
+        <v>0</v>
+      </c>
+      <c r="Z237" s="17">
+        <v>159.547621081404</v>
+      </c>
+      <c r="AM237" s="17">
+        <v>4.9395792241945902</v>
+      </c>
+    </row>
+    <row r="238" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A238" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B238" s="4">
+        <f t="shared" si="14"/>
+        <v>32190.478260869564</v>
+      </c>
+      <c r="C238" s="15">
+        <v>43.478260869565197</v>
+      </c>
+      <c r="Y238">
+        <v>0</v>
+      </c>
+      <c r="Z238" s="17">
+        <v>331.39147518578602</v>
+      </c>
+      <c r="AM238" s="17">
+        <v>8.4912393162393105</v>
+      </c>
+    </row>
+    <row r="239" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A239" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B239" s="4">
+        <f t="shared" si="14"/>
+        <v>32200.391304347824</v>
+      </c>
+      <c r="C239" s="15">
+        <v>53.391304347826001</v>
+      </c>
+      <c r="Y239" s="17">
+        <v>5.8098573503032096</v>
+      </c>
+      <c r="Z239" s="17">
+        <v>536.26582386606299</v>
+      </c>
+      <c r="AM239" s="17">
+        <v>10.3629684418145</v>
+      </c>
+    </row>
+    <row r="240" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A240" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B240" s="4">
+        <f t="shared" si="14"/>
+        <v>32212.391304347828</v>
+      </c>
+      <c r="C240" s="15">
+        <v>65.391304347826093</v>
+      </c>
+      <c r="Y240" s="17">
+        <v>71.542837618518604</v>
+      </c>
+      <c r="Z240" s="17">
+        <v>854.25403604680901</v>
+      </c>
+      <c r="AM240" s="17">
+        <v>17.480785667324099</v>
+      </c>
+    </row>
+    <row r="241" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A241" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B241" s="4">
+        <f t="shared" si="14"/>
+        <v>32227.521739130436</v>
+      </c>
+      <c r="C241" s="15">
+        <v>80.521739130434796</v>
+      </c>
+      <c r="Y241" s="17">
+        <v>285.72443837020501</v>
+      </c>
+      <c r="Z241" s="17">
+        <v>863.327581788673</v>
+      </c>
+      <c r="AM241" s="17">
+        <v>21.431229454306301</v>
+      </c>
+    </row>
+    <row r="242" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A242" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B242" s="4">
+        <f t="shared" si="14"/>
+        <v>32237.434782608696</v>
+      </c>
+      <c r="C242" s="15">
+        <v>90.434782608695599</v>
+      </c>
+      <c r="D242" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y242" s="17">
+        <v>476.35910139232902</v>
+      </c>
+      <c r="Z242" s="17">
+        <v>1084.7048774237601</v>
+      </c>
+    </row>
+    <row r="243" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A243" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B243" s="4">
+        <f t="shared" si="14"/>
+        <v>32169.434782608696</v>
+      </c>
+      <c r="C243" s="15">
+        <v>22.434782608695599</v>
+      </c>
+      <c r="Y243" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z243" s="17">
+        <v>37.192107286238901</v>
+      </c>
+      <c r="AM243" s="17">
+        <v>1.5195430637738201</v>
+      </c>
+    </row>
+    <row r="244" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A244" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B244" s="4">
+        <f t="shared" si="14"/>
+        <v>32179.521739130436</v>
+      </c>
+      <c r="C244" s="15">
+        <v>32.521739130434703</v>
+      </c>
+      <c r="Y244" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z244" s="17">
+        <v>140.687110275903</v>
+      </c>
+      <c r="AM244" s="17">
+        <v>3.45834976988822</v>
+      </c>
+    </row>
+    <row r="245" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A245" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B245" s="4">
+        <f t="shared" si="14"/>
+        <v>32190.652173913044</v>
+      </c>
+      <c r="C245" s="15">
+        <v>43.652173913043399</v>
+      </c>
+      <c r="Y245" s="15">
+        <v>0</v>
+      </c>
+      <c r="Z245" s="17">
+        <v>279.52097035961299</v>
+      </c>
+    </row>
+    <row r="246" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A246" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B246" s="4">
+        <f t="shared" si="14"/>
+        <v>32200.391304347824</v>
+      </c>
+      <c r="C246" s="15">
+        <v>53.391304347826001</v>
+      </c>
+      <c r="T246" s="17"/>
+      <c r="U246" s="17"/>
+      <c r="Y246" s="17">
+        <v>3.4604937217049998</v>
+      </c>
+      <c r="Z246" s="17">
+        <v>418.38763133168101</v>
+      </c>
+    </row>
+    <row r="247" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A247" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B247" s="4">
+        <f t="shared" si="14"/>
+        <v>32212.391304347828</v>
+      </c>
+      <c r="C247" s="15">
+        <v>65.391304347826093</v>
+      </c>
+      <c r="T247" s="17"/>
+      <c r="U247" s="17"/>
+      <c r="Y247" s="17">
+        <v>26.745024344409298</v>
+      </c>
+      <c r="Z247" s="17">
+        <v>618.49765097804698</v>
+      </c>
+    </row>
+    <row r="248" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A248" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B248" s="4">
+        <f t="shared" si="14"/>
+        <v>32227.347826086956</v>
+      </c>
+      <c r="C248" s="15">
+        <v>80.347826086956502</v>
+      </c>
+      <c r="T248" s="17"/>
+      <c r="U248" s="17"/>
+      <c r="Y248" s="17">
+        <v>115.988041342786</v>
+      </c>
+      <c r="Z248" s="17">
+        <v>507.33954044588597</v>
+      </c>
+      <c r="AM248" s="17">
+        <v>8.8398586456278707</v>
+      </c>
+    </row>
+    <row r="249" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A249" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B249" s="4">
+        <f t="shared" si="14"/>
+        <v>32231.17391304348</v>
+      </c>
+      <c r="C249" s="15">
+        <v>84.173913043478194</v>
+      </c>
+      <c r="D249" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T249" s="17"/>
+      <c r="U249" s="17"/>
+      <c r="Y249" s="17">
+        <v>111.174510976338</v>
+      </c>
+      <c r="Z249" s="17">
+        <v>438.87998633296297</v>
+      </c>
+    </row>
+    <row r="250" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A250" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B250" s="4"/>
+      <c r="C250" s="15"/>
+      <c r="D250" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T250" s="17"/>
+      <c r="U250" s="17"/>
+      <c r="Y250" s="19">
+        <v>309.87744905589255</v>
+      </c>
+      <c r="Z250" s="19">
+        <v>556.15939553762939</v>
+      </c>
+    </row>
+    <row r="251" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A251" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B251" s="4"/>
+      <c r="C251" s="15"/>
+      <c r="D251" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="T251" s="17"/>
+      <c r="U251" s="17"/>
+      <c r="Y251" s="19">
+        <v>326.21240395819899</v>
+      </c>
+      <c r="Z251" s="19">
+        <v>655.85501195381346</v>
+      </c>
+    </row>
+    <row r="252" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B252" s="4"/>
+      <c r="C252" s="15">
+        <v>31</v>
+      </c>
+      <c r="G252" s="17">
+        <v>44</v>
+      </c>
+      <c r="H252" s="15">
+        <v>127</v>
+      </c>
+      <c r="T252" s="15">
+        <v>1710.9930320916199</v>
+      </c>
+      <c r="U252" s="15">
+        <v>1531.56588669085</v>
+      </c>
+      <c r="Y252" s="17">
+        <v>368</v>
+      </c>
+      <c r="Z252">
+        <f>6.9*100</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="253" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A253" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B253" s="4"/>
+      <c r="C253" s="15">
+        <v>57</v>
+      </c>
+      <c r="G253" s="17">
+        <v>44</v>
+      </c>
+      <c r="H253" s="15">
+        <v>127</v>
+      </c>
+      <c r="T253" s="15">
+        <v>11842.443955304399</v>
+      </c>
+      <c r="U253" s="15">
+        <v>12200.7935283973</v>
+      </c>
+      <c r="Y253" s="17">
+        <v>368</v>
+      </c>
+      <c r="Z253">
+        <f t="shared" ref="Z253:Z255" si="15">6.9*100</f>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="254" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B254" s="4"/>
+      <c r="C254" s="15">
+        <v>71</v>
+      </c>
+      <c r="G254" s="17">
+        <v>44</v>
+      </c>
+      <c r="H254" s="15">
+        <v>127</v>
+      </c>
+      <c r="T254" s="15">
+        <v>17889.971539529197</v>
+      </c>
+      <c r="U254" s="15">
+        <v>25763.063075693597</v>
+      </c>
+      <c r="Y254" s="17">
+        <v>368</v>
+      </c>
+      <c r="Z254">
+        <f t="shared" si="15"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="255" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A255" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="B255" s="4"/>
+      <c r="C255" s="15">
+        <v>128</v>
+      </c>
+      <c r="D255" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G255" s="17">
+        <v>44</v>
+      </c>
+      <c r="H255" s="15">
+        <v>127</v>
+      </c>
+      <c r="T255" s="15">
+        <v>13451.484010262498</v>
+      </c>
+      <c r="U255" s="15">
+        <v>12736.803734911</v>
+      </c>
+      <c r="Y255" s="17">
+        <v>368</v>
+      </c>
+      <c r="Z255">
+        <f t="shared" si="15"/>
+        <v>690</v>
+      </c>
+    </row>
+    <row r="256" spans="1:39" x14ac:dyDescent="0.55000000000000004">
+      <c r="A256" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B256" s="4">
+        <f>DATE(1980,4,1)+C256</f>
+        <v>29393</v>
+      </c>
+      <c r="C256" s="15">
+        <v>81</v>
+      </c>
+      <c r="D256" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G256" s="17">
+        <v>25</v>
+      </c>
+      <c r="H256" s="15">
+        <v>81</v>
+      </c>
+      <c r="Y256" s="19">
+        <v>280</v>
+      </c>
+      <c r="Z256" s="20">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="257" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A257" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B257" s="4">
+        <f t="shared" ref="B257:B259" si="16">DATE(1980,4,1)+C257</f>
+        <v>29393</v>
+      </c>
+      <c r="C257" s="15">
+        <v>81</v>
+      </c>
+      <c r="D257" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G257" s="17"/>
+      <c r="H257" s="15"/>
+      <c r="Y257" s="19">
+        <v>64</v>
+      </c>
+      <c r="Z257" s="19">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="258" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A258" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B258" s="4">
+        <f t="shared" si="16"/>
+        <v>29393</v>
+      </c>
+      <c r="C258" s="15">
+        <v>81</v>
+      </c>
+      <c r="D258" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G258" s="17"/>
+      <c r="H258" s="15"/>
+      <c r="Y258" s="19">
+        <v>120</v>
+      </c>
+      <c r="Z258" s="20">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="259" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A259" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="B259" s="4">
+        <f>DATE(1979,4,10)+C259</f>
+        <v>29042</v>
+      </c>
+      <c r="C259" s="15">
+        <v>87</v>
+      </c>
+      <c r="D259" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="H259" s="15">
+        <v>87</v>
+      </c>
+      <c r="Y259" s="19">
+        <v>111</v>
+      </c>
+      <c r="Z259" s="19">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="260" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A260" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="B260" s="4">
+        <f t="shared" ref="B260:B261" si="17">DATE(1979,4,10)+C260</f>
+        <v>29042</v>
+      </c>
+      <c r="C260" s="15">
+        <v>87</v>
+      </c>
+      <c r="D260" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y260" s="19">
+        <v>33</v>
+      </c>
+      <c r="Z260" s="19">
+        <v>61</v>
+      </c>
+      <c r="AA260" s="21"/>
+    </row>
+    <row r="261" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A261" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="B261" s="4">
+        <f t="shared" si="17"/>
+        <v>29042</v>
+      </c>
+      <c r="C261" s="15">
+        <v>87</v>
+      </c>
+      <c r="D261" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="Y261" s="19">
+        <v>77</v>
+      </c>
+      <c r="Z261" s="19">
+        <v>136</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fixed NT data and added coleambally
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\APSIMX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30DCB818-5AF9-4829-8389-B61E1D629DA4}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{352887E9-FBAE-4C56-AE17-C1F94D65FC74}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="138" windowWidth="15420" windowHeight="9300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -928,9 +928,6 @@
     <t>seeds_m2</t>
   </si>
   <si>
-    <t>Murumbidgee2003SowDec09CvDjakal_furrow</t>
-  </si>
-  <si>
     <t>Katherine1988WaterIrrigated</t>
   </si>
   <si>
@@ -959,6 +956,9 @@
   </si>
   <si>
     <t>Kununurra1979WaterWetDry</t>
+  </si>
+  <si>
+    <t>ColeamballySowDec09</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1055,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1084,6 +1084,8 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1425,8 +1427,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B61A777-7FB3-4D85-8052-DDB9477BDE84}">
   <dimension ref="A1:CH261"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E242" workbookViewId="0">
-      <selection activeCell="H260" sqref="H260"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="8364" ySplit="576" topLeftCell="AA244" activePane="bottomRight"/>
+      <selection sqref="A1:XFD1"/>
+      <selection pane="topRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A261" sqref="A261"/>
+      <selection pane="bottomRight" activeCell="AC252" sqref="AB252:AC262"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -11900,7 +11906,7 @@
     </row>
     <row r="236" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A236" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B236" s="4">
         <f>DATE(1988,1,5)+C236</f>
@@ -11921,7 +11927,7 @@
     </row>
     <row r="237" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A237" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B237" s="4">
         <f t="shared" ref="B237:B249" si="14">DATE(1988,1,5)+C237</f>
@@ -11942,7 +11948,7 @@
     </row>
     <row r="238" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A238" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B238" s="4">
         <f t="shared" si="14"/>
@@ -11963,7 +11969,7 @@
     </row>
     <row r="239" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A239" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B239" s="4">
         <f t="shared" si="14"/>
@@ -11984,7 +11990,7 @@
     </row>
     <row r="240" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A240" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B240" s="4">
         <f t="shared" si="14"/>
@@ -12005,7 +12011,7 @@
     </row>
     <row r="241" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A241" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B241" s="4">
         <f t="shared" si="14"/>
@@ -12026,7 +12032,7 @@
     </row>
     <row r="242" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A242" s="8" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B242" s="4">
         <f t="shared" si="14"/>
@@ -12047,7 +12053,7 @@
     </row>
     <row r="243" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A243" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B243" s="4">
         <f t="shared" si="14"/>
@@ -12068,7 +12074,7 @@
     </row>
     <row r="244" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A244" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B244" s="4">
         <f t="shared" si="14"/>
@@ -12089,7 +12095,7 @@
     </row>
     <row r="245" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A245" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B245" s="4">
         <f t="shared" si="14"/>
@@ -12107,7 +12113,7 @@
     </row>
     <row r="246" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A246" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B246" s="4">
         <f t="shared" si="14"/>
@@ -12127,7 +12133,7 @@
     </row>
     <row r="247" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A247" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B247" s="4">
         <f t="shared" si="14"/>
@@ -12147,7 +12153,7 @@
     </row>
     <row r="248" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A248" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B248" s="4">
         <f t="shared" si="14"/>
@@ -12170,7 +12176,7 @@
     </row>
     <row r="249" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A249" s="8" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B249" s="4">
         <f t="shared" si="14"/>
@@ -12193,7 +12199,7 @@
     </row>
     <row r="250" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A250" s="8" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B250" s="4"/>
       <c r="C250" s="15"/>
@@ -12211,7 +12217,7 @@
     </row>
     <row r="251" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A251" s="8" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B251" s="4"/>
       <c r="C251" s="15"/>
@@ -12227,124 +12233,112 @@
         <v>655.85501195381346</v>
       </c>
     </row>
-    <row r="252" spans="1:39" x14ac:dyDescent="0.55000000000000004">
-      <c r="A252" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B252" s="4"/>
-      <c r="C252" s="15">
+    <row r="252" spans="1:39" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A252" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B252" s="10">
+        <f>DATE(2003,12,9)+C252</f>
+        <v>37995</v>
+      </c>
+      <c r="C252" s="22">
         <v>31</v>
       </c>
-      <c r="G252" s="17">
+      <c r="G252" s="23"/>
+      <c r="H252" s="22"/>
+      <c r="T252">
+        <v>20.487820204008901</v>
+      </c>
+      <c r="U252">
+        <v>10.4591248978906</v>
+      </c>
+      <c r="Y252" s="23"/>
+      <c r="Z252" s="9">
+        <v>42.530842217707303</v>
+      </c>
+    </row>
+    <row r="253" spans="1:39" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A253" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B253" s="10">
+        <f t="shared" ref="B253:B255" si="15">DATE(2003,12,9)+C253</f>
+        <v>38021</v>
+      </c>
+      <c r="C253" s="22">
+        <v>57</v>
+      </c>
+      <c r="G253" s="23"/>
+      <c r="H253" s="22"/>
+      <c r="T253">
+        <v>115.0755084515</v>
+      </c>
+      <c r="U253">
+        <v>123.07772867226601</v>
+      </c>
+      <c r="Y253" s="23"/>
+      <c r="Z253" s="9">
+        <v>239.33770395660099</v>
+      </c>
+    </row>
+    <row r="254" spans="1:39" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A254" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B254" s="10">
+        <f t="shared" si="15"/>
+        <v>38035</v>
+      </c>
+      <c r="C254" s="22">
+        <v>71</v>
+      </c>
+      <c r="G254" s="23"/>
+      <c r="H254" s="22"/>
+      <c r="T254">
+        <v>183.419558888213</v>
+      </c>
+      <c r="U254">
+        <v>259.58988752277799</v>
+      </c>
+      <c r="Y254" s="23"/>
+      <c r="Z254" s="9">
+        <v>441.99777977923401</v>
+      </c>
+    </row>
+    <row r="255" spans="1:39" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A255" s="13" t="s">
+        <v>308</v>
+      </c>
+      <c r="B255" s="10">
+        <f t="shared" si="15"/>
+        <v>38092</v>
+      </c>
+      <c r="C255" s="22">
+        <v>128</v>
+      </c>
+      <c r="D255" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="G255" s="23">
         <v>44</v>
       </c>
-      <c r="H252" s="15">
+      <c r="H255" s="22">
         <v>127</v>
       </c>
-      <c r="T252" s="15">
-        <v>1710.9930320916199</v>
-      </c>
-      <c r="U252" s="15">
-        <v>1531.56588669085</v>
-      </c>
-      <c r="Y252" s="17">
+      <c r="T255" s="22"/>
+      <c r="U255">
+        <v>130.10912594516401</v>
+      </c>
+      <c r="Y255" s="23">
         <v>368</v>
       </c>
-      <c r="Z252">
-        <f>6.9*100</f>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="253" spans="1:39" x14ac:dyDescent="0.55000000000000004">
-      <c r="A253" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B253" s="4"/>
-      <c r="C253" s="15">
-        <v>57</v>
-      </c>
-      <c r="G253" s="17">
-        <v>44</v>
-      </c>
-      <c r="H253" s="15">
-        <v>127</v>
-      </c>
-      <c r="T253" s="15">
-        <v>11842.443955304399</v>
-      </c>
-      <c r="U253" s="15">
-        <v>12200.7935283973</v>
-      </c>
-      <c r="Y253" s="17">
-        <v>368</v>
-      </c>
-      <c r="Z253">
-        <f t="shared" ref="Z253:Z255" si="15">6.9*100</f>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="254" spans="1:39" x14ac:dyDescent="0.55000000000000004">
-      <c r="A254" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B254" s="4"/>
-      <c r="C254" s="15">
-        <v>71</v>
-      </c>
-      <c r="G254" s="17">
-        <v>44</v>
-      </c>
-      <c r="H254" s="15">
-        <v>127</v>
-      </c>
-      <c r="T254" s="15">
-        <v>17889.971539529197</v>
-      </c>
-      <c r="U254" s="15">
-        <v>25763.063075693597</v>
-      </c>
-      <c r="Y254" s="17">
-        <v>368</v>
-      </c>
-      <c r="Z254">
-        <f t="shared" si="15"/>
-        <v>690</v>
-      </c>
-    </row>
-    <row r="255" spans="1:39" x14ac:dyDescent="0.55000000000000004">
-      <c r="A255" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="B255" s="4"/>
-      <c r="C255" s="15">
-        <v>128</v>
-      </c>
-      <c r="D255" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="G255" s="17">
-        <v>44</v>
-      </c>
-      <c r="H255" s="15">
-        <v>127</v>
-      </c>
-      <c r="T255" s="15">
-        <v>13451.484010262498</v>
-      </c>
-      <c r="U255" s="15">
-        <v>12736.803734911</v>
-      </c>
-      <c r="Y255" s="17">
-        <v>368</v>
-      </c>
-      <c r="Z255">
-        <f t="shared" si="15"/>
-        <v>690</v>
+      <c r="Z255" s="9">
+        <v>693.36866137444201</v>
       </c>
     </row>
     <row r="256" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A256" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B256" s="4">
         <f>DATE(1980,4,1)+C256</f>
@@ -12371,10 +12365,10 @@
     </row>
     <row r="257" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A257" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B257" s="4">
-        <f t="shared" ref="B257:B259" si="16">DATE(1980,4,1)+C257</f>
+        <f t="shared" ref="B257:B258" si="16">DATE(1980,4,1)+C257</f>
         <v>29393</v>
       </c>
       <c r="C257" s="15">
@@ -12394,7 +12388,7 @@
     </row>
     <row r="258" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A258" s="8" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B258" s="4">
         <f t="shared" si="16"/>
@@ -12417,7 +12411,7 @@
     </row>
     <row r="259" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A259" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B259" s="4">
         <f>DATE(1979,4,10)+C259</f>
@@ -12441,7 +12435,7 @@
     </row>
     <row r="260" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A260" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B260" s="4">
         <f t="shared" ref="B260:B261" si="17">DATE(1979,4,10)+C260</f>
@@ -12463,7 +12457,7 @@
     </row>
     <row r="261" spans="1:27" x14ac:dyDescent="0.55000000000000004">
       <c r="A261" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B261" s="4">
         <f t="shared" si="17"/>

</xml_diff>

<commit_message>
second day's work - now using simple leaf with senescence and detachment working.
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr hidePivotFieldList="1" showPivotChartFilter="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05040F49-9781-4392-9EF3-B66AF4C7571D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="16608" windowHeight="10536" tabRatio="1000"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Observed" sheetId="14" r:id="rId1"/>
@@ -28,7 +29,7 @@
   <definedNames>
     <definedName name="Treatment_Structure">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -1045,7 +1046,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
@@ -1180,7 +1181,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_obs" xfId="1"/>
+    <cellStyle name="Normal_obs" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1196,7 +1197,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1546,7 +1547,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-61C3-45C4-AC13-2BFFBD0F635C}"/>
             </c:ext>
@@ -1659,7 +1660,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-61C3-45C4-AC13-2BFFBD0F635C}"/>
             </c:ext>
@@ -1846,7 +1847,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2172,7 +2173,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-1306-47EF-8F4A-B0EE79C3BE5E}"/>
             </c:ext>
@@ -2282,7 +2283,7 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-1306-47EF-8F4A-B0EE79C3BE5E}"/>
             </c:ext>
@@ -3600,7 +3601,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0A00-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3636,7 +3637,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0A00-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0A00-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3735,6 +3736,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3770,6 +3788,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3945,15 +3980,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CO348"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10716" ySplit="576" topLeftCell="AP303" activePane="bottomRight"/>
+      <pane xSplit="10716" ySplit="576" topLeftCell="AI194" activePane="bottomRight"/>
       <selection activeCell="A16" sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="CP1" sqref="CP1"/>
       <selection pane="bottomLeft" activeCell="A318" sqref="A318:XFD318"/>
-      <selection pane="bottomRight" activeCell="AR318" sqref="AR318:AR348"/>
+      <selection pane="bottomRight" activeCell="AK214" sqref="AK214"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12812,8 +12847,12 @@
         <v>0.47</v>
       </c>
       <c r="AN192"/>
-    </row>
-    <row r="193" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ192" s="9">
+        <f>SUM(AJ192:AN192)</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="193" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>225</v>
       </c>
@@ -12853,8 +12892,12 @@
       <c r="AM193">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="194" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ193" s="9">
+        <f t="shared" ref="AQ193:AQ210" si="14">SUM(AJ193:AN193)</f>
+        <v>1.19</v>
+      </c>
+    </row>
+    <row r="194" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>225</v>
       </c>
@@ -12894,8 +12937,12 @@
       <c r="AM194">
         <v>0.62</v>
       </c>
-    </row>
-    <row r="195" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ194" s="9">
+        <f t="shared" si="14"/>
+        <v>2.81</v>
+      </c>
+    </row>
+    <row r="195" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>225</v>
       </c>
@@ -12935,8 +12982,12 @@
       <c r="AM195">
         <v>1.55</v>
       </c>
-    </row>
-    <row r="196" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ195" s="9">
+        <f t="shared" si="14"/>
+        <v>5.24</v>
+      </c>
+    </row>
+    <row r="196" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>225</v>
       </c>
@@ -12976,8 +13027,12 @@
       <c r="AM196">
         <v>2.69</v>
       </c>
-    </row>
-    <row r="197" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ196" s="9">
+        <f t="shared" si="14"/>
+        <v>8.27</v>
+      </c>
+    </row>
+    <row r="197" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>225</v>
       </c>
@@ -13029,8 +13084,12 @@
       <c r="AN197">
         <v>0.88</v>
       </c>
-    </row>
-    <row r="198" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ197" s="9">
+        <f t="shared" si="14"/>
+        <v>14.53</v>
+      </c>
+    </row>
+    <row r="198" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>225</v>
       </c>
@@ -13082,8 +13141,12 @@
       <c r="AN198">
         <v>6.3</v>
       </c>
-    </row>
-    <row r="199" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ198" s="9">
+        <f t="shared" si="14"/>
+        <v>20.38</v>
+      </c>
+    </row>
+    <row r="199" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>225</v>
       </c>
@@ -13135,8 +13198,12 @@
       <c r="AN199">
         <v>19.87</v>
       </c>
-    </row>
-    <row r="200" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ199" s="9">
+        <f t="shared" si="14"/>
+        <v>28.41</v>
+      </c>
+    </row>
+    <row r="200" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>225</v>
       </c>
@@ -13188,8 +13255,12 @@
       <c r="AN200">
         <v>23.11</v>
       </c>
-    </row>
-    <row r="201" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ200" s="9">
+        <f t="shared" si="14"/>
+        <v>26.28</v>
+      </c>
+    </row>
+    <row r="201" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>225</v>
       </c>
@@ -13231,8 +13302,9 @@
         <f>Z201/AA201</f>
         <v>0.55059870595796667</v>
       </c>
-    </row>
-    <row r="202" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ201" s="9"/>
+    </row>
+    <row r="202" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>225</v>
       </c>
@@ -13246,8 +13318,9 @@
       </c>
       <c r="AA202" s="11"/>
       <c r="AB202" s="11"/>
-    </row>
-    <row r="203" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ202" s="9"/>
+    </row>
+    <row r="203" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>226</v>
       </c>
@@ -13287,8 +13360,12 @@
       <c r="AM203">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="204" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ203" s="9">
+        <f t="shared" si="14"/>
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="204" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>226</v>
       </c>
@@ -13328,8 +13405,12 @@
       <c r="AM204">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="205" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ204" s="9">
+        <f t="shared" si="14"/>
+        <v>0.45999999999999996</v>
+      </c>
+    </row>
+    <row r="205" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>226</v>
       </c>
@@ -13369,8 +13450,12 @@
       <c r="AM205">
         <v>0.57999999999999996</v>
       </c>
-    </row>
-    <row r="206" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ205" s="9">
+        <f t="shared" si="14"/>
+        <v>2.1800000000000002</v>
+      </c>
+    </row>
+    <row r="206" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>226</v>
       </c>
@@ -13410,8 +13495,12 @@
       <c r="AM206">
         <v>0.77</v>
       </c>
-    </row>
-    <row r="207" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ206" s="9">
+        <f t="shared" si="14"/>
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="207" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>226</v>
       </c>
@@ -13463,8 +13552,12 @@
       <c r="AN207">
         <v>0.08</v>
       </c>
-    </row>
-    <row r="208" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ207" s="9">
+        <f t="shared" si="14"/>
+        <v>8.43</v>
+      </c>
+    </row>
+    <row r="208" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>226</v>
       </c>
@@ -13516,8 +13609,12 @@
       <c r="AN208">
         <v>1.33</v>
       </c>
-    </row>
-    <row r="209" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ208" s="9">
+        <f t="shared" si="14"/>
+        <v>12.930000000000001</v>
+      </c>
+    </row>
+    <row r="209" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>226</v>
       </c>
@@ -13569,8 +13666,12 @@
       <c r="AN209">
         <v>7.34</v>
       </c>
-    </row>
-    <row r="210" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ209" s="9">
+        <f t="shared" si="14"/>
+        <v>17.43</v>
+      </c>
+    </row>
+    <row r="210" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>226</v>
       </c>
@@ -13622,8 +13723,12 @@
       <c r="AN210">
         <v>16.170000000000002</v>
       </c>
-    </row>
-    <row r="211" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ210" s="9">
+        <f t="shared" si="14"/>
+        <v>22.150000000000002</v>
+      </c>
+    </row>
+    <row r="211" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>226</v>
       </c>
@@ -13655,7 +13760,7 @@
       </c>
       <c r="AB211" s="11"/>
     </row>
-    <row r="212" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>226</v>
       </c>
@@ -13698,7 +13803,7 @@
         <v>0.56851041457267004</v>
       </c>
     </row>
-    <row r="213" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>226</v>
       </c>
@@ -13713,7 +13818,7 @@
       <c r="AA213" s="11"/>
       <c r="AB213" s="11"/>
     </row>
-    <row r="214" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>227</v>
       </c>
@@ -13753,8 +13858,12 @@
       <c r="AM214">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="215" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ214" s="9">
+        <f>SUM(AJ214:AN214)</f>
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="215" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>227</v>
       </c>
@@ -13794,8 +13903,12 @@
       <c r="AM215">
         <v>0.53</v>
       </c>
-    </row>
-    <row r="216" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ215" s="9">
+        <f t="shared" ref="AQ215:AQ232" si="15">SUM(AJ215:AN215)</f>
+        <v>1.96</v>
+      </c>
+    </row>
+    <row r="216" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>227</v>
       </c>
@@ -13835,8 +13948,12 @@
       <c r="AM216">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="217" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ216" s="9">
+        <f t="shared" si="15"/>
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>227</v>
       </c>
@@ -13867,8 +13984,12 @@
       <c r="AM217">
         <v>2.76</v>
       </c>
-    </row>
-    <row r="218" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ217" s="9">
+        <f t="shared" si="15"/>
+        <v>7.62</v>
+      </c>
+    </row>
+    <row r="218" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>227</v>
       </c>
@@ -13908,8 +14029,12 @@
       <c r="AM218">
         <v>4.43</v>
       </c>
-    </row>
-    <row r="219" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ218" s="9">
+        <f t="shared" si="15"/>
+        <v>10.96</v>
+      </c>
+    </row>
+    <row r="219" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>227</v>
       </c>
@@ -13961,8 +14086,12 @@
       <c r="AN219">
         <v>1.69</v>
       </c>
-    </row>
-    <row r="220" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ219" s="9">
+        <f t="shared" si="15"/>
+        <v>16.350000000000001</v>
+      </c>
+    </row>
+    <row r="220" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>227</v>
       </c>
@@ -14014,8 +14143,12 @@
       <c r="AN220">
         <v>8.07</v>
       </c>
-    </row>
-    <row r="221" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ220" s="9">
+        <f t="shared" si="15"/>
+        <v>21.79</v>
+      </c>
+    </row>
+    <row r="221" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>227</v>
       </c>
@@ -14067,8 +14200,12 @@
       <c r="AN221">
         <v>13.73</v>
       </c>
-    </row>
-    <row r="222" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ221" s="9">
+        <f t="shared" si="15"/>
+        <v>22.55</v>
+      </c>
+    </row>
+    <row r="222" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>227</v>
       </c>
@@ -14099,8 +14236,9 @@
         <v>859.78300000000002</v>
       </c>
       <c r="AB222" s="11"/>
-    </row>
-    <row r="223" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ222" s="9"/>
+    </row>
+    <row r="223" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>227</v>
       </c>
@@ -14142,8 +14280,9 @@
         <f>Z223/AA223</f>
         <v>0.58168937754546468</v>
       </c>
-    </row>
-    <row r="224" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="AQ223" s="9"/>
+    </row>
+    <row r="224" spans="1:43" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>227</v>
       </c>
@@ -14157,6 +14296,7 @@
       </c>
       <c r="AA224" s="11"/>
       <c r="AB224" s="11"/>
+      <c r="AQ224" s="9"/>
     </row>
     <row r="225" spans="1:45" hidden="1" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
@@ -14198,6 +14338,10 @@
       <c r="AM225">
         <v>0.12</v>
       </c>
+      <c r="AQ225" s="9">
+        <f t="shared" si="15"/>
+        <v>0.49</v>
+      </c>
     </row>
     <row r="226" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
@@ -14238,6 +14382,10 @@
       </c>
       <c r="AM226">
         <v>0.26</v>
+      </c>
+      <c r="AQ226" s="9">
+        <f t="shared" si="15"/>
+        <v>1.05</v>
       </c>
     </row>
     <row r="227" spans="1:45" x14ac:dyDescent="0.3">
@@ -14271,6 +14419,10 @@
       <c r="AM227">
         <v>1.1100000000000001</v>
       </c>
+      <c r="AQ227" s="9">
+        <f t="shared" si="15"/>
+        <v>3.6399999999999997</v>
+      </c>
     </row>
     <row r="228" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
@@ -14312,6 +14464,10 @@
       <c r="AM228">
         <v>2.25</v>
       </c>
+      <c r="AQ228" s="9">
+        <f t="shared" si="15"/>
+        <v>6.65</v>
+      </c>
     </row>
     <row r="229" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
@@ -14365,6 +14521,10 @@
       <c r="AN229">
         <v>0.06</v>
       </c>
+      <c r="AQ229" s="9">
+        <f t="shared" si="15"/>
+        <v>11.93</v>
+      </c>
     </row>
     <row r="230" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
@@ -14418,6 +14578,10 @@
       <c r="AN230">
         <v>2.27</v>
       </c>
+      <c r="AQ230" s="9">
+        <f t="shared" si="15"/>
+        <v>16.53</v>
+      </c>
     </row>
     <row r="231" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
@@ -14471,6 +14635,10 @@
       <c r="AN231">
         <v>7.03</v>
       </c>
+      <c r="AQ231" s="9">
+        <f t="shared" si="15"/>
+        <v>20.440000000000001</v>
+      </c>
     </row>
     <row r="232" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
@@ -14512,6 +14680,10 @@
       <c r="AN232">
         <v>15.98</v>
       </c>
+      <c r="AQ232" s="9">
+        <f t="shared" si="15"/>
+        <v>19.940000000000001</v>
+      </c>
     </row>
     <row r="233" spans="1:45" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
@@ -14629,7 +14801,7 @@
         <v>298</v>
       </c>
       <c r="B237" s="4">
-        <f t="shared" ref="B237:B249" si="14">DATE(1988,1,5)+C237</f>
+        <f t="shared" ref="B237:B249" si="16">DATE(1988,1,5)+C237</f>
         <v>32179.521739130436</v>
       </c>
       <c r="C237" s="15">
@@ -14653,7 +14825,7 @@
         <v>298</v>
       </c>
       <c r="B238" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32190.478260869564</v>
       </c>
       <c r="C238" s="15">
@@ -14677,7 +14849,7 @@
         <v>298</v>
       </c>
       <c r="B239" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32200.391304347824</v>
       </c>
       <c r="C239" s="15">
@@ -14701,7 +14873,7 @@
         <v>298</v>
       </c>
       <c r="B240" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32212.391304347828</v>
       </c>
       <c r="C240" s="15">
@@ -14725,7 +14897,7 @@
         <v>298</v>
       </c>
       <c r="B241" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32227.521739130436</v>
       </c>
       <c r="C241" s="15">
@@ -14749,7 +14921,7 @@
         <v>298</v>
       </c>
       <c r="B242" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32237.434782608696</v>
       </c>
       <c r="C242" s="15">
@@ -14774,7 +14946,7 @@
         <v>299</v>
       </c>
       <c r="B243" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32169.434782608696</v>
       </c>
       <c r="C243" s="15">
@@ -14798,7 +14970,7 @@
         <v>299</v>
       </c>
       <c r="B244" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32179.521739130436</v>
       </c>
       <c r="C244" s="15">
@@ -14822,7 +14994,7 @@
         <v>299</v>
       </c>
       <c r="B245" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32190.652173913044</v>
       </c>
       <c r="C245" s="15">
@@ -14841,7 +15013,7 @@
         <v>299</v>
       </c>
       <c r="B246" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32200.391304347824</v>
       </c>
       <c r="C246" s="15">
@@ -14862,7 +15034,7 @@
         <v>299</v>
       </c>
       <c r="B247" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32212.391304347828</v>
       </c>
       <c r="C247" s="15">
@@ -14883,7 +15055,7 @@
         <v>299</v>
       </c>
       <c r="B248" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32227.347826086956</v>
       </c>
       <c r="C248" s="15">
@@ -14909,7 +15081,7 @@
         <v>299</v>
       </c>
       <c r="B249" s="4">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>32231.17391304348</v>
       </c>
       <c r="C249" s="15">
@@ -14998,7 +15170,7 @@
         <v>308</v>
       </c>
       <c r="B253" s="10">
-        <f t="shared" ref="B253:B255" si="15">DATE(2003,12,9)+C253</f>
+        <f t="shared" ref="B253:B255" si="17">DATE(2003,12,9)+C253</f>
         <v>38021</v>
       </c>
       <c r="C253" s="22">
@@ -15022,7 +15194,7 @@
         <v>308</v>
       </c>
       <c r="B254" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>38035</v>
       </c>
       <c r="C254" s="22">
@@ -15046,7 +15218,7 @@
         <v>308</v>
       </c>
       <c r="B255" s="10">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>38092</v>
       </c>
       <c r="C255" s="22">
@@ -15072,7 +15244,7 @@
         <v>693.36866137444201</v>
       </c>
       <c r="AB255">
-        <f t="shared" ref="AB255:AB261" si="16">Z255/AA255</f>
+        <f t="shared" ref="AB255:AB261" si="18">Z255/AA255</f>
         <v>0.53074218738199908</v>
       </c>
     </row>
@@ -15103,7 +15275,7 @@
         <v>554</v>
       </c>
       <c r="AB256">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.50541516245487361</v>
       </c>
     </row>
@@ -15112,7 +15284,7 @@
         <v>304</v>
       </c>
       <c r="B257" s="4">
-        <f t="shared" ref="B257:B258" si="17">DATE(1980,4,1)+C257</f>
+        <f t="shared" ref="B257:B258" si="19">DATE(1980,4,1)+C257</f>
         <v>29393</v>
       </c>
       <c r="C257" s="15">
@@ -15130,7 +15302,7 @@
         <v>163</v>
       </c>
       <c r="AB257">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.39263803680981596</v>
       </c>
     </row>
@@ -15139,7 +15311,7 @@
         <v>303</v>
       </c>
       <c r="B258" s="4">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>29393</v>
       </c>
       <c r="C258" s="15">
@@ -15157,7 +15329,7 @@
         <v>329</v>
       </c>
       <c r="AB258">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.36474164133738601</v>
       </c>
     </row>
@@ -15185,7 +15357,7 @@
         <v>190</v>
       </c>
       <c r="AB259">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.58421052631578951</v>
       </c>
     </row>
@@ -15194,7 +15366,7 @@
         <v>306</v>
       </c>
       <c r="B260" s="4">
-        <f t="shared" ref="B260:B261" si="18">DATE(1979,4,10)+C260</f>
+        <f t="shared" ref="B260:B261" si="20">DATE(1979,4,10)+C260</f>
         <v>29042</v>
       </c>
       <c r="C260" s="15">
@@ -15210,7 +15382,7 @@
         <v>61</v>
       </c>
       <c r="AB260">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.54098360655737709</v>
       </c>
       <c r="AC260" s="21"/>
@@ -15220,7 +15392,7 @@
         <v>307</v>
       </c>
       <c r="B261" s="4">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>29042</v>
       </c>
       <c r="C261" s="15">
@@ -15236,7 +15408,7 @@
         <v>136</v>
       </c>
       <c r="AB261">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>0.56617647058823528</v>
       </c>
     </row>
@@ -15303,11 +15475,11 @@
         <v>223.9</v>
       </c>
       <c r="AE263">
-        <f t="shared" ref="AE263:AE317" si="19">AL263/T263</f>
+        <f t="shared" ref="AE263:AE317" si="21">AL263/T263</f>
         <v>5.918367346938775E-2</v>
       </c>
       <c r="AF263">
-        <f t="shared" ref="AF263:AF317" si="20">AM263/U263</f>
+        <f t="shared" ref="AF263:AF317" si="22">AM263/U263</f>
         <v>1.84E-2</v>
       </c>
       <c r="AL263">
@@ -15349,15 +15521,15 @@
         <v>458.3</v>
       </c>
       <c r="AE264">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.6804733727810648E-2</v>
       </c>
       <c r="AF264">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.453287197231834E-2</v>
       </c>
       <c r="AG264">
-        <f t="shared" ref="AG264:AG317" si="21">AN264/V264</f>
+        <f t="shared" ref="AG264:AG317" si="23">AN264/V264</f>
         <v>0.04</v>
       </c>
       <c r="AL264">
@@ -15402,15 +15574,15 @@
         <v>785.8</v>
       </c>
       <c r="AE265">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0256410256410257E-2</v>
       </c>
       <c r="AF265">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7371937639198219E-2</v>
       </c>
       <c r="AG265">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.4951456310679613E-2</v>
       </c>
       <c r="AL265">
@@ -15455,15 +15627,15 @@
         <v>1008.2</v>
       </c>
       <c r="AE266">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.3218884120171672E-2</v>
       </c>
       <c r="AF266">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.0206185567010312E-2</v>
       </c>
       <c r="AG266">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.03448275862069E-2</v>
       </c>
       <c r="AL266">
@@ -15508,15 +15680,15 @@
         <v>1129</v>
       </c>
       <c r="AE267">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.6116504854368932E-2</v>
       </c>
       <c r="AF267">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.5638766519823787E-2</v>
       </c>
       <c r="AG267">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.6055437100213224E-2</v>
       </c>
       <c r="AL267">
@@ -15583,23 +15755,23 @@
         <v>1144.7</v>
       </c>
       <c r="AE268">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.043478260869565E-2</v>
       </c>
       <c r="AF268">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.1282051282051283E-2</v>
       </c>
       <c r="AG268">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.9170437405731522E-2</v>
       </c>
       <c r="AH268">
-        <f t="shared" ref="AH268:AH317" si="22">AO268/W268</f>
+        <f t="shared" ref="AH268:AH317" si="24">AO268/W268</f>
         <v>2.1702127659574466E-2</v>
       </c>
       <c r="AI268">
-        <f t="shared" ref="AI268:AI317" si="23">AP268/Z268</f>
+        <f t="shared" ref="AI268:AI317" si="25">AP268/Z268</f>
         <v>6.4252336448598124E-2</v>
       </c>
       <c r="AL268">
@@ -15647,11 +15819,11 @@
         <v>127</v>
       </c>
       <c r="AE269">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0294117647058817E-2</v>
       </c>
       <c r="AF269">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.3728813559322031E-2</v>
       </c>
       <c r="AL269">
@@ -15690,11 +15862,11 @@
         <v>302</v>
       </c>
       <c r="AE270">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0156250000000001E-2</v>
       </c>
       <c r="AF270">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.9540229885057471E-2</v>
       </c>
       <c r="AL270">
@@ -15736,15 +15908,15 @@
         <v>574</v>
       </c>
       <c r="AE271">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9905660377358484E-2</v>
       </c>
       <c r="AF271">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.8232044198895028E-2</v>
       </c>
       <c r="AG271">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.6000000000000004E-2</v>
       </c>
       <c r="AL271">
@@ -15789,15 +15961,15 @@
         <v>962.7</v>
       </c>
       <c r="AE272">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.7039711191335746E-2</v>
       </c>
       <c r="AF272">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7624521072796932E-2</v>
       </c>
       <c r="AG272">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.414634146341463E-2</v>
       </c>
       <c r="AL272">
@@ -15842,15 +16014,15 @@
         <v>1286.5999999999999</v>
       </c>
       <c r="AE273">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.3608247422680409E-2</v>
       </c>
       <c r="AF273">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7152658662092625E-2</v>
       </c>
       <c r="AG273">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.8571428571428574E-2</v>
       </c>
       <c r="AL273">
@@ -15895,15 +16067,15 @@
         <v>1480.5</v>
       </c>
       <c r="AE274">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.4583333333333329E-2</v>
       </c>
       <c r="AF274">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.3027522935779816E-2</v>
       </c>
       <c r="AG274">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.793103448275862E-2</v>
       </c>
       <c r="AL274">
@@ -15970,23 +16142,23 @@
         <v>1512.8</v>
       </c>
       <c r="AE275">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.1318681318681318E-2</v>
       </c>
       <c r="AF275">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.1259541984732824E-2</v>
       </c>
       <c r="AG275">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.5105328376703842E-2</v>
       </c>
       <c r="AH275">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.8361581920903956E-2</v>
       </c>
       <c r="AI275">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.4238410596026488E-2</v>
       </c>
       <c r="AL275">
@@ -16034,11 +16206,11 @@
         <v>136.69999999999999</v>
       </c>
       <c r="AE276">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.6944444444444436E-2</v>
       </c>
       <c r="AF276">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.4615384615384615E-2</v>
       </c>
       <c r="AL276">
@@ -16077,11 +16249,11 @@
         <v>275</v>
       </c>
       <c r="AE277">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9504132231404959E-2</v>
       </c>
       <c r="AF277">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.8181818181818181E-2</v>
       </c>
       <c r="AL277">
@@ -16123,15 +16295,15 @@
         <v>524</v>
       </c>
       <c r="AE278">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.7671957671957673E-2</v>
       </c>
       <c r="AF278">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.5820895522388058E-2</v>
       </c>
       <c r="AG278">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.04</v>
       </c>
       <c r="AL278">
@@ -16176,15 +16348,15 @@
         <v>848.9</v>
       </c>
       <c r="AE279">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.903614457831325E-2</v>
       </c>
       <c r="AF279">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.9008264462809916E-2</v>
       </c>
       <c r="AG279">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.5897435897435902E-2</v>
       </c>
       <c r="AL279">
@@ -16229,15 +16401,15 @@
         <v>1065.5</v>
       </c>
       <c r="AE280">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.0446428571428573E-2</v>
       </c>
       <c r="AF280">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.0743639921722113E-2</v>
       </c>
       <c r="AG280">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.9607250755287012E-2</v>
       </c>
       <c r="AL280">
@@ -16282,15 +16454,15 @@
         <v>1167.5</v>
       </c>
       <c r="AE281">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.4973544973544971E-2</v>
       </c>
       <c r="AF281">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7672413793103445E-2</v>
       </c>
       <c r="AG281">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.2023346303501949E-2</v>
       </c>
       <c r="AL281">
@@ -16357,23 +16529,23 @@
         <v>1165.9000000000001</v>
       </c>
       <c r="AE282">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.6760563380281689E-2</v>
       </c>
       <c r="AF282">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.0126582278481013E-2</v>
       </c>
       <c r="AG282">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.7285714285714285E-2</v>
       </c>
       <c r="AH282">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>2.0542635658914728E-2</v>
       </c>
       <c r="AI282">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.2669683257918551E-2</v>
       </c>
       <c r="AL282">
@@ -16421,11 +16593,11 @@
         <v>124.9</v>
       </c>
       <c r="AE283">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0606060606060608E-2</v>
       </c>
       <c r="AF283">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.2033898305084745E-2</v>
       </c>
       <c r="AL283">
@@ -16464,11 +16636,11 @@
         <v>329.1</v>
       </c>
       <c r="AE284">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9574468085106386E-2</v>
       </c>
       <c r="AF284">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.8085106382978722E-2</v>
       </c>
       <c r="AL284">
@@ -16510,15 +16682,15 @@
         <v>647.6</v>
       </c>
       <c r="AE285">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.8050847457627112E-2</v>
       </c>
       <c r="AF285">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7233009708737864E-2</v>
       </c>
       <c r="AG285">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.6363636363636362E-2</v>
       </c>
       <c r="AL285">
@@ -16563,15 +16735,15 @@
         <v>1071.5</v>
       </c>
       <c r="AE286">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0130718954248361E-2</v>
       </c>
       <c r="AF286">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7109634551495018E-2</v>
       </c>
       <c r="AG286">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.4969325153374232E-2</v>
       </c>
       <c r="AL286">
@@ -16616,15 +16788,15 @@
         <v>1362.6</v>
       </c>
       <c r="AE287">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.2758620689655172E-2</v>
       </c>
       <c r="AF287">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.6693944353518821E-2</v>
       </c>
       <c r="AG287">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.7922077922077924E-2</v>
       </c>
       <c r="AL287">
@@ -16669,15 +16841,15 @@
         <v>1487.7</v>
       </c>
       <c r="AE288">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.1393442622950818E-2</v>
       </c>
       <c r="AF288">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.3114754098360656E-2</v>
       </c>
       <c r="AG288">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.7697841726618705E-2</v>
       </c>
       <c r="AL288">
@@ -16744,23 +16916,23 @@
         <v>1497</v>
       </c>
       <c r="AE289">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.7567567567567567E-2</v>
       </c>
       <c r="AF289">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.1068702290076336E-2</v>
       </c>
       <c r="AG289">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.4359949302915085E-2</v>
       </c>
       <c r="AH289">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.6374269005847951E-2</v>
       </c>
       <c r="AI289">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.4349775784753357E-2</v>
       </c>
       <c r="AL289">
@@ -16808,11 +16980,11 @@
         <v>147.19999999999999</v>
       </c>
       <c r="AE290">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.6250000000000001E-2</v>
       </c>
       <c r="AF290">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.6865671641791045E-2</v>
       </c>
       <c r="AL290">
@@ -16851,11 +17023,11 @@
         <v>285.8</v>
       </c>
       <c r="AE291">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9200000000000003E-2</v>
       </c>
       <c r="AF291">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.0496894409937887E-2</v>
       </c>
       <c r="AL291">
@@ -16897,15 +17069,15 @@
         <v>519.4</v>
       </c>
       <c r="AE292">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.5675675675675683E-2</v>
       </c>
       <c r="AF292">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.4925373134328358E-2</v>
       </c>
       <c r="AG292">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.8095238095238099E-2</v>
       </c>
       <c r="AL292">
@@ -16950,15 +17122,15 @@
         <v>843.8</v>
       </c>
       <c r="AE293">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.7851239669421489E-2</v>
       </c>
       <c r="AF293">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.4784394250513347E-2</v>
       </c>
       <c r="AG293">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.3913043478260872E-2</v>
       </c>
       <c r="AL293">
@@ -17003,15 +17175,15 @@
         <v>1065</v>
       </c>
       <c r="AE294">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.1739130434782607E-2</v>
       </c>
       <c r="AF294">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.1305182341650672E-2</v>
       </c>
       <c r="AG294">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.8662420382165606E-2</v>
       </c>
       <c r="AL294">
@@ -17056,15 +17228,15 @@
         <v>1186.5</v>
       </c>
       <c r="AE295">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.228855721393035E-2</v>
       </c>
       <c r="AF295">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.5789473684210527E-2</v>
       </c>
       <c r="AG295">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.2973523421588597E-2</v>
       </c>
       <c r="AL295">
@@ -17131,23 +17303,23 @@
         <v>1208.5</v>
       </c>
       <c r="AE296">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.9914529914529916E-2</v>
       </c>
       <c r="AF296">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.0730593607305937E-2</v>
       </c>
       <c r="AG296">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.8929663608562692E-2</v>
       </c>
       <c r="AH296">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>2.1333333333333333E-2</v>
       </c>
       <c r="AI296">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.3403263403263396E-2</v>
       </c>
       <c r="AL296">
@@ -17195,11 +17367,11 @@
         <v>142.30000000000001</v>
       </c>
       <c r="AE297">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.133333333333333E-2</v>
       </c>
       <c r="AF297">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.5373134328358207E-2</v>
       </c>
       <c r="AL297">
@@ -17238,11 +17410,11 @@
         <v>335.8</v>
       </c>
       <c r="AE298">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0000000000000005E-2</v>
       </c>
       <c r="AF298">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.9387755102040816E-2</v>
       </c>
       <c r="AL298">
@@ -17284,15 +17456,15 @@
         <v>628.6</v>
       </c>
       <c r="AE299">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.7268722466960353E-2</v>
       </c>
       <c r="AF299">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="AG299">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.7037037037037035E-2</v>
       </c>
       <c r="AL299">
@@ -17337,15 +17509,15 @@
         <v>1024.7</v>
       </c>
       <c r="AE300">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.7192982456140351E-2</v>
       </c>
       <c r="AF300">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7730496453900711E-2</v>
       </c>
       <c r="AG300">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.4090909090909088E-2</v>
       </c>
       <c r="AL300">
@@ -17390,15 +17562,15 @@
         <v>1333.8</v>
       </c>
       <c r="AE301">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.4063604240282691E-2</v>
       </c>
       <c r="AF301">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7214397496087636E-2</v>
       </c>
       <c r="AG301">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.8883495145631068E-2</v>
       </c>
       <c r="AL301">
@@ -17443,15 +17615,15 @@
         <v>1499.8</v>
       </c>
       <c r="AE302">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.2975206611570248E-2</v>
       </c>
       <c r="AF302">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.348122866894198E-2</v>
       </c>
       <c r="AG302">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.8690476190476192E-2</v>
       </c>
       <c r="AL302">
@@ -17518,23 +17690,23 @@
         <v>1502.9</v>
       </c>
       <c r="AE303">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.8313253012048192E-2</v>
       </c>
       <c r="AF303">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.1517367458866544E-2</v>
       </c>
       <c r="AG303">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.5569620253164557E-2</v>
       </c>
       <c r="AH303">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.9705882352941177E-2</v>
       </c>
       <c r="AI303">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="AL303">
@@ -17582,11 +17754,11 @@
         <v>104</v>
       </c>
       <c r="AE304">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.3571428571428568E-2</v>
       </c>
       <c r="AF304">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.2916666666666669E-2</v>
       </c>
       <c r="AL304">
@@ -17625,11 +17797,11 @@
         <v>221.2</v>
       </c>
       <c r="AE305">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.0204081632653061E-2</v>
       </c>
       <c r="AF305">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.935483870967742E-2</v>
       </c>
       <c r="AL305">
@@ -17671,15 +17843,15 @@
         <v>447.7</v>
       </c>
       <c r="AE306">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.4819277108433734E-2</v>
       </c>
       <c r="AF306">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.5602836879432626E-2</v>
       </c>
       <c r="AG306">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.3333333333333333E-2</v>
       </c>
       <c r="AL306">
@@ -17724,15 +17896,15 @@
         <v>784.6</v>
       </c>
       <c r="AE307">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.6502242152466367E-2</v>
       </c>
       <c r="AF307">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.6008771929824563E-2</v>
       </c>
       <c r="AG307">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.5849056603773584E-2</v>
       </c>
       <c r="AL307">
@@ -17777,15 +17949,15 @@
         <v>979</v>
       </c>
       <c r="AE308">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.0970873786407765E-2</v>
       </c>
       <c r="AF308">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7073170731707318E-2</v>
       </c>
       <c r="AG308">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.8260869565217391E-2</v>
       </c>
       <c r="AL308">
@@ -17830,15 +18002,15 @@
         <v>1072.5999999999999</v>
       </c>
       <c r="AE309">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.2245989304812839E-2</v>
       </c>
       <c r="AF309">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.4939759036144579E-2</v>
       </c>
       <c r="AG309">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.5647558386411886E-2</v>
       </c>
       <c r="AL309">
@@ -17905,23 +18077,23 @@
         <v>1078.0999999999999</v>
       </c>
       <c r="AE310">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.8749999999999998E-2</v>
       </c>
       <c r="AF310">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.7826086956521747E-3</v>
       </c>
       <c r="AG310">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.9047619047619048E-2</v>
       </c>
       <c r="AH310">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>2.4774774774774775E-2</v>
       </c>
       <c r="AI310">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.2254901960784308E-2</v>
       </c>
       <c r="AL310">
@@ -17969,11 +18141,11 @@
         <v>148.5</v>
       </c>
       <c r="AE311">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>6.2025316455696207E-2</v>
       </c>
       <c r="AF311">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.4285714285714285E-2</v>
       </c>
       <c r="AL311">
@@ -18012,11 +18184,11 @@
         <v>338</v>
       </c>
       <c r="AE312">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9574468085106386E-2</v>
       </c>
       <c r="AF312">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.979695431472081E-2</v>
       </c>
       <c r="AL312">
@@ -18058,15 +18230,15 @@
         <v>630.1</v>
       </c>
       <c r="AE313">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9909909909909916E-2</v>
       </c>
       <c r="AF313">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7662337662337661E-2</v>
       </c>
       <c r="AG313">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.4782608695652174E-2</v>
       </c>
       <c r="AL313">
@@ -18111,15 +18283,15 @@
         <v>945.5</v>
       </c>
       <c r="AE314">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.9003831417624525E-2</v>
       </c>
       <c r="AF314">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.7391304347826087E-2</v>
       </c>
       <c r="AG314">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.5195530726256981E-2</v>
       </c>
       <c r="AL314">
@@ -18164,15 +18336,15 @@
         <v>1196.5999999999999</v>
       </c>
       <c r="AE315">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.3600000000000002E-2</v>
       </c>
       <c r="AF315">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.645101663585952E-2</v>
       </c>
       <c r="AG315">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>2.8817733990147781E-2</v>
       </c>
       <c r="AL315">
@@ -18217,15 +18389,15 @@
         <v>1342.6</v>
       </c>
       <c r="AE316">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>4.3203883495145631E-2</v>
       </c>
       <c r="AF316">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.1350293542074364E-2</v>
       </c>
       <c r="AG316">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.7220447284345051E-2</v>
       </c>
       <c r="AL316">
@@ -18292,23 +18464,23 @@
         <v>1349.9</v>
       </c>
       <c r="AE317">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>3.1360946745562127E-2</v>
       </c>
       <c r="AF317">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>1.0660980810234541E-2</v>
       </c>
       <c r="AG317">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>4.396067415730337E-2</v>
       </c>
       <c r="AH317">
-        <f t="shared" si="22"/>
+        <f t="shared" si="24"/>
         <v>1.6842105263157894E-2</v>
       </c>
       <c r="AI317">
-        <f t="shared" si="23"/>
+        <f t="shared" si="25"/>
         <v>6.323185011709602E-2</v>
       </c>
       <c r="AL317">
@@ -18776,7 +18948,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:X61"/>
   <sheetViews>
     <sheetView topLeftCell="K6" workbookViewId="0">
@@ -21521,7 +21693,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:L148"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -22206,7 +22378,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:CI261"/>
   <sheetViews>
     <sheetView topLeftCell="G1" workbookViewId="0">
@@ -35781,7 +35953,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:CH261">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:CH261">
     <sortCondition ref="A2:A261"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35790,7 +35962,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -36421,7 +36593,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D118"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -38171,7 +38343,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:M576"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -47988,7 +48160,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AF15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -49474,7 +49646,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I576"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
@@ -61312,7 +61484,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:T9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -61891,7 +62063,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:AR46"/>
   <sheetViews>
     <sheetView topLeftCell="A24" workbookViewId="0">
@@ -65002,7 +65174,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:AS20"/>
   <sheetViews>
     <sheetView topLeftCell="AE1" workbookViewId="0">

</xml_diff>

<commit_message>
Finished Flowering DAS for Leeton
</commit_message>
<xml_diff>
--- a/Prototypes/Soybean/Observed.xlsx
+++ b/Prototypes/Soybean/Observed.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ApsimX\Prototypes\Soybean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C196BE9-D6A8-4878-BB20-0E77E0317A4B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2174D756-072A-4FA7-BF66-432F53BE0196}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" tabRatio="1000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2743" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2943" uniqueCount="434">
   <si>
     <t>SimulationName</t>
   </si>
@@ -1044,6 +1044,306 @@
   </si>
   <si>
     <t>Soybean.Grain.FWt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvFiskebyV</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvF148_7</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvDjakal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvBowyer</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvBunya</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvCowrie</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvSoya791</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvManark</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvWarrigal</t>
+  </si>
+  <si>
+    <t>Leeton2006SowNov27CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec04CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec11CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec18CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowDec24CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan02CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan09CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan16CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan22CvLeichhardt</t>
+  </si>
+  <si>
+    <t>Leeton2006SowJan29CvLeichhardt</t>
   </si>
 </sst>
 </file>
@@ -3984,14 +4284,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CP348"/>
+  <dimension ref="A1:CP448"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="10716" ySplit="576" topLeftCell="Z73" activePane="bottomRight"/>
+      <pane xSplit="10716" ySplit="576" topLeftCell="A331" activePane="bottomRight"/>
       <selection activeCell="A16" sqref="A1:XFD1048576"/>
       <selection pane="topRight" activeCell="AA1" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="A85" sqref="A85"/>
-      <selection pane="bottomRight" activeCell="Z79" sqref="Z79:Z114"/>
+      <selection pane="bottomLeft" activeCell="A439" sqref="A439"/>
+      <selection pane="bottomRight" activeCell="H349" sqref="H349:H411"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19125,6 +19425,1280 @@
       </c>
       <c r="CP348" s="12">
         <v>3.88</v>
+      </c>
+    </row>
+    <row r="349" spans="1:94" x14ac:dyDescent="0.3">
+      <c r="A349" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="D349" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G349">
+        <v>34</v>
+      </c>
+      <c r="H349">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="350" spans="1:94" x14ac:dyDescent="0.3">
+      <c r="A350" t="s">
+        <v>335</v>
+      </c>
+      <c r="D350" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G350">
+        <v>28</v>
+      </c>
+      <c r="H350">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="351" spans="1:94" x14ac:dyDescent="0.3">
+      <c r="A351" t="s">
+        <v>336</v>
+      </c>
+      <c r="D351" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G351">
+        <v>30</v>
+      </c>
+      <c r="H351">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="352" spans="1:94" x14ac:dyDescent="0.3">
+      <c r="A352" t="s">
+        <v>337</v>
+      </c>
+      <c r="D352" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G352">
+        <v>30</v>
+      </c>
+      <c r="H352">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="353" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A353" t="s">
+        <v>338</v>
+      </c>
+      <c r="D353" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G353">
+        <v>28</v>
+      </c>
+      <c r="H353">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="354" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A354" t="s">
+        <v>339</v>
+      </c>
+      <c r="D354" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G354">
+        <v>30</v>
+      </c>
+      <c r="H354">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="355" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A355" t="s">
+        <v>340</v>
+      </c>
+      <c r="D355" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G355">
+        <v>28</v>
+      </c>
+      <c r="H355">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="356" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A356" t="s">
+        <v>341</v>
+      </c>
+      <c r="D356" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G356">
+        <v>27</v>
+      </c>
+      <c r="H356">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="357" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A357" t="s">
+        <v>342</v>
+      </c>
+      <c r="D357" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G357">
+        <v>28</v>
+      </c>
+      <c r="H357">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="358" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A358" t="s">
+        <v>343</v>
+      </c>
+      <c r="D358" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G358">
+        <v>25</v>
+      </c>
+      <c r="H358">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="359" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A359" t="s">
+        <v>344</v>
+      </c>
+      <c r="D359" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G359">
+        <v>36</v>
+      </c>
+      <c r="H359">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="360" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A360" t="s">
+        <v>345</v>
+      </c>
+      <c r="D360" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G360">
+        <v>36</v>
+      </c>
+      <c r="H360">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="361" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A361" t="s">
+        <v>346</v>
+      </c>
+      <c r="D361" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G361">
+        <v>34</v>
+      </c>
+      <c r="H361">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="362" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A362" t="s">
+        <v>347</v>
+      </c>
+      <c r="D362" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G362">
+        <v>35</v>
+      </c>
+      <c r="H362">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="363" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A363" t="s">
+        <v>348</v>
+      </c>
+      <c r="D363" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G363">
+        <v>31</v>
+      </c>
+      <c r="H363">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="364" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A364" t="s">
+        <v>349</v>
+      </c>
+      <c r="D364" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G364">
+        <v>33</v>
+      </c>
+      <c r="H364">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="365" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A365" t="s">
+        <v>350</v>
+      </c>
+      <c r="D365" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G365">
+        <v>30</v>
+      </c>
+      <c r="H365">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="366" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A366" t="s">
+        <v>351</v>
+      </c>
+      <c r="D366" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G366">
+        <v>30</v>
+      </c>
+      <c r="H366">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="367" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A367" t="s">
+        <v>352</v>
+      </c>
+      <c r="D367" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G367">
+        <v>30</v>
+      </c>
+      <c r="H367">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="368" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A368" t="s">
+        <v>353</v>
+      </c>
+      <c r="D368" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G368">
+        <v>27</v>
+      </c>
+      <c r="H368">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="369" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A369" t="s">
+        <v>354</v>
+      </c>
+      <c r="D369" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G369">
+        <v>43</v>
+      </c>
+      <c r="H369">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="370" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A370" t="s">
+        <v>355</v>
+      </c>
+      <c r="D370" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G370">
+        <v>42</v>
+      </c>
+      <c r="H370">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="371" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A371" t="s">
+        <v>356</v>
+      </c>
+      <c r="D371" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G371">
+        <v>39</v>
+      </c>
+      <c r="H371">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="372" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A372" t="s">
+        <v>357</v>
+      </c>
+      <c r="D372" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G372">
+        <v>39</v>
+      </c>
+      <c r="H372">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="373" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A373" t="s">
+        <v>358</v>
+      </c>
+      <c r="D373" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G373">
+        <v>37</v>
+      </c>
+      <c r="H373">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="374" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A374" t="s">
+        <v>359</v>
+      </c>
+      <c r="D374" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G374">
+        <v>37</v>
+      </c>
+      <c r="H374">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="375" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A375" t="s">
+        <v>360</v>
+      </c>
+      <c r="D375" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G375">
+        <v>36</v>
+      </c>
+      <c r="H375">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="376" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A376" t="s">
+        <v>361</v>
+      </c>
+      <c r="D376" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G376">
+        <v>35</v>
+      </c>
+      <c r="H376">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="377" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A377" t="s">
+        <v>362</v>
+      </c>
+      <c r="D377" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G377">
+        <v>33</v>
+      </c>
+      <c r="H377">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="378" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A378" t="s">
+        <v>363</v>
+      </c>
+      <c r="D378" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G378">
+        <v>33</v>
+      </c>
+      <c r="H378">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="379" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A379" t="s">
+        <v>364</v>
+      </c>
+      <c r="D379" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G379">
+        <v>48</v>
+      </c>
+      <c r="H379">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="380" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A380" t="s">
+        <v>365</v>
+      </c>
+      <c r="D380" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G380">
+        <v>45</v>
+      </c>
+      <c r="H380">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="381" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A381" t="s">
+        <v>366</v>
+      </c>
+      <c r="D381" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G381">
+        <v>46</v>
+      </c>
+      <c r="H381">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="382" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A382" t="s">
+        <v>367</v>
+      </c>
+      <c r="D382" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G382">
+        <v>41</v>
+      </c>
+      <c r="H382">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="383" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A383" t="s">
+        <v>368</v>
+      </c>
+      <c r="D383" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G383">
+        <v>43</v>
+      </c>
+      <c r="H383">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="384" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A384" t="s">
+        <v>369</v>
+      </c>
+      <c r="D384" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G384">
+        <v>40</v>
+      </c>
+      <c r="H384">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="385" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A385" t="s">
+        <v>370</v>
+      </c>
+      <c r="D385" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G385">
+        <v>36</v>
+      </c>
+      <c r="H385">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="386" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A386" t="s">
+        <v>371</v>
+      </c>
+      <c r="D386" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G386">
+        <v>38</v>
+      </c>
+      <c r="H386">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="387" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A387" t="s">
+        <v>372</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G387">
+        <v>34</v>
+      </c>
+      <c r="H387">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="388" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A388" t="s">
+        <v>373</v>
+      </c>
+      <c r="D388" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G388">
+        <v>32</v>
+      </c>
+      <c r="H388">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="389" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A389" t="s">
+        <v>374</v>
+      </c>
+      <c r="D389" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G389">
+        <v>56</v>
+      </c>
+      <c r="H389">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="390" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A390" t="s">
+        <v>375</v>
+      </c>
+      <c r="D390" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G390">
+        <v>56</v>
+      </c>
+      <c r="H390">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="391" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A391" t="s">
+        <v>376</v>
+      </c>
+      <c r="D391" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G391">
+        <v>53</v>
+      </c>
+      <c r="H391">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="392" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A392" t="s">
+        <v>377</v>
+      </c>
+      <c r="D392" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G392">
+        <v>53</v>
+      </c>
+      <c r="H392">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="393" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A393" t="s">
+        <v>378</v>
+      </c>
+      <c r="D393" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G393">
+        <v>51</v>
+      </c>
+      <c r="H393">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="394" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A394" t="s">
+        <v>379</v>
+      </c>
+      <c r="D394" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G394">
+        <v>49</v>
+      </c>
+      <c r="H394">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="395" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A395" t="s">
+        <v>380</v>
+      </c>
+      <c r="D395" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G395">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="396" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A396" t="s">
+        <v>381</v>
+      </c>
+      <c r="D396" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G396">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="397" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A397" t="s">
+        <v>382</v>
+      </c>
+      <c r="D397" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G397">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="398" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A398" t="s">
+        <v>383</v>
+      </c>
+      <c r="D398" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G398">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="399" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A399" t="s">
+        <v>384</v>
+      </c>
+      <c r="D399" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G399">
+        <v>62</v>
+      </c>
+      <c r="H399">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="400" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A400" t="s">
+        <v>385</v>
+      </c>
+      <c r="D400" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G400">
+        <v>60</v>
+      </c>
+      <c r="H400">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="401" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A401" t="s">
+        <v>386</v>
+      </c>
+      <c r="D401" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G401">
+        <v>59</v>
+      </c>
+      <c r="H401">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="402" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A402" t="s">
+        <v>387</v>
+      </c>
+      <c r="D402" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G402">
+        <v>55</v>
+      </c>
+      <c r="H402">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="403" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A403" t="s">
+        <v>388</v>
+      </c>
+      <c r="D403" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G403">
+        <v>55</v>
+      </c>
+      <c r="H403">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="404" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A404" t="s">
+        <v>389</v>
+      </c>
+      <c r="D404" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G404">
+        <v>50</v>
+      </c>
+      <c r="H404">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="405" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A405" t="s">
+        <v>390</v>
+      </c>
+      <c r="D405" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G405">
+        <v>46</v>
+      </c>
+      <c r="H405">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="406" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A406" t="s">
+        <v>391</v>
+      </c>
+      <c r="D406" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G406">
+        <v>45</v>
+      </c>
+      <c r="H406">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="407" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A407" t="s">
+        <v>392</v>
+      </c>
+      <c r="D407" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G407">
+        <v>42</v>
+      </c>
+      <c r="H407">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="408" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A408" t="s">
+        <v>393</v>
+      </c>
+      <c r="D408" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G408">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="409" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A409" t="s">
+        <v>394</v>
+      </c>
+      <c r="D409" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G409">
+        <v>74</v>
+      </c>
+      <c r="H409">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="410" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A410" t="s">
+        <v>395</v>
+      </c>
+      <c r="D410" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G410">
+        <v>73</v>
+      </c>
+      <c r="H410">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="411" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A411" t="s">
+        <v>396</v>
+      </c>
+      <c r="D411" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G411">
+        <v>70</v>
+      </c>
+      <c r="H411">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="412" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A412" t="s">
+        <v>397</v>
+      </c>
+      <c r="D412" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G412">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="413" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A413" t="s">
+        <v>398</v>
+      </c>
+      <c r="D413" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G413">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="414" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A414" t="s">
+        <v>399</v>
+      </c>
+      <c r="D414" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G414">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="415" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A415" t="s">
+        <v>400</v>
+      </c>
+      <c r="D415" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G415">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="416" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A416" t="s">
+        <v>401</v>
+      </c>
+      <c r="D416" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G416">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="417" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A417" t="s">
+        <v>402</v>
+      </c>
+      <c r="D417" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G417">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="418" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A418" t="s">
+        <v>403</v>
+      </c>
+      <c r="D418" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G418">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="419" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A419" t="s">
+        <v>404</v>
+      </c>
+      <c r="D419" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G419">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="420" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A420" t="s">
+        <v>405</v>
+      </c>
+      <c r="D420" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G420">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="421" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A421" t="s">
+        <v>406</v>
+      </c>
+      <c r="D421" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G421">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="422" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A422" t="s">
+        <v>407</v>
+      </c>
+      <c r="D422" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G422">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="423" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A423" t="s">
+        <v>408</v>
+      </c>
+      <c r="D423" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G423">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="424" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A424" t="s">
+        <v>409</v>
+      </c>
+      <c r="D424" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G424">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="425" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A425" t="s">
+        <v>410</v>
+      </c>
+      <c r="D425" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G425">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="426" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A426" t="s">
+        <v>411</v>
+      </c>
+      <c r="D426" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G426">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="427" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A427" t="s">
+        <v>412</v>
+      </c>
+      <c r="D427" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G427">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="428" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A428" t="s">
+        <v>413</v>
+      </c>
+      <c r="D428" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G428">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="429" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A429" t="s">
+        <v>414</v>
+      </c>
+      <c r="D429" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G429">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="430" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A430" t="s">
+        <v>415</v>
+      </c>
+      <c r="D430" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G430">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="431" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A431" t="s">
+        <v>416</v>
+      </c>
+      <c r="D431" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G431">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="432" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A432" t="s">
+        <v>417</v>
+      </c>
+      <c r="D432" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G432">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="433" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A433" t="s">
+        <v>418</v>
+      </c>
+      <c r="D433" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G433">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="434" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A434" t="s">
+        <v>419</v>
+      </c>
+      <c r="D434" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G434">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="435" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A435" t="s">
+        <v>420</v>
+      </c>
+      <c r="D435" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G435">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="436" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A436" t="s">
+        <v>421</v>
+      </c>
+      <c r="D436" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G436">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="437" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A437" t="s">
+        <v>422</v>
+      </c>
+      <c r="D437" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G437">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="438" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A438" t="s">
+        <v>423</v>
+      </c>
+      <c r="D438" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G438">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="439" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A439" t="s">
+        <v>424</v>
+      </c>
+      <c r="D439" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G439">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="440" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A440" t="s">
+        <v>425</v>
+      </c>
+      <c r="D440" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G440">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="441" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A441" t="s">
+        <v>426</v>
+      </c>
+      <c r="D441" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G441">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="442" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A442" t="s">
+        <v>427</v>
+      </c>
+      <c r="D442" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G442">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="443" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A443" t="s">
+        <v>428</v>
+      </c>
+      <c r="D443" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G443">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="444" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A444" t="s">
+        <v>429</v>
+      </c>
+      <c r="D444" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G444">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="445" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A445" t="s">
+        <v>430</v>
+      </c>
+      <c r="D445" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G445">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="446" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A446" t="s">
+        <v>431</v>
+      </c>
+      <c r="D446" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G446">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="447" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A447" t="s">
+        <v>432</v>
+      </c>
+      <c r="D447" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G447">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="448" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A448" t="s">
+        <v>433</v>
+      </c>
+      <c r="D448" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G448">
+        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>